<commit_message>
stagger the color between lines
</commit_message>
<xml_diff>
--- a/generateEXCEL/index.xlsx
+++ b/generateEXCEL/index.xlsx
@@ -286,12 +286,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="0019b457"/>
+        <fgColor rgb="00EAEAEA"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00ffb261"/>
+        <fgColor rgb="0019b457"/>
       </patternFill>
     </fill>
     <fill>
@@ -322,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -333,13 +333,16 @@
     <xf applyAlignment="1" borderId="0" fillId="2" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="0" fillId="4" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -695,34 +698,34 @@
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="6" t="n">
         <v>99.09999999999999</v>
       </c>
-      <c r="D4" s="4" t="n">
+      <c r="D4" s="5" t="n">
         <v>20</v>
       </c>
-      <c r="E4" s="5" t="n">
+      <c r="E4" s="6" t="n">
         <v>99.59999999999999</v>
       </c>
-      <c r="F4" s="4" t="n">
+      <c r="F4" s="5" t="n">
         <v>93</v>
       </c>
-      <c r="G4" s="5" t="n">
+      <c r="G4" s="6" t="n">
         <v>98.09999999999999</v>
       </c>
-      <c r="H4" s="4" t="n">
+      <c r="H4" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="I4" s="5" t="n">
+      <c r="I4" s="6" t="n">
         <v>99.90000000000001</v>
       </c>
-      <c r="K4" s="6" t="n">
+      <c r="K4" s="5" t="n">
         <v>99.8</v>
       </c>
     </row>
@@ -730,63 +733,63 @@
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="4" t="n">
+      <c r="B5" s="5" t="n">
         <v>51</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="7" t="n">
         <v>98.90000000000001</v>
       </c>
-      <c r="D5" s="4" t="n">
+      <c r="D5" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="E5" s="5" t="n">
+      <c r="E5" s="7" t="n">
         <v>99.3</v>
       </c>
-      <c r="F5" s="4" t="n">
+      <c r="F5" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G5" s="5" t="n">
+      <c r="G5" s="7" t="n">
         <v>99.90000000000001</v>
       </c>
-      <c r="H5" s="4" t="n">
+      <c r="H5" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="I5" s="5" t="n">
+      <c r="I5" s="7" t="n">
         <v>99.2</v>
       </c>
-      <c r="K5" s="6" t="n">
+      <c r="K5" s="5" t="n">
         <v>99.59999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="n">
+      <c r="B6" s="8" t="n">
         <v>324</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="6" t="n">
         <v>87.8</v>
       </c>
-      <c r="D6" s="4" t="n">
+      <c r="D6" s="5" t="n">
         <v>100</v>
       </c>
-      <c r="E6" s="5" t="n">
+      <c r="E6" s="6" t="n">
         <v>97.90000000000001</v>
       </c>
-      <c r="F6" s="4" t="n">
+      <c r="F6" s="5" t="n">
         <v>74</v>
       </c>
-      <c r="G6" s="5" t="n">
+      <c r="G6" s="6" t="n">
         <v>98.5</v>
       </c>
-      <c r="H6" s="4" t="n">
+      <c r="H6" s="5" t="n">
         <v>111</v>
       </c>
-      <c r="I6" s="5" t="n">
+      <c r="I6" s="6" t="n">
         <v>97.7</v>
       </c>
-      <c r="K6" s="6" t="n">
+      <c r="K6" s="5" t="n">
         <v>98.2</v>
       </c>
     </row>
@@ -794,63 +797,63 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="n">
+      <c r="B7" s="8" t="n">
         <v>233</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="7" t="n">
         <v>89.8</v>
       </c>
-      <c r="D7" s="8" t="n">
+      <c r="D7" s="9" t="n">
         <v>2069</v>
       </c>
-      <c r="E7" s="5" t="n">
+      <c r="E7" s="7" t="n">
         <v>47</v>
       </c>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="5" t="n">
         <v>178</v>
       </c>
-      <c r="G7" s="5" t="n">
+      <c r="G7" s="7" t="n">
         <v>96.3</v>
       </c>
-      <c r="H7" s="4" t="n">
+      <c r="H7" s="5" t="n">
         <v>61</v>
       </c>
-      <c r="I7" s="5" t="n">
+      <c r="I7" s="7" t="n">
         <v>98.8</v>
       </c>
-      <c r="K7" s="6" t="n">
+      <c r="K7" s="5" t="n">
         <v>97.5</v>
       </c>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>117</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="6" t="n">
         <v>97.40000000000001</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="5" t="n">
         <v>163</v>
       </c>
-      <c r="E8" s="5" t="n">
+      <c r="E8" s="6" t="n">
         <v>96.59999999999999</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="F8" s="8" t="n">
         <v>675</v>
       </c>
-      <c r="G8" s="5" t="n">
+      <c r="G8" s="6" t="n">
         <v>81.09999999999999</v>
       </c>
-      <c r="H8" s="4" t="n">
+      <c r="H8" s="5" t="n">
         <v>109</v>
       </c>
-      <c r="I8" s="5" t="n">
+      <c r="I8" s="6" t="n">
         <v>97.8</v>
       </c>
-      <c r="K8" s="6" t="n">
+      <c r="K8" s="5" t="n">
         <v>97.2</v>
       </c>
     </row>
@@ -858,63 +861,63 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="n">
+      <c r="B9" s="5" t="n">
         <v>112</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="7" t="n">
         <v>97.5</v>
       </c>
-      <c r="D9" s="4" t="n">
+      <c r="D9" s="5" t="n">
         <v>164</v>
       </c>
-      <c r="E9" s="5" t="n">
+      <c r="E9" s="7" t="n">
         <v>96.59999999999999</v>
       </c>
-      <c r="F9" s="4" t="n">
+      <c r="F9" s="5" t="n">
         <v>154</v>
       </c>
-      <c r="G9" s="5" t="n">
+      <c r="G9" s="7" t="n">
         <v>96.8</v>
       </c>
-      <c r="H9" s="7" t="n">
+      <c r="H9" s="8" t="n">
         <v>637</v>
       </c>
-      <c r="I9" s="5" t="n">
+      <c r="I9" s="7" t="n">
         <v>82</v>
       </c>
-      <c r="K9" s="6" t="n">
+      <c r="K9" s="5" t="n">
         <v>96.7</v>
       </c>
     </row>
     <row r="10" spans="1:11">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="n">
+      <c r="B10" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="C10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="5" t="n">
+      <c r="C10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="E10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" s="5" t="n">
+      <c r="E10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="G10" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="4" t="n">
+      <c r="G10" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5" t="n">
         <v>169</v>
       </c>
-      <c r="I10" s="5" t="n">
+      <c r="I10" s="6" t="n">
         <v>96.59999999999999</v>
       </c>
-      <c r="K10" s="6" t="n">
+      <c r="K10" s="5" t="n">
         <v>96.59999999999999</v>
       </c>
     </row>
@@ -922,63 +925,63 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7" t="n">
+      <c r="B11" s="8" t="n">
         <v>251</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="7" t="n">
         <v>89.40000000000001</v>
       </c>
-      <c r="D11" s="4" t="n">
+      <c r="D11" s="5" t="n">
         <v>127</v>
       </c>
-      <c r="E11" s="5" t="n">
+      <c r="E11" s="7" t="n">
         <v>97.40000000000001</v>
       </c>
-      <c r="F11" s="7" t="n">
+      <c r="F11" s="8" t="n">
         <v>581</v>
       </c>
-      <c r="G11" s="5" t="n">
+      <c r="G11" s="7" t="n">
         <v>83</v>
       </c>
-      <c r="H11" s="4" t="n">
+      <c r="H11" s="5" t="n">
         <v>218</v>
       </c>
-      <c r="I11" s="5" t="n">
+      <c r="I11" s="7" t="n">
         <v>95.59999999999999</v>
       </c>
-      <c r="K11" s="6" t="n">
+      <c r="K11" s="5" t="n">
         <v>96.5</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="n">
+      <c r="B12" s="8" t="n">
         <v>514</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="6" t="n">
         <v>83.5</v>
       </c>
-      <c r="D12" s="4" t="n">
+      <c r="D12" s="5" t="n">
         <v>128</v>
       </c>
-      <c r="E12" s="5" t="n">
+      <c r="E12" s="6" t="n">
         <v>97.3</v>
       </c>
-      <c r="F12" s="4" t="n">
+      <c r="F12" s="5" t="n">
         <v>222</v>
       </c>
-      <c r="G12" s="5" t="n">
+      <c r="G12" s="6" t="n">
         <v>95.40000000000001</v>
       </c>
-      <c r="H12" s="7" t="n">
+      <c r="H12" s="8" t="n">
         <v>250</v>
       </c>
-      <c r="I12" s="5" t="n">
+      <c r="I12" s="6" t="n">
         <v>89.90000000000001</v>
       </c>
-      <c r="K12" s="6" t="n">
+      <c r="K12" s="5" t="n">
         <v>96.40000000000001</v>
       </c>
     </row>
@@ -986,63 +989,63 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="7" t="n">
+      <c r="B13" s="8" t="n">
         <v>429</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="7" t="n">
         <v>85.40000000000001</v>
       </c>
-      <c r="D13" s="4" t="n">
+      <c r="D13" s="5" t="n">
         <v>174</v>
       </c>
-      <c r="E13" s="5" t="n">
+      <c r="E13" s="7" t="n">
         <v>96.40000000000001</v>
       </c>
-      <c r="F13" s="4" t="n">
+      <c r="F13" s="5" t="n">
         <v>322</v>
       </c>
-      <c r="G13" s="5" t="n">
+      <c r="G13" s="7" t="n">
         <v>93.40000000000001</v>
       </c>
-      <c r="H13" s="7" t="n">
+      <c r="H13" s="8" t="n">
         <v>492</v>
       </c>
-      <c r="I13" s="5" t="n">
+      <c r="I13" s="7" t="n">
         <v>85</v>
       </c>
-      <c r="K13" s="6" t="n">
+      <c r="K13" s="5" t="n">
         <v>94.90000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9" t="n">
+      <c r="B14" s="10" t="n">
         <v>1455</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="6" t="n">
         <v>52.5</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="8" t="n">
         <v>1023</v>
       </c>
-      <c r="E14" s="5" t="n">
+      <c r="E14" s="6" t="n">
         <v>73.7</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="5" t="n">
         <v>345</v>
       </c>
-      <c r="G14" s="5" t="n">
+      <c r="G14" s="6" t="n">
         <v>92.90000000000001</v>
       </c>
-      <c r="H14" s="4" t="n">
+      <c r="H14" s="5" t="n">
         <v>184</v>
       </c>
-      <c r="I14" s="5" t="n">
+      <c r="I14" s="6" t="n">
         <v>96.2</v>
       </c>
-      <c r="K14" s="6" t="n">
+      <c r="K14" s="5" t="n">
         <v>94.59999999999999</v>
       </c>
     </row>
@@ -1050,63 +1053,63 @@
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="4" t="n">
+      <c r="B15" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="7" t="n">
         <v>98.7</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="8" t="n">
         <v>454</v>
       </c>
-      <c r="E15" s="5" t="n">
+      <c r="E15" s="7" t="n">
         <v>85.59999999999999</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="5" t="n">
         <v>425</v>
       </c>
-      <c r="G15" s="5" t="n">
+      <c r="G15" s="7" t="n">
         <v>91.2</v>
       </c>
-      <c r="H15" s="4" t="n">
+      <c r="H15" s="5" t="n">
         <v>103</v>
       </c>
-      <c r="I15" s="5" t="n">
+      <c r="I15" s="7" t="n">
         <v>97.90000000000001</v>
       </c>
-      <c r="K15" s="6" t="n">
+      <c r="K15" s="5" t="n">
         <v>94.59999999999999</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="7" t="n">
+      <c r="B16" s="8" t="n">
         <v>642</v>
       </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" s="6" t="n">
         <v>80.7</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="8" t="n">
         <v>672</v>
       </c>
-      <c r="E16" s="5" t="n">
+      <c r="E16" s="6" t="n">
         <v>81</v>
       </c>
-      <c r="F16" s="4" t="n">
+      <c r="F16" s="5" t="n">
         <v>518</v>
       </c>
-      <c r="G16" s="5" t="n">
+      <c r="G16" s="6" t="n">
         <v>89.3</v>
       </c>
-      <c r="H16" s="4" t="n">
+      <c r="H16" s="5" t="n">
         <v>205</v>
       </c>
-      <c r="I16" s="5" t="n">
+      <c r="I16" s="6" t="n">
         <v>95.8</v>
       </c>
-      <c r="K16" s="6" t="n">
+      <c r="K16" s="5" t="n">
         <v>92.59999999999999</v>
       </c>
     </row>
@@ -1114,63 +1117,63 @@
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="7" t="n">
+      <c r="B17" s="8" t="n">
         <v>578</v>
       </c>
-      <c r="C17" s="5" t="n">
+      <c r="C17" s="7" t="n">
         <v>82.09999999999999</v>
       </c>
-      <c r="D17" s="4" t="n">
+      <c r="D17" s="5" t="n">
         <v>233</v>
       </c>
-      <c r="E17" s="5" t="n">
+      <c r="E17" s="7" t="n">
         <v>95.2</v>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="5" t="n">
         <v>502</v>
       </c>
-      <c r="G17" s="5" t="n">
+      <c r="G17" s="7" t="n">
         <v>89.59999999999999</v>
       </c>
-      <c r="H17" s="9" t="n">
+      <c r="H17" s="10" t="n">
         <v>1641</v>
       </c>
-      <c r="I17" s="5" t="n">
+      <c r="I17" s="7" t="n">
         <v>51.5</v>
       </c>
-      <c r="K17" s="6" t="n">
+      <c r="K17" s="5" t="n">
         <v>92.40000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="7" t="n">
+      <c r="B18" s="8" t="n">
         <v>301</v>
       </c>
-      <c r="C18" s="5" t="n">
+      <c r="C18" s="6" t="n">
         <v>88.3</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D18" s="8" t="n">
         <v>344</v>
       </c>
-      <c r="E18" s="5" t="n">
+      <c r="E18" s="6" t="n">
         <v>87.8</v>
       </c>
-      <c r="F18" s="4" t="n">
+      <c r="F18" s="5" t="n">
         <v>232</v>
       </c>
-      <c r="G18" s="5" t="n">
+      <c r="G18" s="6" t="n">
         <v>95.2</v>
       </c>
-      <c r="H18" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I18" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K18" s="6" t="n">
+      <c r="H18" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I18" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K18" s="5" t="n">
         <v>91.5</v>
       </c>
     </row>
@@ -1178,63 +1181,63 @@
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="7" t="n">
+      <c r="B19" s="8" t="n">
         <v>500</v>
       </c>
-      <c r="C19" s="5" t="n">
+      <c r="C19" s="7" t="n">
         <v>83.8</v>
       </c>
-      <c r="D19" s="4" t="n">
+      <c r="D19" s="5" t="n">
         <v>225</v>
       </c>
-      <c r="E19" s="5" t="n">
+      <c r="E19" s="7" t="n">
         <v>95.3</v>
       </c>
-      <c r="F19" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G19" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="7" t="n">
+      <c r="F19" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G19" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="8" t="n">
         <v>430</v>
       </c>
-      <c r="I19" s="5" t="n">
+      <c r="I19" s="7" t="n">
         <v>86.2</v>
       </c>
-      <c r="K19" s="6" t="n">
+      <c r="K19" s="5" t="n">
         <v>90.8</v>
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="8" t="n">
+      <c r="B20" s="9" t="n">
         <v>1266</v>
       </c>
-      <c r="C20" s="5" t="n">
+      <c r="C20" s="6" t="n">
         <v>61.8</v>
       </c>
-      <c r="D20" s="7" t="n">
+      <c r="D20" s="8" t="n">
         <v>345</v>
       </c>
-      <c r="E20" s="5" t="n">
+      <c r="E20" s="6" t="n">
         <v>87.8</v>
       </c>
-      <c r="F20" s="4" t="n">
+      <c r="F20" s="5" t="n">
         <v>339</v>
       </c>
-      <c r="G20" s="5" t="n">
+      <c r="G20" s="6" t="n">
         <v>93</v>
       </c>
-      <c r="H20" s="7" t="n">
+      <c r="H20" s="8" t="n">
         <v>488</v>
       </c>
-      <c r="I20" s="5" t="n">
+      <c r="I20" s="6" t="n">
         <v>85.09999999999999</v>
       </c>
-      <c r="K20" s="6" t="n">
+      <c r="K20" s="5" t="n">
         <v>90.40000000000001</v>
       </c>
     </row>
@@ -1242,63 +1245,63 @@
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="7" t="n">
+      <c r="B21" s="8" t="n">
         <v>290</v>
       </c>
-      <c r="C21" s="5" t="n">
+      <c r="C21" s="7" t="n">
         <v>88.5</v>
       </c>
-      <c r="D21" s="7" t="n">
+      <c r="D21" s="8" t="n">
         <v>443</v>
       </c>
-      <c r="E21" s="5" t="n">
+      <c r="E21" s="7" t="n">
         <v>85.8</v>
       </c>
-      <c r="F21" s="4" t="n">
+      <c r="F21" s="5" t="n">
         <v>336</v>
       </c>
-      <c r="G21" s="5" t="n">
+      <c r="G21" s="7" t="n">
         <v>93.09999999999999</v>
       </c>
-      <c r="H21" s="7" t="n">
+      <c r="H21" s="8" t="n">
         <v>497</v>
       </c>
-      <c r="I21" s="5" t="n">
+      <c r="I21" s="7" t="n">
         <v>84.90000000000001</v>
       </c>
-      <c r="K21" s="6" t="n">
+      <c r="K21" s="5" t="n">
         <v>89.5</v>
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="8" t="n">
+      <c r="B22" s="9" t="n">
         <v>1302</v>
       </c>
-      <c r="C22" s="5" t="n">
+      <c r="C22" s="6" t="n">
         <v>61</v>
       </c>
-      <c r="D22" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E22" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" s="4" t="n">
+      <c r="D22" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" s="5" t="n">
         <v>240</v>
       </c>
-      <c r="G22" s="5" t="n">
+      <c r="G22" s="6" t="n">
         <v>95</v>
       </c>
-      <c r="H22" s="7" t="n">
+      <c r="H22" s="8" t="n">
         <v>560</v>
       </c>
-      <c r="I22" s="5" t="n">
+      <c r="I22" s="6" t="n">
         <v>83.59999999999999</v>
       </c>
-      <c r="K22" s="6" t="n">
+      <c r="K22" s="5" t="n">
         <v>89.3</v>
       </c>
     </row>
@@ -1306,63 +1309,63 @@
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="7" t="n">
+      <c r="B23" s="8" t="n">
         <v>612</v>
       </c>
-      <c r="C23" s="5" t="n">
+      <c r="C23" s="7" t="n">
         <v>81.40000000000001</v>
       </c>
-      <c r="D23" s="9" t="n">
+      <c r="D23" s="10" t="n">
         <v>2384</v>
       </c>
-      <c r="E23" s="5" t="n">
+      <c r="E23" s="7" t="n">
         <v>35.4</v>
       </c>
-      <c r="F23" s="4" t="n">
+      <c r="F23" s="5" t="n">
         <v>397</v>
       </c>
-      <c r="G23" s="5" t="n">
+      <c r="G23" s="7" t="n">
         <v>91.8</v>
       </c>
-      <c r="H23" s="7" t="n">
+      <c r="H23" s="8" t="n">
         <v>561</v>
       </c>
-      <c r="I23" s="5" t="n">
+      <c r="I23" s="7" t="n">
         <v>83.59999999999999</v>
       </c>
-      <c r="K23" s="6" t="n">
+      <c r="K23" s="5" t="n">
         <v>87.7</v>
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="7" t="n">
+      <c r="B24" s="8" t="n">
         <v>394</v>
       </c>
-      <c r="C24" s="5" t="n">
+      <c r="C24" s="6" t="n">
         <v>86.2</v>
       </c>
-      <c r="D24" s="7" t="n">
+      <c r="D24" s="8" t="n">
         <v>509</v>
       </c>
-      <c r="E24" s="5" t="n">
+      <c r="E24" s="6" t="n">
         <v>84.40000000000001</v>
       </c>
-      <c r="F24" s="9" t="n">
+      <c r="F24" s="10" t="n">
         <v>2350</v>
       </c>
-      <c r="G24" s="5" t="n">
+      <c r="G24" s="6" t="n">
         <v>36.5</v>
       </c>
-      <c r="H24" s="7" t="n">
+      <c r="H24" s="8" t="n">
         <v>276</v>
       </c>
-      <c r="I24" s="5" t="n">
+      <c r="I24" s="6" t="n">
         <v>89.40000000000001</v>
       </c>
-      <c r="K24" s="6" t="n">
+      <c r="K24" s="5" t="n">
         <v>86.90000000000001</v>
       </c>
     </row>
@@ -1370,63 +1373,63 @@
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="8" t="n">
+      <c r="B25" s="9" t="n">
         <v>1191</v>
       </c>
-      <c r="C25" s="5" t="n">
+      <c r="C25" s="7" t="n">
         <v>63.4</v>
       </c>
-      <c r="D25" s="7" t="n">
+      <c r="D25" s="8" t="n">
         <v>638</v>
       </c>
-      <c r="E25" s="5" t="n">
+      <c r="E25" s="7" t="n">
         <v>81.7</v>
       </c>
-      <c r="F25" s="7" t="n">
+      <c r="F25" s="8" t="n">
         <v>645</v>
       </c>
-      <c r="G25" s="5" t="n">
+      <c r="G25" s="7" t="n">
         <v>81.7</v>
       </c>
-      <c r="H25" s="7" t="n">
+      <c r="H25" s="8" t="n">
         <v>271</v>
       </c>
-      <c r="I25" s="5" t="n">
+      <c r="I25" s="7" t="n">
         <v>89.5</v>
       </c>
-      <c r="K25" s="6" t="n">
+      <c r="K25" s="5" t="n">
         <v>85.59999999999999</v>
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C26" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="7" t="n">
+      <c r="B26" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C26" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="8" t="n">
         <v>711</v>
       </c>
-      <c r="E26" s="5" t="n">
+      <c r="E26" s="6" t="n">
         <v>80.2</v>
       </c>
-      <c r="F26" s="4" t="n">
+      <c r="F26" s="5" t="n">
         <v>474</v>
       </c>
-      <c r="G26" s="5" t="n">
+      <c r="G26" s="6" t="n">
         <v>90.2</v>
       </c>
-      <c r="H26" s="8" t="n">
+      <c r="H26" s="9" t="n">
         <v>806</v>
       </c>
-      <c r="I26" s="5" t="n">
+      <c r="I26" s="6" t="n">
         <v>73.59999999999999</v>
       </c>
-      <c r="K26" s="6" t="n">
+      <c r="K26" s="5" t="n">
         <v>85.2</v>
       </c>
     </row>
@@ -1434,63 +1437,63 @@
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="9" t="n">
+      <c r="B27" s="10" t="n">
         <v>1904</v>
       </c>
-      <c r="C27" s="5" t="n">
+      <c r="C27" s="7" t="n">
         <v>42.5</v>
       </c>
-      <c r="D27" s="7" t="n">
+      <c r="D27" s="8" t="n">
         <v>793</v>
       </c>
-      <c r="E27" s="5" t="n">
+      <c r="E27" s="7" t="n">
         <v>78.5</v>
       </c>
-      <c r="F27" s="4" t="n">
+      <c r="F27" s="5" t="n">
         <v>420</v>
       </c>
-      <c r="G27" s="5" t="n">
+      <c r="G27" s="7" t="n">
         <v>91.3</v>
       </c>
-      <c r="H27" s="8" t="n">
+      <c r="H27" s="9" t="n">
         <v>721</v>
       </c>
-      <c r="I27" s="5" t="n">
+      <c r="I27" s="7" t="n">
         <v>75.3</v>
       </c>
-      <c r="K27" s="6" t="n">
+      <c r="K27" s="5" t="n">
         <v>84.90000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="5" t="n">
+      <c r="B28" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="C28" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="5" t="n">
+      <c r="C28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="E28" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" s="5" t="n">
+      <c r="E28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="G28" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="7" t="n">
+      <c r="G28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="8" t="n">
         <v>541</v>
       </c>
-      <c r="I28" s="5" t="n">
+      <c r="I28" s="6" t="n">
         <v>84</v>
       </c>
-      <c r="K28" s="6" t="n">
+      <c r="K28" s="5" t="n">
         <v>84</v>
       </c>
     </row>
@@ -1498,63 +1501,63 @@
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="8" t="n">
+      <c r="B29" s="9" t="n">
         <v>1153</v>
       </c>
-      <c r="C29" s="5" t="n">
+      <c r="C29" s="7" t="n">
         <v>64.3</v>
       </c>
-      <c r="D29" s="7" t="n">
+      <c r="D29" s="8" t="n">
         <v>477</v>
       </c>
-      <c r="E29" s="5" t="n">
+      <c r="E29" s="7" t="n">
         <v>85.09999999999999</v>
       </c>
-      <c r="F29" s="8" t="n">
+      <c r="F29" s="9" t="n">
         <v>1612</v>
       </c>
-      <c r="G29" s="5" t="n">
+      <c r="G29" s="7" t="n">
         <v>56.7</v>
       </c>
-      <c r="H29" s="7" t="n">
+      <c r="H29" s="8" t="n">
         <v>629</v>
       </c>
-      <c r="I29" s="5" t="n">
+      <c r="I29" s="7" t="n">
         <v>82.2</v>
       </c>
-      <c r="K29" s="6" t="n">
+      <c r="K29" s="5" t="n">
         <v>83.7</v>
       </c>
     </row>
     <row r="30" spans="1:11">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="7" t="n">
+      <c r="B30" s="8" t="n">
         <v>565</v>
       </c>
-      <c r="C30" s="5" t="n">
+      <c r="C30" s="6" t="n">
         <v>82.40000000000001</v>
       </c>
-      <c r="D30" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E30" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" s="7" t="n">
+      <c r="D30" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E30" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" s="8" t="n">
         <v>845</v>
       </c>
-      <c r="G30" s="5" t="n">
+      <c r="G30" s="6" t="n">
         <v>77.59999999999999</v>
       </c>
-      <c r="H30" s="7" t="n">
+      <c r="H30" s="8" t="n">
         <v>419</v>
       </c>
-      <c r="I30" s="5" t="n">
+      <c r="I30" s="6" t="n">
         <v>86.5</v>
       </c>
-      <c r="K30" s="6" t="n">
+      <c r="K30" s="5" t="n">
         <v>82</v>
       </c>
     </row>
@@ -1562,63 +1565,63 @@
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="8" t="n">
+      <c r="B31" s="9" t="n">
         <v>1117</v>
       </c>
-      <c r="C31" s="5" t="n">
+      <c r="C31" s="7" t="n">
         <v>65.09999999999999</v>
       </c>
-      <c r="D31" s="7" t="n">
+      <c r="D31" s="8" t="n">
         <v>459</v>
       </c>
-      <c r="E31" s="5" t="n">
+      <c r="E31" s="7" t="n">
         <v>85.5</v>
       </c>
-      <c r="F31" s="7" t="n">
+      <c r="F31" s="8" t="n">
         <v>846</v>
       </c>
-      <c r="G31" s="5" t="n">
+      <c r="G31" s="7" t="n">
         <v>77.5</v>
       </c>
-      <c r="H31" s="8" t="n">
+      <c r="H31" s="9" t="n">
         <v>828</v>
       </c>
-      <c r="I31" s="5" t="n">
+      <c r="I31" s="7" t="n">
         <v>73.09999999999999</v>
       </c>
-      <c r="K31" s="6" t="n">
+      <c r="K31" s="5" t="n">
         <v>81.5</v>
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="8" t="n">
+      <c r="B32" s="9" t="n">
         <v>760</v>
       </c>
-      <c r="C32" s="5" t="n">
+      <c r="C32" s="6" t="n">
         <v>73</v>
       </c>
-      <c r="D32" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E32" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" s="4" t="n">
+      <c r="D32" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E32" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" s="5" t="n">
         <v>221</v>
       </c>
-      <c r="G32" s="5" t="n">
+      <c r="G32" s="6" t="n">
         <v>95.40000000000001</v>
       </c>
-      <c r="H32" s="8" t="n">
+      <c r="H32" s="9" t="n">
         <v>1114</v>
       </c>
-      <c r="I32" s="5" t="n">
+      <c r="I32" s="6" t="n">
         <v>67.3</v>
       </c>
-      <c r="K32" s="6" t="n">
+      <c r="K32" s="5" t="n">
         <v>81.3</v>
       </c>
     </row>
@@ -1626,63 +1629,63 @@
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="9" t="n">
+      <c r="B33" s="10" t="n">
         <v>1421</v>
       </c>
-      <c r="C33" s="5" t="n">
+      <c r="C33" s="7" t="n">
         <v>53.3</v>
       </c>
-      <c r="D33" s="7" t="n">
+      <c r="D33" s="8" t="n">
         <v>410</v>
       </c>
-      <c r="E33" s="5" t="n">
+      <c r="E33" s="7" t="n">
         <v>86.5</v>
       </c>
-      <c r="F33" s="7" t="n">
+      <c r="F33" s="8" t="n">
         <v>935</v>
       </c>
-      <c r="G33" s="5" t="n">
+      <c r="G33" s="7" t="n">
         <v>75.7</v>
       </c>
-      <c r="H33" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I33" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" s="6" t="n">
+      <c r="H33" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I33" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="5" t="n">
         <v>81.09999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:11">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B34" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C34" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" s="7" t="n">
+      <c r="B34" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C34" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" s="8" t="n">
         <v>484</v>
       </c>
-      <c r="E34" s="5" t="n">
+      <c r="E34" s="6" t="n">
         <v>84.90000000000001</v>
       </c>
-      <c r="F34" s="7" t="n">
+      <c r="F34" s="8" t="n">
         <v>872</v>
       </c>
-      <c r="G34" s="5" t="n">
+      <c r="G34" s="6" t="n">
         <v>77</v>
       </c>
-      <c r="H34" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I34" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K34" s="6" t="n">
+      <c r="H34" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I34" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K34" s="5" t="n">
         <v>81</v>
       </c>
     </row>
@@ -1690,63 +1693,63 @@
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="7" t="n">
+      <c r="B35" s="8" t="n">
         <v>567</v>
       </c>
-      <c r="C35" s="5" t="n">
+      <c r="C35" s="7" t="n">
         <v>82.40000000000001</v>
       </c>
-      <c r="D35" s="7" t="n">
+      <c r="D35" s="8" t="n">
         <v>865</v>
       </c>
-      <c r="E35" s="5" t="n">
+      <c r="E35" s="7" t="n">
         <v>77</v>
       </c>
-      <c r="F35" s="8" t="n">
+      <c r="F35" s="9" t="n">
         <v>1717</v>
       </c>
-      <c r="G35" s="5" t="n">
+      <c r="G35" s="7" t="n">
         <v>54.6</v>
       </c>
-      <c r="H35" s="7" t="n">
+      <c r="H35" s="8" t="n">
         <v>506</v>
       </c>
-      <c r="I35" s="5" t="n">
+      <c r="I35" s="7" t="n">
         <v>84.7</v>
       </c>
-      <c r="K35" s="6" t="n">
+      <c r="K35" s="5" t="n">
         <v>80.90000000000001</v>
       </c>
     </row>
     <row r="36" spans="1:11">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="9" t="n">
+      <c r="B36" s="10" t="n">
         <v>2181</v>
       </c>
-      <c r="C36" s="5" t="n">
+      <c r="C36" s="6" t="n">
         <v>36.4</v>
       </c>
-      <c r="D36" s="7" t="n">
+      <c r="D36" s="8" t="n">
         <v>460</v>
       </c>
-      <c r="E36" s="5" t="n">
+      <c r="E36" s="6" t="n">
         <v>85.40000000000001</v>
       </c>
-      <c r="F36" s="7" t="n">
+      <c r="F36" s="8" t="n">
         <v>967</v>
       </c>
-      <c r="G36" s="5" t="n">
+      <c r="G36" s="6" t="n">
         <v>75</v>
       </c>
-      <c r="H36" s="8" t="n">
+      <c r="H36" s="9" t="n">
         <v>1280</v>
       </c>
-      <c r="I36" s="5" t="n">
+      <c r="I36" s="6" t="n">
         <v>63.9</v>
       </c>
-      <c r="K36" s="6" t="n">
+      <c r="K36" s="5" t="n">
         <v>80.2</v>
       </c>
     </row>
@@ -1754,63 +1757,63 @@
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="8" t="n">
+      <c r="B37" s="9" t="n">
         <v>952</v>
       </c>
-      <c r="C37" s="5" t="n">
+      <c r="C37" s="7" t="n">
         <v>68.8</v>
       </c>
-      <c r="D37" s="7" t="n">
+      <c r="D37" s="8" t="n">
         <v>886</v>
       </c>
-      <c r="E37" s="5" t="n">
+      <c r="E37" s="7" t="n">
         <v>76.59999999999999</v>
       </c>
-      <c r="F37" s="8" t="n">
+      <c r="F37" s="9" t="n">
         <v>1971</v>
       </c>
-      <c r="G37" s="5" t="n">
+      <c r="G37" s="7" t="n">
         <v>49.3</v>
       </c>
-      <c r="H37" s="7" t="n">
+      <c r="H37" s="8" t="n">
         <v>625</v>
       </c>
-      <c r="I37" s="5" t="n">
+      <c r="I37" s="7" t="n">
         <v>82.3</v>
       </c>
-      <c r="K37" s="6" t="n">
+      <c r="K37" s="5" t="n">
         <v>79.40000000000001</v>
       </c>
     </row>
     <row r="38" spans="1:11">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="8" t="n">
+      <c r="B38" s="9" t="n">
         <v>1242</v>
       </c>
-      <c r="C38" s="5" t="n">
+      <c r="C38" s="6" t="n">
         <v>62.3</v>
       </c>
-      <c r="D38" s="7" t="n">
+      <c r="D38" s="8" t="n">
         <v>903</v>
       </c>
-      <c r="E38" s="5" t="n">
+      <c r="E38" s="6" t="n">
         <v>76.2</v>
       </c>
-      <c r="F38" s="8" t="n">
+      <c r="F38" s="9" t="n">
         <v>1582</v>
       </c>
-      <c r="G38" s="5" t="n">
+      <c r="G38" s="6" t="n">
         <v>57.3</v>
       </c>
-      <c r="H38" s="7" t="n">
+      <c r="H38" s="8" t="n">
         <v>621</v>
       </c>
-      <c r="I38" s="5" t="n">
+      <c r="I38" s="6" t="n">
         <v>82.3</v>
       </c>
-      <c r="K38" s="6" t="n">
+      <c r="K38" s="5" t="n">
         <v>79.2</v>
       </c>
     </row>
@@ -1818,63 +1821,63 @@
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="9" t="n">
+      <c r="B39" s="10" t="n">
         <v>1799</v>
       </c>
-      <c r="C39" s="5" t="n">
+      <c r="C39" s="7" t="n">
         <v>44.9</v>
       </c>
-      <c r="D39" s="7" t="n">
+      <c r="D39" s="8" t="n">
         <v>555</v>
       </c>
-      <c r="E39" s="5" t="n">
+      <c r="E39" s="7" t="n">
         <v>83.5</v>
       </c>
-      <c r="F39" s="8" t="n">
+      <c r="F39" s="9" t="n">
         <v>1622</v>
       </c>
-      <c r="G39" s="5" t="n">
+      <c r="G39" s="7" t="n">
         <v>56.5</v>
       </c>
-      <c r="H39" s="8" t="n">
+      <c r="H39" s="9" t="n">
         <v>769</v>
       </c>
-      <c r="I39" s="5" t="n">
+      <c r="I39" s="7" t="n">
         <v>74.3</v>
       </c>
-      <c r="K39" s="6" t="n">
+      <c r="K39" s="5" t="n">
         <v>78.90000000000001</v>
       </c>
     </row>
     <row r="40" spans="1:11">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="8" t="n">
+      <c r="B40" s="9" t="n">
         <v>1332</v>
       </c>
-      <c r="C40" s="5" t="n">
+      <c r="C40" s="6" t="n">
         <v>60.3</v>
       </c>
-      <c r="D40" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E40" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" s="7" t="n">
+      <c r="D40" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E40" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" s="8" t="n">
         <v>948</v>
       </c>
-      <c r="G40" s="5" t="n">
+      <c r="G40" s="6" t="n">
         <v>75.40000000000001</v>
       </c>
-      <c r="H40" s="7" t="n">
+      <c r="H40" s="8" t="n">
         <v>617</v>
       </c>
-      <c r="I40" s="5" t="n">
+      <c r="I40" s="6" t="n">
         <v>82.40000000000001</v>
       </c>
-      <c r="K40" s="6" t="n">
+      <c r="K40" s="5" t="n">
         <v>78.90000000000001</v>
       </c>
     </row>
@@ -1882,63 +1885,63 @@
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="8" t="n">
+      <c r="B41" s="9" t="n">
         <v>1272</v>
       </c>
-      <c r="C41" s="5" t="n">
+      <c r="C41" s="7" t="n">
         <v>61.6</v>
       </c>
-      <c r="D41" s="7" t="n">
+      <c r="D41" s="8" t="n">
         <v>451</v>
       </c>
-      <c r="E41" s="5" t="n">
+      <c r="E41" s="7" t="n">
         <v>85.59999999999999</v>
       </c>
-      <c r="F41" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G41" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="8" t="n">
+      <c r="F41" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G41" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="9" t="n">
         <v>897</v>
       </c>
-      <c r="I41" s="5" t="n">
+      <c r="I41" s="7" t="n">
         <v>71.7</v>
       </c>
-      <c r="K41" s="6" t="n">
+      <c r="K41" s="5" t="n">
         <v>78.7</v>
       </c>
     </row>
     <row r="42" spans="1:11">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="8" t="n">
+      <c r="B42" s="9" t="n">
         <v>730</v>
       </c>
-      <c r="C42" s="5" t="n">
+      <c r="C42" s="6" t="n">
         <v>73.7</v>
       </c>
-      <c r="D42" s="7" t="n">
+      <c r="D42" s="8" t="n">
         <v>1024</v>
       </c>
-      <c r="E42" s="5" t="n">
+      <c r="E42" s="6" t="n">
         <v>73.7</v>
       </c>
-      <c r="F42" s="7" t="n">
+      <c r="F42" s="8" t="n">
         <v>557</v>
       </c>
-      <c r="G42" s="5" t="n">
+      <c r="G42" s="6" t="n">
         <v>83.5</v>
       </c>
-      <c r="H42" s="8" t="n">
+      <c r="H42" s="9" t="n">
         <v>1092</v>
       </c>
-      <c r="I42" s="5" t="n">
+      <c r="I42" s="6" t="n">
         <v>67.7</v>
       </c>
-      <c r="K42" s="6" t="n">
+      <c r="K42" s="5" t="n">
         <v>78.59999999999999</v>
       </c>
     </row>
@@ -1946,63 +1949,63 @@
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C43" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" s="8" t="n">
+      <c r="B43" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C43" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="9" t="n">
         <v>1144</v>
       </c>
-      <c r="E43" s="5" t="n">
+      <c r="E43" s="7" t="n">
         <v>66.2</v>
       </c>
-      <c r="F43" s="7" t="n">
+      <c r="F43" s="8" t="n">
         <v>598</v>
       </c>
-      <c r="G43" s="5" t="n">
+      <c r="G43" s="7" t="n">
         <v>82.7</v>
       </c>
-      <c r="H43" s="8" t="n">
+      <c r="H43" s="9" t="n">
         <v>798</v>
       </c>
-      <c r="I43" s="5" t="n">
+      <c r="I43" s="7" t="n">
         <v>73.7</v>
       </c>
-      <c r="K43" s="6" t="n">
+      <c r="K43" s="5" t="n">
         <v>78.2</v>
       </c>
     </row>
     <row r="44" spans="1:11">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="8" t="n">
+      <c r="B44" s="9" t="n">
         <v>1210</v>
       </c>
-      <c r="C44" s="5" t="n">
+      <c r="C44" s="6" t="n">
         <v>63</v>
       </c>
-      <c r="D44" s="7" t="n">
+      <c r="D44" s="8" t="n">
         <v>648</v>
       </c>
-      <c r="E44" s="5" t="n">
+      <c r="E44" s="6" t="n">
         <v>81.5</v>
       </c>
-      <c r="F44" s="7" t="n">
+      <c r="F44" s="8" t="n">
         <v>985</v>
       </c>
-      <c r="G44" s="5" t="n">
+      <c r="G44" s="6" t="n">
         <v>74.7</v>
       </c>
-      <c r="H44" s="9" t="n">
+      <c r="H44" s="10" t="n">
         <v>1860</v>
       </c>
-      <c r="I44" s="5" t="n">
+      <c r="I44" s="6" t="n">
         <v>47.1</v>
       </c>
-      <c r="K44" s="6" t="n">
+      <c r="K44" s="5" t="n">
         <v>78.09999999999999</v>
       </c>
     </row>
@@ -2010,63 +2013,63 @@
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="8" t="n">
+      <c r="B45" s="9" t="n">
         <v>1136</v>
       </c>
-      <c r="C45" s="5" t="n">
+      <c r="C45" s="7" t="n">
         <v>64.7</v>
       </c>
-      <c r="D45" s="8" t="n">
+      <c r="D45" s="9" t="n">
         <v>1238</v>
       </c>
-      <c r="E45" s="5" t="n">
+      <c r="E45" s="7" t="n">
         <v>64.3</v>
       </c>
-      <c r="F45" s="8" t="n">
+      <c r="F45" s="9" t="n">
         <v>1178</v>
       </c>
-      <c r="G45" s="5" t="n">
+      <c r="G45" s="7" t="n">
         <v>65.7</v>
       </c>
-      <c r="H45" s="7" t="n">
+      <c r="H45" s="8" t="n">
         <v>268</v>
       </c>
-      <c r="I45" s="5" t="n">
+      <c r="I45" s="7" t="n">
         <v>89.5</v>
       </c>
-      <c r="K45" s="6" t="n">
+      <c r="K45" s="5" t="n">
         <v>77.59999999999999</v>
       </c>
     </row>
     <row r="46" spans="1:11">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="8" t="n">
+      <c r="B46" s="9" t="n">
         <v>901</v>
       </c>
-      <c r="C46" s="5" t="n">
+      <c r="C46" s="6" t="n">
         <v>69.90000000000001</v>
       </c>
-      <c r="D46" s="7" t="n">
+      <c r="D46" s="8" t="n">
         <v>350</v>
       </c>
-      <c r="E46" s="5" t="n">
+      <c r="E46" s="6" t="n">
         <v>87.7</v>
       </c>
-      <c r="F46" s="8" t="n">
+      <c r="F46" s="9" t="n">
         <v>1127</v>
       </c>
-      <c r="G46" s="5" t="n">
+      <c r="G46" s="6" t="n">
         <v>66.7</v>
       </c>
-      <c r="H46" s="9" t="n">
+      <c r="H46" s="10" t="n">
         <v>1573</v>
       </c>
-      <c r="I46" s="5" t="n">
+      <c r="I46" s="6" t="n">
         <v>52.9</v>
       </c>
-      <c r="K46" s="6" t="n">
+      <c r="K46" s="5" t="n">
         <v>77.2</v>
       </c>
     </row>
@@ -2074,63 +2077,63 @@
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C47" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" s="7" t="n">
+      <c r="B47" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C47" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="8" t="n">
         <v>958</v>
       </c>
-      <c r="E47" s="5" t="n">
+      <c r="E47" s="7" t="n">
         <v>75.09999999999999</v>
       </c>
-      <c r="F47" s="7" t="n">
+      <c r="F47" s="8" t="n">
         <v>817</v>
       </c>
-      <c r="G47" s="5" t="n">
+      <c r="G47" s="7" t="n">
         <v>78.09999999999999</v>
       </c>
-      <c r="H47" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I47" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K47" s="6" t="n">
+      <c r="H47" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I47" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="5" t="n">
         <v>76.59999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:11">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="9" t="n">
+      <c r="B48" s="10" t="n">
         <v>1855</v>
       </c>
-      <c r="C48" s="5" t="n">
+      <c r="C48" s="6" t="n">
         <v>43.6</v>
       </c>
-      <c r="D48" s="7" t="n">
+      <c r="D48" s="8" t="n">
         <v>892</v>
       </c>
-      <c r="E48" s="5" t="n">
+      <c r="E48" s="6" t="n">
         <v>76.5</v>
       </c>
-      <c r="F48" s="8" t="n">
+      <c r="F48" s="9" t="n">
         <v>1429</v>
       </c>
-      <c r="G48" s="5" t="n">
+      <c r="G48" s="6" t="n">
         <v>60.5</v>
       </c>
-      <c r="H48" s="8" t="n">
+      <c r="H48" s="9" t="n">
         <v>811</v>
       </c>
-      <c r="I48" s="5" t="n">
+      <c r="I48" s="6" t="n">
         <v>73.5</v>
       </c>
-      <c r="K48" s="6" t="n">
+      <c r="K48" s="5" t="n">
         <v>75</v>
       </c>
     </row>
@@ -2138,63 +2141,63 @@
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="8" t="n">
+      <c r="B49" s="9" t="n">
         <v>1133</v>
       </c>
-      <c r="C49" s="5" t="n">
+      <c r="C49" s="7" t="n">
         <v>64.7</v>
       </c>
-      <c r="D49" s="7" t="n">
+      <c r="D49" s="8" t="n">
         <v>975</v>
       </c>
-      <c r="E49" s="5" t="n">
+      <c r="E49" s="7" t="n">
         <v>74.7</v>
       </c>
-      <c r="F49" s="7" t="n">
+      <c r="F49" s="8" t="n">
         <v>959</v>
       </c>
-      <c r="G49" s="5" t="n">
+      <c r="G49" s="7" t="n">
         <v>75.2</v>
       </c>
-      <c r="H49" s="9" t="n">
+      <c r="H49" s="10" t="n">
         <v>1754</v>
       </c>
-      <c r="I49" s="5" t="n">
+      <c r="I49" s="7" t="n">
         <v>49.2</v>
       </c>
-      <c r="K49" s="6" t="n">
+      <c r="K49" s="5" t="n">
         <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:11">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="8" t="n">
+      <c r="B50" s="9" t="n">
         <v>1025</v>
       </c>
-      <c r="C50" s="5" t="n">
+      <c r="C50" s="6" t="n">
         <v>67.09999999999999</v>
       </c>
-      <c r="D50" s="9" t="n">
+      <c r="D50" s="10" t="n">
         <v>2546</v>
       </c>
-      <c r="E50" s="5" t="n">
+      <c r="E50" s="6" t="n">
         <v>32.1</v>
       </c>
-      <c r="F50" s="8" t="n">
+      <c r="F50" s="9" t="n">
         <v>1136</v>
       </c>
-      <c r="G50" s="5" t="n">
+      <c r="G50" s="6" t="n">
         <v>66.59999999999999</v>
       </c>
-      <c r="H50" s="7" t="n">
+      <c r="H50" s="8" t="n">
         <v>579</v>
       </c>
-      <c r="I50" s="5" t="n">
+      <c r="I50" s="6" t="n">
         <v>83.2</v>
       </c>
-      <c r="K50" s="6" t="n">
+      <c r="K50" s="5" t="n">
         <v>74.90000000000001</v>
       </c>
     </row>
@@ -2202,63 +2205,63 @@
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C51" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" s="7" t="n">
+      <c r="B51" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C51" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="8" t="n">
         <v>1043</v>
       </c>
-      <c r="E51" s="5" t="n">
+      <c r="E51" s="7" t="n">
         <v>73.3</v>
       </c>
-      <c r="F51" s="8" t="n">
+      <c r="F51" s="9" t="n">
         <v>2069</v>
       </c>
-      <c r="G51" s="5" t="n">
+      <c r="G51" s="7" t="n">
         <v>47.3</v>
       </c>
-      <c r="H51" s="8" t="n">
+      <c r="H51" s="9" t="n">
         <v>790</v>
       </c>
-      <c r="I51" s="5" t="n">
+      <c r="I51" s="7" t="n">
         <v>73.90000000000001</v>
       </c>
-      <c r="K51" s="6" t="n">
+      <c r="K51" s="5" t="n">
         <v>73.59999999999999</v>
       </c>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="9" t="n">
+      <c r="B52" s="10" t="n">
         <v>2018</v>
       </c>
-      <c r="C52" s="5" t="n">
+      <c r="C52" s="6" t="n">
         <v>40</v>
       </c>
-      <c r="D52" s="7" t="n">
+      <c r="D52" s="8" t="n">
         <v>510</v>
       </c>
-      <c r="E52" s="5" t="n">
+      <c r="E52" s="6" t="n">
         <v>84.40000000000001</v>
       </c>
-      <c r="F52" s="8" t="n">
+      <c r="F52" s="9" t="n">
         <v>1414</v>
       </c>
-      <c r="G52" s="5" t="n">
+      <c r="G52" s="6" t="n">
         <v>60.8</v>
       </c>
-      <c r="H52" s="9" t="n">
+      <c r="H52" s="10" t="n">
         <v>1900</v>
       </c>
-      <c r="I52" s="5" t="n">
+      <c r="I52" s="6" t="n">
         <v>46.3</v>
       </c>
-      <c r="K52" s="6" t="n">
+      <c r="K52" s="5" t="n">
         <v>72.59999999999999</v>
       </c>
     </row>
@@ -2266,63 +2269,63 @@
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="8" t="n">
+      <c r="B53" s="9" t="n">
         <v>870</v>
       </c>
-      <c r="C53" s="5" t="n">
+      <c r="C53" s="7" t="n">
         <v>70.59999999999999</v>
       </c>
-      <c r="D53" s="7" t="n">
+      <c r="D53" s="8" t="n">
         <v>385</v>
       </c>
-      <c r="E53" s="5" t="n">
+      <c r="E53" s="7" t="n">
         <v>87</v>
       </c>
-      <c r="F53" s="8" t="n">
+      <c r="F53" s="9" t="n">
         <v>1727</v>
       </c>
-      <c r="G53" s="5" t="n">
+      <c r="G53" s="7" t="n">
         <v>54.4</v>
       </c>
-      <c r="H53" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I53" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K53" s="6" t="n">
+      <c r="H53" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I53" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" s="5" t="n">
         <v>70.7</v>
       </c>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="8" t="n">
+      <c r="B54" s="9" t="n">
         <v>858</v>
       </c>
-      <c r="C54" s="5" t="n">
+      <c r="C54" s="6" t="n">
         <v>70.90000000000001</v>
       </c>
-      <c r="D54" s="7" t="n">
+      <c r="D54" s="8" t="n">
         <v>458</v>
       </c>
-      <c r="E54" s="5" t="n">
+      <c r="E54" s="6" t="n">
         <v>85.5</v>
       </c>
-      <c r="F54" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G54" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H54" s="9" t="n">
+      <c r="F54" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G54" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H54" s="10" t="n">
         <v>1463</v>
       </c>
-      <c r="I54" s="5" t="n">
+      <c r="I54" s="6" t="n">
         <v>55.2</v>
       </c>
-      <c r="K54" s="6" t="n">
+      <c r="K54" s="5" t="n">
         <v>70.3</v>
       </c>
     </row>
@@ -2330,63 +2333,63 @@
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C55" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" s="8" t="n">
+      <c r="B55" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C55" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" s="9" t="n">
         <v>1223</v>
       </c>
-      <c r="E55" s="5" t="n">
+      <c r="E55" s="7" t="n">
         <v>64.59999999999999</v>
       </c>
-      <c r="F55" s="8" t="n">
+      <c r="F55" s="9" t="n">
         <v>1340</v>
       </c>
-      <c r="G55" s="5" t="n">
+      <c r="G55" s="7" t="n">
         <v>62.3</v>
       </c>
-      <c r="H55" s="8" t="n">
+      <c r="H55" s="9" t="n">
         <v>740</v>
       </c>
-      <c r="I55" s="5" t="n">
+      <c r="I55" s="7" t="n">
         <v>74.90000000000001</v>
       </c>
-      <c r="K55" s="6" t="n">
+      <c r="K55" s="5" t="n">
         <v>69.8</v>
       </c>
     </row>
     <row r="56" spans="1:11">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="8" t="n">
+      <c r="B56" s="9" t="n">
         <v>736</v>
       </c>
-      <c r="C56" s="5" t="n">
+      <c r="C56" s="6" t="n">
         <v>73.59999999999999</v>
       </c>
-      <c r="D56" s="8" t="n">
+      <c r="D56" s="9" t="n">
         <v>1283</v>
       </c>
-      <c r="E56" s="5" t="n">
+      <c r="E56" s="6" t="n">
         <v>63.3</v>
       </c>
-      <c r="F56" s="9" t="n">
+      <c r="F56" s="10" t="n">
         <v>2615</v>
       </c>
-      <c r="G56" s="5" t="n">
+      <c r="G56" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="H56" s="8" t="n">
+      <c r="H56" s="9" t="n">
         <v>792</v>
       </c>
-      <c r="I56" s="5" t="n">
+      <c r="I56" s="6" t="n">
         <v>73.90000000000001</v>
       </c>
-      <c r="K56" s="6" t="n">
+      <c r="K56" s="5" t="n">
         <v>68.59999999999999</v>
       </c>
     </row>
@@ -2394,63 +2397,63 @@
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="8" t="n">
+      <c r="B57" s="9" t="n">
         <v>1109</v>
       </c>
-      <c r="C57" s="5" t="n">
+      <c r="C57" s="7" t="n">
         <v>65.3</v>
       </c>
-      <c r="D57" s="8" t="n">
+      <c r="D57" s="9" t="n">
         <v>1181</v>
       </c>
-      <c r="E57" s="5" t="n">
+      <c r="E57" s="7" t="n">
         <v>65.40000000000001</v>
       </c>
-      <c r="F57" s="8" t="n">
+      <c r="F57" s="9" t="n">
         <v>1223</v>
       </c>
-      <c r="G57" s="5" t="n">
+      <c r="G57" s="7" t="n">
         <v>64.8</v>
       </c>
-      <c r="H57" s="8" t="n">
+      <c r="H57" s="9" t="n">
         <v>913</v>
       </c>
-      <c r="I57" s="5" t="n">
+      <c r="I57" s="7" t="n">
         <v>71.40000000000001</v>
       </c>
-      <c r="K57" s="6" t="n">
+      <c r="K57" s="5" t="n">
         <v>68.40000000000001</v>
       </c>
     </row>
     <row r="58" spans="1:11">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="7" t="n">
+      <c r="B58" s="8" t="n">
         <v>315</v>
       </c>
-      <c r="C58" s="5" t="n">
+      <c r="C58" s="6" t="n">
         <v>88</v>
       </c>
-      <c r="D58" s="8" t="n">
+      <c r="D58" s="9" t="n">
         <v>2123</v>
       </c>
-      <c r="E58" s="5" t="n">
+      <c r="E58" s="6" t="n">
         <v>45.9</v>
       </c>
-      <c r="F58" s="7" t="n">
+      <c r="F58" s="8" t="n">
         <v>757</v>
       </c>
-      <c r="G58" s="5" t="n">
+      <c r="G58" s="6" t="n">
         <v>79.40000000000001</v>
       </c>
-      <c r="H58" s="9" t="n">
+      <c r="H58" s="10" t="n">
         <v>1642</v>
       </c>
-      <c r="I58" s="5" t="n">
+      <c r="I58" s="6" t="n">
         <v>51.5</v>
       </c>
-      <c r="K58" s="6" t="n">
+      <c r="K58" s="5" t="n">
         <v>65.5</v>
       </c>
     </row>
@@ -2458,63 +2461,63 @@
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="9" t="n">
+      <c r="B59" s="10" t="n">
         <v>2048</v>
       </c>
-      <c r="C59" s="5" t="n">
+      <c r="C59" s="7" t="n">
         <v>39.3</v>
       </c>
-      <c r="D59" s="8" t="n">
+      <c r="D59" s="9" t="n">
         <v>1234</v>
       </c>
-      <c r="E59" s="5" t="n">
+      <c r="E59" s="7" t="n">
         <v>64.3</v>
       </c>
-      <c r="F59" s="8" t="n">
+      <c r="F59" s="9" t="n">
         <v>1181</v>
       </c>
-      <c r="G59" s="5" t="n">
+      <c r="G59" s="7" t="n">
         <v>65.59999999999999</v>
       </c>
-      <c r="H59" s="8" t="n">
+      <c r="H59" s="9" t="n">
         <v>1297</v>
       </c>
-      <c r="I59" s="5" t="n">
+      <c r="I59" s="7" t="n">
         <v>63.6</v>
       </c>
-      <c r="K59" s="6" t="n">
+      <c r="K59" s="5" t="n">
         <v>65</v>
       </c>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="9" t="n">
+      <c r="B60" s="10" t="n">
         <v>2157</v>
       </c>
-      <c r="C60" s="5" t="n">
+      <c r="C60" s="6" t="n">
         <v>36.9</v>
       </c>
-      <c r="D60" s="8" t="n">
+      <c r="D60" s="9" t="n">
         <v>1642</v>
       </c>
-      <c r="E60" s="5" t="n">
+      <c r="E60" s="6" t="n">
         <v>55.9</v>
       </c>
-      <c r="F60" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G60" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H60" s="8" t="n">
+      <c r="F60" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G60" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H60" s="9" t="n">
         <v>789</v>
       </c>
-      <c r="I60" s="5" t="n">
+      <c r="I60" s="6" t="n">
         <v>73.90000000000001</v>
       </c>
-      <c r="K60" s="6" t="n">
+      <c r="K60" s="5" t="n">
         <v>64.90000000000001</v>
       </c>
     </row>
@@ -2522,63 +2525,63 @@
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="8" t="n">
+      <c r="B61" s="9" t="n">
         <v>1215</v>
       </c>
-      <c r="C61" s="5" t="n">
+      <c r="C61" s="7" t="n">
         <v>62.9</v>
       </c>
-      <c r="D61" s="8" t="n">
+      <c r="D61" s="9" t="n">
         <v>1648</v>
       </c>
-      <c r="E61" s="5" t="n">
+      <c r="E61" s="7" t="n">
         <v>55.7</v>
       </c>
-      <c r="F61" s="8" t="n">
+      <c r="F61" s="9" t="n">
         <v>1754</v>
       </c>
-      <c r="G61" s="5" t="n">
+      <c r="G61" s="7" t="n">
         <v>53.8</v>
       </c>
-      <c r="H61" s="8" t="n">
+      <c r="H61" s="9" t="n">
         <v>883</v>
       </c>
-      <c r="I61" s="5" t="n">
+      <c r="I61" s="7" t="n">
         <v>72</v>
       </c>
-      <c r="K61" s="6" t="n">
+      <c r="K61" s="5" t="n">
         <v>63.9</v>
       </c>
     </row>
     <row r="62" spans="1:11">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B62" s="5" t="n">
+      <c r="B62" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="C62" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D62" s="5" t="n">
+      <c r="C62" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="E62" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F62" s="7" t="n">
+      <c r="E62" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F62" s="8" t="n">
         <v>608</v>
       </c>
-      <c r="G62" s="5" t="n">
+      <c r="G62" s="6" t="n">
         <v>82.5</v>
       </c>
-      <c r="H62" s="9" t="n">
+      <c r="H62" s="10" t="n">
         <v>1959</v>
       </c>
-      <c r="I62" s="5" t="n">
+      <c r="I62" s="6" t="n">
         <v>45.1</v>
       </c>
-      <c r="K62" s="6" t="n">
+      <c r="K62" s="5" t="n">
         <v>63.8</v>
       </c>
     </row>
@@ -2586,63 +2589,63 @@
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B63" s="8" t="n">
+      <c r="B63" s="9" t="n">
         <v>867</v>
       </c>
-      <c r="C63" s="5" t="n">
+      <c r="C63" s="7" t="n">
         <v>70.7</v>
       </c>
-      <c r="D63" s="8" t="n">
+      <c r="D63" s="9" t="n">
         <v>1421</v>
       </c>
-      <c r="E63" s="5" t="n">
+      <c r="E63" s="7" t="n">
         <v>60.4</v>
       </c>
-      <c r="F63" s="9" t="n">
+      <c r="F63" s="10" t="n">
         <v>2124</v>
       </c>
-      <c r="G63" s="5" t="n">
+      <c r="G63" s="7" t="n">
         <v>41.2</v>
       </c>
-      <c r="H63" s="8" t="n">
+      <c r="H63" s="9" t="n">
         <v>1153</v>
       </c>
-      <c r="I63" s="5" t="n">
+      <c r="I63" s="7" t="n">
         <v>66.5</v>
       </c>
-      <c r="K63" s="6" t="n">
+      <c r="K63" s="5" t="n">
         <v>63.4</v>
       </c>
     </row>
     <row r="64" spans="1:11">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B64" s="8" t="n">
+      <c r="B64" s="9" t="n">
         <v>995</v>
       </c>
-      <c r="C64" s="5" t="n">
+      <c r="C64" s="6" t="n">
         <v>67.8</v>
       </c>
-      <c r="D64" s="7" t="n">
+      <c r="D64" s="8" t="n">
         <v>914</v>
       </c>
-      <c r="E64" s="5" t="n">
+      <c r="E64" s="6" t="n">
         <v>76</v>
       </c>
-      <c r="F64" s="8" t="n">
+      <c r="F64" s="9" t="n">
         <v>2034</v>
       </c>
-      <c r="G64" s="5" t="n">
+      <c r="G64" s="6" t="n">
         <v>48</v>
       </c>
-      <c r="H64" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I64" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K64" s="6" t="n">
+      <c r="H64" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I64" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K64" s="5" t="n">
         <v>62</v>
       </c>
     </row>
@@ -2650,63 +2653,63 @@
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="9" t="n">
+      <c r="B65" s="10" t="n">
         <v>1537</v>
       </c>
-      <c r="C65" s="5" t="n">
+      <c r="C65" s="7" t="n">
         <v>50.7</v>
       </c>
-      <c r="D65" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E65" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F65" s="7" t="n">
+      <c r="D65" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E65" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="8" t="n">
         <v>986</v>
       </c>
-      <c r="G65" s="5" t="n">
+      <c r="G65" s="7" t="n">
         <v>74.59999999999999</v>
       </c>
-      <c r="H65" s="9" t="n">
+      <c r="H65" s="10" t="n">
         <v>1778</v>
       </c>
-      <c r="I65" s="5" t="n">
+      <c r="I65" s="7" t="n">
         <v>48.8</v>
       </c>
-      <c r="K65" s="6" t="n">
+      <c r="K65" s="5" t="n">
         <v>61.7</v>
       </c>
     </row>
     <row r="66" spans="1:11">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="9" t="n">
+      <c r="B66" s="10" t="n">
         <v>2119</v>
       </c>
-      <c r="C66" s="5" t="n">
+      <c r="C66" s="6" t="n">
         <v>37.7</v>
       </c>
-      <c r="D66" s="8" t="n">
+      <c r="D66" s="9" t="n">
         <v>1412</v>
       </c>
-      <c r="E66" s="5" t="n">
+      <c r="E66" s="6" t="n">
         <v>60.6</v>
       </c>
-      <c r="F66" s="8" t="n">
+      <c r="F66" s="9" t="n">
         <v>1876</v>
       </c>
-      <c r="G66" s="5" t="n">
+      <c r="G66" s="6" t="n">
         <v>51.3</v>
       </c>
-      <c r="H66" s="9" t="n">
+      <c r="H66" s="10" t="n">
         <v>1373</v>
       </c>
-      <c r="I66" s="5" t="n">
+      <c r="I66" s="6" t="n">
         <v>57</v>
       </c>
-      <c r="K66" s="6" t="n">
+      <c r="K66" s="5" t="n">
         <v>58.8</v>
       </c>
     </row>
@@ -2714,63 +2717,63 @@
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B67" s="9" t="n">
+      <c r="B67" s="10" t="n">
         <v>2011</v>
       </c>
-      <c r="C67" s="5" t="n">
+      <c r="C67" s="7" t="n">
         <v>40.1</v>
       </c>
-      <c r="D67" s="8" t="n">
+      <c r="D67" s="9" t="n">
         <v>1398</v>
       </c>
-      <c r="E67" s="5" t="n">
+      <c r="E67" s="7" t="n">
         <v>60.9</v>
       </c>
-      <c r="F67" s="8" t="n">
+      <c r="F67" s="9" t="n">
         <v>2099</v>
       </c>
-      <c r="G67" s="5" t="n">
+      <c r="G67" s="7" t="n">
         <v>46.7</v>
       </c>
-      <c r="H67" s="9" t="n">
+      <c r="H67" s="10" t="n">
         <v>1665</v>
       </c>
-      <c r="I67" s="5" t="n">
+      <c r="I67" s="7" t="n">
         <v>51.1</v>
       </c>
-      <c r="K67" s="6" t="n">
+      <c r="K67" s="5" t="n">
         <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:11">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B68" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C68" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D68" s="7" t="n">
+      <c r="B68" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C68" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D68" s="8" t="n">
         <v>942</v>
       </c>
-      <c r="E68" s="5" t="n">
+      <c r="E68" s="6" t="n">
         <v>75.40000000000001</v>
       </c>
-      <c r="F68" s="9" t="n">
+      <c r="F68" s="10" t="n">
         <v>2382</v>
       </c>
-      <c r="G68" s="5" t="n">
+      <c r="G68" s="6" t="n">
         <v>35.8</v>
       </c>
-      <c r="H68" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I68" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K68" s="6" t="n">
+      <c r="H68" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I68" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K68" s="5" t="n">
         <v>55.6</v>
       </c>
     </row>
@@ -2778,63 +2781,63 @@
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B69" s="9" t="n">
+      <c r="B69" s="10" t="n">
         <v>2014</v>
       </c>
-      <c r="C69" s="5" t="n">
+      <c r="C69" s="7" t="n">
         <v>40.1</v>
       </c>
-      <c r="D69" s="8" t="n">
+      <c r="D69" s="9" t="n">
         <v>2067</v>
       </c>
-      <c r="E69" s="5" t="n">
+      <c r="E69" s="7" t="n">
         <v>47</v>
       </c>
-      <c r="F69" s="8" t="n">
+      <c r="F69" s="9" t="n">
         <v>1309</v>
       </c>
-      <c r="G69" s="5" t="n">
+      <c r="G69" s="7" t="n">
         <v>63</v>
       </c>
-      <c r="H69" s="9" t="n">
+      <c r="H69" s="10" t="n">
         <v>1917</v>
       </c>
-      <c r="I69" s="5" t="n">
+      <c r="I69" s="7" t="n">
         <v>45.9</v>
       </c>
-      <c r="K69" s="6" t="n">
+      <c r="K69" s="5" t="n">
         <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:11">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B70" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C70" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D70" s="8" t="n">
+      <c r="B70" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C70" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D70" s="9" t="n">
         <v>1657</v>
       </c>
-      <c r="E70" s="5" t="n">
+      <c r="E70" s="6" t="n">
         <v>55.5</v>
       </c>
-      <c r="F70" s="8" t="n">
+      <c r="F70" s="9" t="n">
         <v>1955</v>
       </c>
-      <c r="G70" s="5" t="n">
+      <c r="G70" s="6" t="n">
         <v>49.6</v>
       </c>
-      <c r="H70" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I70" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K70" s="6" t="n">
+      <c r="H70" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I70" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K70" s="5" t="n">
         <v>52.5</v>
       </c>
     </row>
@@ -2842,63 +2845,63 @@
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="9" t="n">
+      <c r="B71" s="10" t="n">
         <v>1637</v>
       </c>
-      <c r="C71" s="5" t="n">
+      <c r="C71" s="7" t="n">
         <v>48.5</v>
       </c>
-      <c r="D71" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E71" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F71" s="9" t="n">
+      <c r="D71" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E71" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="10" t="n">
         <v>2217</v>
       </c>
-      <c r="G71" s="5" t="n">
+      <c r="G71" s="7" t="n">
         <v>39.2</v>
       </c>
-      <c r="H71" s="8" t="n">
+      <c r="H71" s="9" t="n">
         <v>1275</v>
       </c>
-      <c r="I71" s="5" t="n">
+      <c r="I71" s="7" t="n">
         <v>64</v>
       </c>
-      <c r="K71" s="6" t="n">
+      <c r="K71" s="5" t="n">
         <v>51.6</v>
       </c>
     </row>
     <row r="72" spans="1:11">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B72" s="5" t="n">
+      <c r="B72" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="C72" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D72" s="5" t="n">
+      <c r="C72" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D72" s="6" t="n">
         <v>-2</v>
       </c>
-      <c r="E72" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F72" s="8" t="n">
+      <c r="E72" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F72" s="9" t="n">
         <v>1761</v>
       </c>
-      <c r="G72" s="5" t="n">
+      <c r="G72" s="6" t="n">
         <v>53.7</v>
       </c>
-      <c r="H72" s="9" t="n">
+      <c r="H72" s="10" t="n">
         <v>1838</v>
       </c>
-      <c r="I72" s="5" t="n">
+      <c r="I72" s="6" t="n">
         <v>47.5</v>
       </c>
-      <c r="K72" s="6" t="n">
+      <c r="K72" s="5" t="n">
         <v>50.6</v>
       </c>
     </row>
@@ -2906,63 +2909,63 @@
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B73" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C73" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D73" s="8" t="n">
+      <c r="B73" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C73" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" s="9" t="n">
         <v>2027</v>
       </c>
-      <c r="E73" s="5" t="n">
+      <c r="E73" s="7" t="n">
         <v>47.8</v>
       </c>
-      <c r="F73" s="8" t="n">
+      <c r="F73" s="9" t="n">
         <v>2079</v>
       </c>
-      <c r="G73" s="5" t="n">
+      <c r="G73" s="7" t="n">
         <v>47.1</v>
       </c>
-      <c r="H73" s="9" t="n">
+      <c r="H73" s="10" t="n">
         <v>1762</v>
       </c>
-      <c r="I73" s="5" t="n">
+      <c r="I73" s="7" t="n">
         <v>49.1</v>
       </c>
-      <c r="K73" s="6" t="n">
+      <c r="K73" s="5" t="n">
         <v>48.5</v>
       </c>
     </row>
     <row r="74" spans="1:11">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="7" t="n">
+      <c r="B74" s="8" t="n">
         <v>461</v>
       </c>
-      <c r="C74" s="5" t="n">
+      <c r="C74" s="6" t="n">
         <v>84.7</v>
       </c>
-      <c r="D74" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E74" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F74" s="7" t="n">
+      <c r="D74" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E74" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F74" s="8" t="n">
         <v>544</v>
       </c>
-      <c r="G74" s="5" t="n">
+      <c r="G74" s="6" t="n">
         <v>83.8</v>
       </c>
-      <c r="H74" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I74" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K74" s="6" t="n">
+      <c r="H74" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I74" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K74" s="5" t="n">
         <v>41.9</v>
       </c>
     </row>
@@ -2970,63 +2973,63 @@
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B75" s="8" t="n">
+      <c r="B75" s="9" t="n">
         <v>1361</v>
       </c>
-      <c r="C75" s="5" t="n">
+      <c r="C75" s="7" t="n">
         <v>59.6</v>
       </c>
-      <c r="D75" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E75" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F75" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G75" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H75" s="8" t="n">
+      <c r="D75" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E75" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G75" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" s="9" t="n">
         <v>908</v>
       </c>
-      <c r="I75" s="5" t="n">
+      <c r="I75" s="7" t="n">
         <v>71.5</v>
       </c>
-      <c r="K75" s="6" t="n">
+      <c r="K75" s="5" t="n">
         <v>35.8</v>
       </c>
     </row>
     <row r="76" spans="1:11">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B76" s="7" t="n">
+      <c r="B76" s="8" t="n">
         <v>641</v>
       </c>
-      <c r="C76" s="5" t="n">
+      <c r="C76" s="6" t="n">
         <v>80.7</v>
       </c>
-      <c r="D76" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E76" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F76" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G76" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H76" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I76" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K76" s="6" t="n">
+      <c r="D76" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E76" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F76" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G76" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H76" s="6" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I76" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="K76" s="5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3034,41 +3037,41 @@
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B77" s="5" t="n">
+      <c r="B77" s="7" t="n">
         <v>-2</v>
       </c>
-      <c r="C77" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D77" s="5" t="n">
+      <c r="C77" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" s="7" t="n">
         <v>-2</v>
       </c>
-      <c r="E77" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F77" s="5" t="n">
+      <c r="E77" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" s="7" t="n">
         <v>-2</v>
       </c>
-      <c r="G77" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H77" s="5" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I77" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K77" s="6" t="n">
+      <c r="G77" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" s="7" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I77" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" s="5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="10" t="s">
+      <c r="A80" s="11" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="10" t="s">
+      <c r="A81" s="11" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix a color bug
</commit_message>
<xml_diff>
--- a/generateEXCEL/index.xlsx
+++ b/generateEXCEL/index.xlsx
@@ -272,7 +272,7 @@
       <sz val="15"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill/>
     </fill>
@@ -292,6 +292,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0019b457"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00ffb261"/>
       </patternFill>
     </fill>
     <fill>
@@ -322,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
@@ -342,16 +347,19 @@
     <xf applyAlignment="1" borderId="0" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="7" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="8" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -725,7 +733,7 @@
       <c r="I4" s="6" t="n">
         <v>99.90000000000001</v>
       </c>
-      <c r="K4" s="5" t="n">
+      <c r="K4" s="7" t="n">
         <v>99.8</v>
       </c>
     </row>
@@ -736,28 +744,28 @@
       <c r="B5" s="5" t="n">
         <v>51</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="8" t="n">
         <v>98.90000000000001</v>
       </c>
       <c r="D5" s="5" t="n">
         <v>36</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="8" t="n">
         <v>99.3</v>
       </c>
       <c r="F5" s="5" t="n">
         <v>7</v>
       </c>
-      <c r="G5" s="7" t="n">
+      <c r="G5" s="8" t="n">
         <v>99.90000000000001</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>39</v>
       </c>
-      <c r="I5" s="7" t="n">
+      <c r="I5" s="8" t="n">
         <v>99.2</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="7" t="n">
         <v>99.59999999999999</v>
       </c>
     </row>
@@ -765,7 +773,7 @@
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="n">
+      <c r="B6" s="9" t="n">
         <v>324</v>
       </c>
       <c r="C6" s="6" t="n">
@@ -789,7 +797,7 @@
       <c r="I6" s="6" t="n">
         <v>97.7</v>
       </c>
-      <c r="K6" s="5" t="n">
+      <c r="K6" s="7" t="n">
         <v>98.2</v>
       </c>
     </row>
@@ -797,31 +805,31 @@
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="n">
+      <c r="B7" s="9" t="n">
         <v>233</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="8" t="n">
         <v>89.8</v>
       </c>
-      <c r="D7" s="9" t="n">
+      <c r="D7" s="10" t="n">
         <v>2069</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="8" t="n">
         <v>47</v>
       </c>
       <c r="F7" s="5" t="n">
         <v>178</v>
       </c>
-      <c r="G7" s="7" t="n">
+      <c r="G7" s="8" t="n">
         <v>96.3</v>
       </c>
       <c r="H7" s="5" t="n">
         <v>61</v>
       </c>
-      <c r="I7" s="7" t="n">
+      <c r="I7" s="8" t="n">
         <v>98.8</v>
       </c>
-      <c r="K7" s="5" t="n">
+      <c r="K7" s="7" t="n">
         <v>97.5</v>
       </c>
     </row>
@@ -841,7 +849,7 @@
       <c r="E8" s="6" t="n">
         <v>96.59999999999999</v>
       </c>
-      <c r="F8" s="8" t="n">
+      <c r="F8" s="9" t="n">
         <v>675</v>
       </c>
       <c r="G8" s="6" t="n">
@@ -853,7 +861,7 @@
       <c r="I8" s="6" t="n">
         <v>97.8</v>
       </c>
-      <c r="K8" s="5" t="n">
+      <c r="K8" s="7" t="n">
         <v>97.2</v>
       </c>
     </row>
@@ -864,28 +872,28 @@
       <c r="B9" s="5" t="n">
         <v>112</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="8" t="n">
         <v>97.5</v>
       </c>
       <c r="D9" s="5" t="n">
         <v>164</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="8" t="n">
         <v>96.59999999999999</v>
       </c>
       <c r="F9" s="5" t="n">
         <v>154</v>
       </c>
-      <c r="G9" s="7" t="n">
+      <c r="G9" s="8" t="n">
         <v>96.8</v>
       </c>
-      <c r="H9" s="8" t="n">
+      <c r="H9" s="9" t="n">
         <v>637</v>
       </c>
-      <c r="I9" s="7" t="n">
+      <c r="I9" s="8" t="n">
         <v>82</v>
       </c>
-      <c r="K9" s="5" t="n">
+      <c r="K9" s="7" t="n">
         <v>96.7</v>
       </c>
     </row>
@@ -917,7 +925,7 @@
       <c r="I10" s="6" t="n">
         <v>96.59999999999999</v>
       </c>
-      <c r="K10" s="5" t="n">
+      <c r="K10" s="7" t="n">
         <v>96.59999999999999</v>
       </c>
     </row>
@@ -925,31 +933,31 @@
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="n">
+      <c r="B11" s="9" t="n">
         <v>251</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="8" t="n">
         <v>89.40000000000001</v>
       </c>
       <c r="D11" s="5" t="n">
         <v>127</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="E11" s="8" t="n">
         <v>97.40000000000001</v>
       </c>
-      <c r="F11" s="8" t="n">
+      <c r="F11" s="9" t="n">
         <v>581</v>
       </c>
-      <c r="G11" s="7" t="n">
+      <c r="G11" s="8" t="n">
         <v>83</v>
       </c>
       <c r="H11" s="5" t="n">
         <v>218</v>
       </c>
-      <c r="I11" s="7" t="n">
+      <c r="I11" s="8" t="n">
         <v>95.59999999999999</v>
       </c>
-      <c r="K11" s="5" t="n">
+      <c r="K11" s="7" t="n">
         <v>96.5</v>
       </c>
     </row>
@@ -957,7 +965,7 @@
       <c r="A12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="9" t="n">
         <v>514</v>
       </c>
       <c r="C12" s="6" t="n">
@@ -975,13 +983,13 @@
       <c r="G12" s="6" t="n">
         <v>95.40000000000001</v>
       </c>
-      <c r="H12" s="8" t="n">
+      <c r="H12" s="9" t="n">
         <v>250</v>
       </c>
       <c r="I12" s="6" t="n">
         <v>89.90000000000001</v>
       </c>
-      <c r="K12" s="5" t="n">
+      <c r="K12" s="7" t="n">
         <v>96.40000000000001</v>
       </c>
     </row>
@@ -989,31 +997,31 @@
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="9" t="n">
         <v>429</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="8" t="n">
         <v>85.40000000000001</v>
       </c>
       <c r="D13" s="5" t="n">
         <v>174</v>
       </c>
-      <c r="E13" s="7" t="n">
+      <c r="E13" s="8" t="n">
         <v>96.40000000000001</v>
       </c>
       <c r="F13" s="5" t="n">
         <v>322</v>
       </c>
-      <c r="G13" s="7" t="n">
+      <c r="G13" s="8" t="n">
         <v>93.40000000000001</v>
       </c>
-      <c r="H13" s="8" t="n">
+      <c r="H13" s="9" t="n">
         <v>492</v>
       </c>
-      <c r="I13" s="7" t="n">
+      <c r="I13" s="8" t="n">
         <v>85</v>
       </c>
-      <c r="K13" s="5" t="n">
+      <c r="K13" s="7" t="n">
         <v>94.90000000000001</v>
       </c>
     </row>
@@ -1021,13 +1029,13 @@
       <c r="A14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="10" t="n">
+      <c r="B14" s="11" t="n">
         <v>1455</v>
       </c>
       <c r="C14" s="6" t="n">
         <v>52.5</v>
       </c>
-      <c r="D14" s="8" t="n">
+      <c r="D14" s="9" t="n">
         <v>1023</v>
       </c>
       <c r="E14" s="6" t="n">
@@ -1045,7 +1053,7 @@
       <c r="I14" s="6" t="n">
         <v>96.2</v>
       </c>
-      <c r="K14" s="5" t="n">
+      <c r="K14" s="7" t="n">
         <v>94.59999999999999</v>
       </c>
     </row>
@@ -1056,28 +1064,28 @@
       <c r="B15" s="5" t="n">
         <v>60</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="8" t="n">
         <v>98.7</v>
       </c>
-      <c r="D15" s="8" t="n">
+      <c r="D15" s="9" t="n">
         <v>454</v>
       </c>
-      <c r="E15" s="7" t="n">
+      <c r="E15" s="8" t="n">
         <v>85.59999999999999</v>
       </c>
       <c r="F15" s="5" t="n">
         <v>425</v>
       </c>
-      <c r="G15" s="7" t="n">
+      <c r="G15" s="8" t="n">
         <v>91.2</v>
       </c>
       <c r="H15" s="5" t="n">
         <v>103</v>
       </c>
-      <c r="I15" s="7" t="n">
+      <c r="I15" s="8" t="n">
         <v>97.90000000000001</v>
       </c>
-      <c r="K15" s="5" t="n">
+      <c r="K15" s="7" t="n">
         <v>94.59999999999999</v>
       </c>
     </row>
@@ -1085,13 +1093,13 @@
       <c r="A16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="8" t="n">
+      <c r="B16" s="9" t="n">
         <v>642</v>
       </c>
       <c r="C16" s="6" t="n">
         <v>80.7</v>
       </c>
-      <c r="D16" s="8" t="n">
+      <c r="D16" s="9" t="n">
         <v>672</v>
       </c>
       <c r="E16" s="6" t="n">
@@ -1109,7 +1117,7 @@
       <c r="I16" s="6" t="n">
         <v>95.8</v>
       </c>
-      <c r="K16" s="5" t="n">
+      <c r="K16" s="7" t="n">
         <v>92.59999999999999</v>
       </c>
     </row>
@@ -1117,31 +1125,31 @@
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="8" t="n">
+      <c r="B17" s="9" t="n">
         <v>578</v>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="8" t="n">
         <v>82.09999999999999</v>
       </c>
       <c r="D17" s="5" t="n">
         <v>233</v>
       </c>
-      <c r="E17" s="7" t="n">
+      <c r="E17" s="8" t="n">
         <v>95.2</v>
       </c>
       <c r="F17" s="5" t="n">
         <v>502</v>
       </c>
-      <c r="G17" s="7" t="n">
+      <c r="G17" s="8" t="n">
         <v>89.59999999999999</v>
       </c>
-      <c r="H17" s="10" t="n">
+      <c r="H17" s="11" t="n">
         <v>1641</v>
       </c>
-      <c r="I17" s="7" t="n">
+      <c r="I17" s="8" t="n">
         <v>51.5</v>
       </c>
-      <c r="K17" s="5" t="n">
+      <c r="K17" s="7" t="n">
         <v>92.40000000000001</v>
       </c>
     </row>
@@ -1149,13 +1157,13 @@
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="8" t="n">
+      <c r="B18" s="9" t="n">
         <v>301</v>
       </c>
       <c r="C18" s="6" t="n">
         <v>88.3</v>
       </c>
-      <c r="D18" s="8" t="n">
+      <c r="D18" s="9" t="n">
         <v>344</v>
       </c>
       <c r="E18" s="6" t="n">
@@ -1173,7 +1181,7 @@
       <c r="I18" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="K18" s="5" t="n">
+      <c r="K18" s="7" t="n">
         <v>91.5</v>
       </c>
     </row>
@@ -1181,31 +1189,31 @@
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="8" t="n">
+      <c r="B19" s="9" t="n">
         <v>500</v>
       </c>
-      <c r="C19" s="7" t="n">
+      <c r="C19" s="8" t="n">
         <v>83.8</v>
       </c>
       <c r="D19" s="5" t="n">
         <v>225</v>
       </c>
-      <c r="E19" s="7" t="n">
+      <c r="E19" s="8" t="n">
         <v>95.3</v>
       </c>
-      <c r="F19" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G19" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H19" s="8" t="n">
+      <c r="F19" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G19" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9" t="n">
         <v>430</v>
       </c>
-      <c r="I19" s="7" t="n">
+      <c r="I19" s="8" t="n">
         <v>86.2</v>
       </c>
-      <c r="K19" s="5" t="n">
+      <c r="K19" s="7" t="n">
         <v>90.8</v>
       </c>
     </row>
@@ -1213,13 +1221,13 @@
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9" t="n">
+      <c r="B20" s="10" t="n">
         <v>1266</v>
       </c>
       <c r="C20" s="6" t="n">
         <v>61.8</v>
       </c>
-      <c r="D20" s="8" t="n">
+      <c r="D20" s="9" t="n">
         <v>345</v>
       </c>
       <c r="E20" s="6" t="n">
@@ -1231,13 +1239,13 @@
       <c r="G20" s="6" t="n">
         <v>93</v>
       </c>
-      <c r="H20" s="8" t="n">
+      <c r="H20" s="9" t="n">
         <v>488</v>
       </c>
       <c r="I20" s="6" t="n">
         <v>85.09999999999999</v>
       </c>
-      <c r="K20" s="5" t="n">
+      <c r="K20" s="7" t="n">
         <v>90.40000000000001</v>
       </c>
     </row>
@@ -1245,31 +1253,31 @@
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="8" t="n">
+      <c r="B21" s="9" t="n">
         <v>290</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="8" t="n">
         <v>88.5</v>
       </c>
-      <c r="D21" s="8" t="n">
+      <c r="D21" s="9" t="n">
         <v>443</v>
       </c>
-      <c r="E21" s="7" t="n">
+      <c r="E21" s="8" t="n">
         <v>85.8</v>
       </c>
       <c r="F21" s="5" t="n">
         <v>336</v>
       </c>
-      <c r="G21" s="7" t="n">
+      <c r="G21" s="8" t="n">
         <v>93.09999999999999</v>
       </c>
-      <c r="H21" s="8" t="n">
+      <c r="H21" s="9" t="n">
         <v>497</v>
       </c>
-      <c r="I21" s="7" t="n">
+      <c r="I21" s="8" t="n">
         <v>84.90000000000001</v>
       </c>
-      <c r="K21" s="5" t="n">
+      <c r="K21" s="7" t="n">
         <v>89.5</v>
       </c>
     </row>
@@ -1277,7 +1285,7 @@
       <c r="A22" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="9" t="n">
+      <c r="B22" s="10" t="n">
         <v>1302</v>
       </c>
       <c r="C22" s="6" t="n">
@@ -1295,13 +1303,13 @@
       <c r="G22" s="6" t="n">
         <v>95</v>
       </c>
-      <c r="H22" s="8" t="n">
+      <c r="H22" s="9" t="n">
         <v>560</v>
       </c>
       <c r="I22" s="6" t="n">
         <v>83.59999999999999</v>
       </c>
-      <c r="K22" s="5" t="n">
+      <c r="K22" s="7" t="n">
         <v>89.3</v>
       </c>
     </row>
@@ -1309,31 +1317,31 @@
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="8" t="n">
+      <c r="B23" s="9" t="n">
         <v>612</v>
       </c>
-      <c r="C23" s="7" t="n">
+      <c r="C23" s="8" t="n">
         <v>81.40000000000001</v>
       </c>
-      <c r="D23" s="10" t="n">
+      <c r="D23" s="11" t="n">
         <v>2384</v>
       </c>
-      <c r="E23" s="7" t="n">
+      <c r="E23" s="8" t="n">
         <v>35.4</v>
       </c>
       <c r="F23" s="5" t="n">
         <v>397</v>
       </c>
-      <c r="G23" s="7" t="n">
+      <c r="G23" s="8" t="n">
         <v>91.8</v>
       </c>
-      <c r="H23" s="8" t="n">
+      <c r="H23" s="9" t="n">
         <v>561</v>
       </c>
-      <c r="I23" s="7" t="n">
+      <c r="I23" s="8" t="n">
         <v>83.59999999999999</v>
       </c>
-      <c r="K23" s="5" t="n">
+      <c r="K23" s="7" t="n">
         <v>87.7</v>
       </c>
     </row>
@@ -1341,31 +1349,31 @@
       <c r="A24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="8" t="n">
+      <c r="B24" s="9" t="n">
         <v>394</v>
       </c>
       <c r="C24" s="6" t="n">
         <v>86.2</v>
       </c>
-      <c r="D24" s="8" t="n">
+      <c r="D24" s="9" t="n">
         <v>509</v>
       </c>
       <c r="E24" s="6" t="n">
         <v>84.40000000000001</v>
       </c>
-      <c r="F24" s="10" t="n">
+      <c r="F24" s="11" t="n">
         <v>2350</v>
       </c>
       <c r="G24" s="6" t="n">
         <v>36.5</v>
       </c>
-      <c r="H24" s="8" t="n">
+      <c r="H24" s="9" t="n">
         <v>276</v>
       </c>
       <c r="I24" s="6" t="n">
         <v>89.40000000000001</v>
       </c>
-      <c r="K24" s="5" t="n">
+      <c r="K24" s="7" t="n">
         <v>86.90000000000001</v>
       </c>
     </row>
@@ -1373,31 +1381,31 @@
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9" t="n">
+      <c r="B25" s="10" t="n">
         <v>1191</v>
       </c>
-      <c r="C25" s="7" t="n">
+      <c r="C25" s="8" t="n">
         <v>63.4</v>
       </c>
-      <c r="D25" s="8" t="n">
+      <c r="D25" s="9" t="n">
         <v>638</v>
       </c>
-      <c r="E25" s="7" t="n">
+      <c r="E25" s="8" t="n">
         <v>81.7</v>
       </c>
-      <c r="F25" s="8" t="n">
+      <c r="F25" s="9" t="n">
         <v>645</v>
       </c>
-      <c r="G25" s="7" t="n">
+      <c r="G25" s="8" t="n">
         <v>81.7</v>
       </c>
-      <c r="H25" s="8" t="n">
+      <c r="H25" s="9" t="n">
         <v>271</v>
       </c>
-      <c r="I25" s="7" t="n">
+      <c r="I25" s="8" t="n">
         <v>89.5</v>
       </c>
-      <c r="K25" s="5" t="n">
+      <c r="K25" s="7" t="n">
         <v>85.59999999999999</v>
       </c>
     </row>
@@ -1411,7 +1419,7 @@
       <c r="C26" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D26" s="8" t="n">
+      <c r="D26" s="9" t="n">
         <v>711</v>
       </c>
       <c r="E26" s="6" t="n">
@@ -1423,13 +1431,13 @@
       <c r="G26" s="6" t="n">
         <v>90.2</v>
       </c>
-      <c r="H26" s="9" t="n">
+      <c r="H26" s="10" t="n">
         <v>806</v>
       </c>
       <c r="I26" s="6" t="n">
         <v>73.59999999999999</v>
       </c>
-      <c r="K26" s="5" t="n">
+      <c r="K26" s="7" t="n">
         <v>85.2</v>
       </c>
     </row>
@@ -1437,31 +1445,31 @@
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="10" t="n">
+      <c r="B27" s="11" t="n">
         <v>1904</v>
       </c>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="8" t="n">
         <v>42.5</v>
       </c>
-      <c r="D27" s="8" t="n">
+      <c r="D27" s="9" t="n">
         <v>793</v>
       </c>
-      <c r="E27" s="7" t="n">
+      <c r="E27" s="8" t="n">
         <v>78.5</v>
       </c>
       <c r="F27" s="5" t="n">
         <v>420</v>
       </c>
-      <c r="G27" s="7" t="n">
+      <c r="G27" s="8" t="n">
         <v>91.3</v>
       </c>
-      <c r="H27" s="9" t="n">
+      <c r="H27" s="10" t="n">
         <v>721</v>
       </c>
-      <c r="I27" s="7" t="n">
+      <c r="I27" s="8" t="n">
         <v>75.3</v>
       </c>
-      <c r="K27" s="5" t="n">
+      <c r="K27" s="7" t="n">
         <v>84.90000000000001</v>
       </c>
     </row>
@@ -1487,13 +1495,13 @@
       <c r="G28" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H28" s="8" t="n">
+      <c r="H28" s="9" t="n">
         <v>541</v>
       </c>
       <c r="I28" s="6" t="n">
         <v>84</v>
       </c>
-      <c r="K28" s="5" t="n">
+      <c r="K28" s="7" t="n">
         <v>84</v>
       </c>
     </row>
@@ -1501,31 +1509,31 @@
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="9" t="n">
+      <c r="B29" s="10" t="n">
         <v>1153</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C29" s="8" t="n">
         <v>64.3</v>
       </c>
-      <c r="D29" s="8" t="n">
+      <c r="D29" s="9" t="n">
         <v>477</v>
       </c>
-      <c r="E29" s="7" t="n">
+      <c r="E29" s="8" t="n">
         <v>85.09999999999999</v>
       </c>
-      <c r="F29" s="9" t="n">
+      <c r="F29" s="10" t="n">
         <v>1612</v>
       </c>
-      <c r="G29" s="7" t="n">
+      <c r="G29" s="8" t="n">
         <v>56.7</v>
       </c>
-      <c r="H29" s="8" t="n">
+      <c r="H29" s="9" t="n">
         <v>629</v>
       </c>
-      <c r="I29" s="7" t="n">
+      <c r="I29" s="8" t="n">
         <v>82.2</v>
       </c>
-      <c r="K29" s="5" t="n">
+      <c r="K29" s="7" t="n">
         <v>83.7</v>
       </c>
     </row>
@@ -1533,7 +1541,7 @@
       <c r="A30" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="8" t="n">
+      <c r="B30" s="9" t="n">
         <v>565</v>
       </c>
       <c r="C30" s="6" t="n">
@@ -1545,19 +1553,19 @@
       <c r="E30" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F30" s="8" t="n">
+      <c r="F30" s="9" t="n">
         <v>845</v>
       </c>
       <c r="G30" s="6" t="n">
         <v>77.59999999999999</v>
       </c>
-      <c r="H30" s="8" t="n">
+      <c r="H30" s="9" t="n">
         <v>419</v>
       </c>
       <c r="I30" s="6" t="n">
         <v>86.5</v>
       </c>
-      <c r="K30" s="5" t="n">
+      <c r="K30" s="7" t="n">
         <v>82</v>
       </c>
     </row>
@@ -1565,31 +1573,31 @@
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="9" t="n">
+      <c r="B31" s="10" t="n">
         <v>1117</v>
       </c>
-      <c r="C31" s="7" t="n">
+      <c r="C31" s="8" t="n">
         <v>65.09999999999999</v>
       </c>
-      <c r="D31" s="8" t="n">
+      <c r="D31" s="9" t="n">
         <v>459</v>
       </c>
-      <c r="E31" s="7" t="n">
+      <c r="E31" s="8" t="n">
         <v>85.5</v>
       </c>
-      <c r="F31" s="8" t="n">
+      <c r="F31" s="9" t="n">
         <v>846</v>
       </c>
-      <c r="G31" s="7" t="n">
+      <c r="G31" s="8" t="n">
         <v>77.5</v>
       </c>
-      <c r="H31" s="9" t="n">
+      <c r="H31" s="10" t="n">
         <v>828</v>
       </c>
-      <c r="I31" s="7" t="n">
+      <c r="I31" s="8" t="n">
         <v>73.09999999999999</v>
       </c>
-      <c r="K31" s="5" t="n">
+      <c r="K31" s="7" t="n">
         <v>81.5</v>
       </c>
     </row>
@@ -1597,7 +1605,7 @@
       <c r="A32" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="9" t="n">
+      <c r="B32" s="10" t="n">
         <v>760</v>
       </c>
       <c r="C32" s="6" t="n">
@@ -1615,13 +1623,13 @@
       <c r="G32" s="6" t="n">
         <v>95.40000000000001</v>
       </c>
-      <c r="H32" s="9" t="n">
+      <c r="H32" s="10" t="n">
         <v>1114</v>
       </c>
       <c r="I32" s="6" t="n">
         <v>67.3</v>
       </c>
-      <c r="K32" s="5" t="n">
+      <c r="K32" s="7" t="n">
         <v>81.3</v>
       </c>
     </row>
@@ -1629,31 +1637,31 @@
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33" s="10" t="n">
+      <c r="B33" s="11" t="n">
         <v>1421</v>
       </c>
-      <c r="C33" s="7" t="n">
+      <c r="C33" s="8" t="n">
         <v>53.3</v>
       </c>
-      <c r="D33" s="8" t="n">
+      <c r="D33" s="9" t="n">
         <v>410</v>
       </c>
-      <c r="E33" s="7" t="n">
+      <c r="E33" s="8" t="n">
         <v>86.5</v>
       </c>
-      <c r="F33" s="8" t="n">
+      <c r="F33" s="9" t="n">
         <v>935</v>
       </c>
-      <c r="G33" s="7" t="n">
+      <c r="G33" s="8" t="n">
         <v>75.7</v>
       </c>
-      <c r="H33" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I33" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K33" s="5" t="n">
+      <c r="H33" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I33" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K33" s="7" t="n">
         <v>81.09999999999999</v>
       </c>
     </row>
@@ -1667,13 +1675,13 @@
       <c r="C34" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D34" s="8" t="n">
+      <c r="D34" s="9" t="n">
         <v>484</v>
       </c>
       <c r="E34" s="6" t="n">
         <v>84.90000000000001</v>
       </c>
-      <c r="F34" s="8" t="n">
+      <c r="F34" s="9" t="n">
         <v>872</v>
       </c>
       <c r="G34" s="6" t="n">
@@ -1685,7 +1693,7 @@
       <c r="I34" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="K34" s="5" t="n">
+      <c r="K34" s="7" t="n">
         <v>81</v>
       </c>
     </row>
@@ -1693,31 +1701,31 @@
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B35" s="8" t="n">
+      <c r="B35" s="9" t="n">
         <v>567</v>
       </c>
-      <c r="C35" s="7" t="n">
+      <c r="C35" s="8" t="n">
         <v>82.40000000000001</v>
       </c>
-      <c r="D35" s="8" t="n">
+      <c r="D35" s="9" t="n">
         <v>865</v>
       </c>
-      <c r="E35" s="7" t="n">
+      <c r="E35" s="8" t="n">
         <v>77</v>
       </c>
-      <c r="F35" s="9" t="n">
+      <c r="F35" s="10" t="n">
         <v>1717</v>
       </c>
-      <c r="G35" s="7" t="n">
+      <c r="G35" s="8" t="n">
         <v>54.6</v>
       </c>
-      <c r="H35" s="8" t="n">
+      <c r="H35" s="9" t="n">
         <v>506</v>
       </c>
-      <c r="I35" s="7" t="n">
+      <c r="I35" s="8" t="n">
         <v>84.7</v>
       </c>
-      <c r="K35" s="5" t="n">
+      <c r="K35" s="7" t="n">
         <v>80.90000000000001</v>
       </c>
     </row>
@@ -1725,31 +1733,31 @@
       <c r="A36" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="10" t="n">
+      <c r="B36" s="11" t="n">
         <v>2181</v>
       </c>
       <c r="C36" s="6" t="n">
         <v>36.4</v>
       </c>
-      <c r="D36" s="8" t="n">
+      <c r="D36" s="9" t="n">
         <v>460</v>
       </c>
       <c r="E36" s="6" t="n">
         <v>85.40000000000001</v>
       </c>
-      <c r="F36" s="8" t="n">
+      <c r="F36" s="9" t="n">
         <v>967</v>
       </c>
       <c r="G36" s="6" t="n">
         <v>75</v>
       </c>
-      <c r="H36" s="9" t="n">
+      <c r="H36" s="10" t="n">
         <v>1280</v>
       </c>
       <c r="I36" s="6" t="n">
         <v>63.9</v>
       </c>
-      <c r="K36" s="5" t="n">
+      <c r="K36" s="7" t="n">
         <v>80.2</v>
       </c>
     </row>
@@ -1757,31 +1765,31 @@
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="9" t="n">
+      <c r="B37" s="10" t="n">
         <v>952</v>
       </c>
-      <c r="C37" s="7" t="n">
+      <c r="C37" s="8" t="n">
         <v>68.8</v>
       </c>
-      <c r="D37" s="8" t="n">
+      <c r="D37" s="9" t="n">
         <v>886</v>
       </c>
-      <c r="E37" s="7" t="n">
+      <c r="E37" s="8" t="n">
         <v>76.59999999999999</v>
       </c>
-      <c r="F37" s="9" t="n">
+      <c r="F37" s="10" t="n">
         <v>1971</v>
       </c>
-      <c r="G37" s="7" t="n">
+      <c r="G37" s="8" t="n">
         <v>49.3</v>
       </c>
-      <c r="H37" s="8" t="n">
+      <c r="H37" s="9" t="n">
         <v>625</v>
       </c>
-      <c r="I37" s="7" t="n">
+      <c r="I37" s="8" t="n">
         <v>82.3</v>
       </c>
-      <c r="K37" s="5" t="n">
+      <c r="K37" s="7" t="n">
         <v>79.40000000000001</v>
       </c>
     </row>
@@ -1789,31 +1797,31 @@
       <c r="A38" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B38" s="9" t="n">
+      <c r="B38" s="10" t="n">
         <v>1242</v>
       </c>
       <c r="C38" s="6" t="n">
         <v>62.3</v>
       </c>
-      <c r="D38" s="8" t="n">
+      <c r="D38" s="9" t="n">
         <v>903</v>
       </c>
       <c r="E38" s="6" t="n">
         <v>76.2</v>
       </c>
-      <c r="F38" s="9" t="n">
+      <c r="F38" s="10" t="n">
         <v>1582</v>
       </c>
       <c r="G38" s="6" t="n">
         <v>57.3</v>
       </c>
-      <c r="H38" s="8" t="n">
+      <c r="H38" s="9" t="n">
         <v>621</v>
       </c>
       <c r="I38" s="6" t="n">
         <v>82.3</v>
       </c>
-      <c r="K38" s="5" t="n">
+      <c r="K38" s="7" t="n">
         <v>79.2</v>
       </c>
     </row>
@@ -1821,31 +1829,31 @@
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B39" s="10" t="n">
+      <c r="B39" s="11" t="n">
         <v>1799</v>
       </c>
-      <c r="C39" s="7" t="n">
+      <c r="C39" s="8" t="n">
         <v>44.9</v>
       </c>
-      <c r="D39" s="8" t="n">
+      <c r="D39" s="9" t="n">
         <v>555</v>
       </c>
-      <c r="E39" s="7" t="n">
+      <c r="E39" s="8" t="n">
         <v>83.5</v>
       </c>
-      <c r="F39" s="9" t="n">
+      <c r="F39" s="10" t="n">
         <v>1622</v>
       </c>
-      <c r="G39" s="7" t="n">
+      <c r="G39" s="8" t="n">
         <v>56.5</v>
       </c>
-      <c r="H39" s="9" t="n">
+      <c r="H39" s="10" t="n">
         <v>769</v>
       </c>
-      <c r="I39" s="7" t="n">
+      <c r="I39" s="8" t="n">
         <v>74.3</v>
       </c>
-      <c r="K39" s="5" t="n">
+      <c r="K39" s="7" t="n">
         <v>78.90000000000001</v>
       </c>
     </row>
@@ -1853,7 +1861,7 @@
       <c r="A40" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="9" t="n">
+      <c r="B40" s="10" t="n">
         <v>1332</v>
       </c>
       <c r="C40" s="6" t="n">
@@ -1865,19 +1873,19 @@
       <c r="E40" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F40" s="8" t="n">
+      <c r="F40" s="9" t="n">
         <v>948</v>
       </c>
       <c r="G40" s="6" t="n">
         <v>75.40000000000001</v>
       </c>
-      <c r="H40" s="8" t="n">
+      <c r="H40" s="9" t="n">
         <v>617</v>
       </c>
       <c r="I40" s="6" t="n">
         <v>82.40000000000001</v>
       </c>
-      <c r="K40" s="5" t="n">
+      <c r="K40" s="7" t="n">
         <v>78.90000000000001</v>
       </c>
     </row>
@@ -1885,31 +1893,31 @@
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B41" s="9" t="n">
+      <c r="B41" s="10" t="n">
         <v>1272</v>
       </c>
-      <c r="C41" s="7" t="n">
+      <c r="C41" s="8" t="n">
         <v>61.6</v>
       </c>
-      <c r="D41" s="8" t="n">
+      <c r="D41" s="9" t="n">
         <v>451</v>
       </c>
-      <c r="E41" s="7" t="n">
+      <c r="E41" s="8" t="n">
         <v>85.59999999999999</v>
       </c>
-      <c r="F41" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G41" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H41" s="9" t="n">
+      <c r="F41" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G41" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H41" s="10" t="n">
         <v>897</v>
       </c>
-      <c r="I41" s="7" t="n">
+      <c r="I41" s="8" t="n">
         <v>71.7</v>
       </c>
-      <c r="K41" s="5" t="n">
+      <c r="K41" s="7" t="n">
         <v>78.7</v>
       </c>
     </row>
@@ -1917,31 +1925,31 @@
       <c r="A42" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B42" s="9" t="n">
+      <c r="B42" s="10" t="n">
         <v>730</v>
       </c>
       <c r="C42" s="6" t="n">
         <v>73.7</v>
       </c>
-      <c r="D42" s="8" t="n">
+      <c r="D42" s="9" t="n">
         <v>1024</v>
       </c>
       <c r="E42" s="6" t="n">
         <v>73.7</v>
       </c>
-      <c r="F42" s="8" t="n">
+      <c r="F42" s="9" t="n">
         <v>557</v>
       </c>
       <c r="G42" s="6" t="n">
         <v>83.5</v>
       </c>
-      <c r="H42" s="9" t="n">
+      <c r="H42" s="10" t="n">
         <v>1092</v>
       </c>
       <c r="I42" s="6" t="n">
         <v>67.7</v>
       </c>
-      <c r="K42" s="5" t="n">
+      <c r="K42" s="7" t="n">
         <v>78.59999999999999</v>
       </c>
     </row>
@@ -1949,31 +1957,31 @@
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B43" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C43" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" s="9" t="n">
+      <c r="B43" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C43" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" s="10" t="n">
         <v>1144</v>
       </c>
-      <c r="E43" s="7" t="n">
+      <c r="E43" s="8" t="n">
         <v>66.2</v>
       </c>
-      <c r="F43" s="8" t="n">
+      <c r="F43" s="9" t="n">
         <v>598</v>
       </c>
-      <c r="G43" s="7" t="n">
+      <c r="G43" s="8" t="n">
         <v>82.7</v>
       </c>
-      <c r="H43" s="9" t="n">
+      <c r="H43" s="10" t="n">
         <v>798</v>
       </c>
-      <c r="I43" s="7" t="n">
+      <c r="I43" s="8" t="n">
         <v>73.7</v>
       </c>
-      <c r="K43" s="5" t="n">
+      <c r="K43" s="7" t="n">
         <v>78.2</v>
       </c>
     </row>
@@ -1981,31 +1989,31 @@
       <c r="A44" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="9" t="n">
+      <c r="B44" s="10" t="n">
         <v>1210</v>
       </c>
       <c r="C44" s="6" t="n">
         <v>63</v>
       </c>
-      <c r="D44" s="8" t="n">
+      <c r="D44" s="9" t="n">
         <v>648</v>
       </c>
       <c r="E44" s="6" t="n">
         <v>81.5</v>
       </c>
-      <c r="F44" s="8" t="n">
+      <c r="F44" s="9" t="n">
         <v>985</v>
       </c>
       <c r="G44" s="6" t="n">
         <v>74.7</v>
       </c>
-      <c r="H44" s="10" t="n">
+      <c r="H44" s="11" t="n">
         <v>1860</v>
       </c>
       <c r="I44" s="6" t="n">
         <v>47.1</v>
       </c>
-      <c r="K44" s="5" t="n">
+      <c r="K44" s="7" t="n">
         <v>78.09999999999999</v>
       </c>
     </row>
@@ -2013,31 +2021,31 @@
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B45" s="9" t="n">
+      <c r="B45" s="10" t="n">
         <v>1136</v>
       </c>
-      <c r="C45" s="7" t="n">
+      <c r="C45" s="8" t="n">
         <v>64.7</v>
       </c>
-      <c r="D45" s="9" t="n">
+      <c r="D45" s="10" t="n">
         <v>1238</v>
       </c>
-      <c r="E45" s="7" t="n">
+      <c r="E45" s="8" t="n">
         <v>64.3</v>
       </c>
-      <c r="F45" s="9" t="n">
+      <c r="F45" s="10" t="n">
         <v>1178</v>
       </c>
-      <c r="G45" s="7" t="n">
+      <c r="G45" s="8" t="n">
         <v>65.7</v>
       </c>
-      <c r="H45" s="8" t="n">
+      <c r="H45" s="9" t="n">
         <v>268</v>
       </c>
-      <c r="I45" s="7" t="n">
+      <c r="I45" s="8" t="n">
         <v>89.5</v>
       </c>
-      <c r="K45" s="5" t="n">
+      <c r="K45" s="7" t="n">
         <v>77.59999999999999</v>
       </c>
     </row>
@@ -2045,31 +2053,31 @@
       <c r="A46" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B46" s="9" t="n">
+      <c r="B46" s="10" t="n">
         <v>901</v>
       </c>
       <c r="C46" s="6" t="n">
         <v>69.90000000000001</v>
       </c>
-      <c r="D46" s="8" t="n">
+      <c r="D46" s="9" t="n">
         <v>350</v>
       </c>
       <c r="E46" s="6" t="n">
         <v>87.7</v>
       </c>
-      <c r="F46" s="9" t="n">
+      <c r="F46" s="10" t="n">
         <v>1127</v>
       </c>
       <c r="G46" s="6" t="n">
         <v>66.7</v>
       </c>
-      <c r="H46" s="10" t="n">
+      <c r="H46" s="11" t="n">
         <v>1573</v>
       </c>
       <c r="I46" s="6" t="n">
         <v>52.9</v>
       </c>
-      <c r="K46" s="5" t="n">
+      <c r="K46" s="7" t="n">
         <v>77.2</v>
       </c>
     </row>
@@ -2077,31 +2085,31 @@
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B47" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C47" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" s="8" t="n">
+      <c r="B47" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C47" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" s="9" t="n">
         <v>958</v>
       </c>
-      <c r="E47" s="7" t="n">
+      <c r="E47" s="8" t="n">
         <v>75.09999999999999</v>
       </c>
-      <c r="F47" s="8" t="n">
+      <c r="F47" s="9" t="n">
         <v>817</v>
       </c>
-      <c r="G47" s="7" t="n">
+      <c r="G47" s="8" t="n">
         <v>78.09999999999999</v>
       </c>
-      <c r="H47" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I47" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K47" s="5" t="n">
+      <c r="H47" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I47" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K47" s="7" t="n">
         <v>76.59999999999999</v>
       </c>
     </row>
@@ -2109,31 +2117,31 @@
       <c r="A48" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B48" s="10" t="n">
+      <c r="B48" s="11" t="n">
         <v>1855</v>
       </c>
       <c r="C48" s="6" t="n">
         <v>43.6</v>
       </c>
-      <c r="D48" s="8" t="n">
+      <c r="D48" s="9" t="n">
         <v>892</v>
       </c>
       <c r="E48" s="6" t="n">
         <v>76.5</v>
       </c>
-      <c r="F48" s="9" t="n">
+      <c r="F48" s="10" t="n">
         <v>1429</v>
       </c>
       <c r="G48" s="6" t="n">
         <v>60.5</v>
       </c>
-      <c r="H48" s="9" t="n">
+      <c r="H48" s="10" t="n">
         <v>811</v>
       </c>
       <c r="I48" s="6" t="n">
         <v>73.5</v>
       </c>
-      <c r="K48" s="5" t="n">
+      <c r="K48" s="7" t="n">
         <v>75</v>
       </c>
     </row>
@@ -2141,31 +2149,31 @@
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B49" s="9" t="n">
+      <c r="B49" s="10" t="n">
         <v>1133</v>
       </c>
-      <c r="C49" s="7" t="n">
+      <c r="C49" s="8" t="n">
         <v>64.7</v>
       </c>
-      <c r="D49" s="8" t="n">
+      <c r="D49" s="9" t="n">
         <v>975</v>
       </c>
-      <c r="E49" s="7" t="n">
+      <c r="E49" s="8" t="n">
         <v>74.7</v>
       </c>
-      <c r="F49" s="8" t="n">
+      <c r="F49" s="9" t="n">
         <v>959</v>
       </c>
-      <c r="G49" s="7" t="n">
+      <c r="G49" s="8" t="n">
         <v>75.2</v>
       </c>
-      <c r="H49" s="10" t="n">
+      <c r="H49" s="11" t="n">
         <v>1754</v>
       </c>
-      <c r="I49" s="7" t="n">
+      <c r="I49" s="8" t="n">
         <v>49.2</v>
       </c>
-      <c r="K49" s="5" t="n">
+      <c r="K49" s="7" t="n">
         <v>75</v>
       </c>
     </row>
@@ -2173,31 +2181,31 @@
       <c r="A50" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B50" s="9" t="n">
+      <c r="B50" s="10" t="n">
         <v>1025</v>
       </c>
       <c r="C50" s="6" t="n">
         <v>67.09999999999999</v>
       </c>
-      <c r="D50" s="10" t="n">
+      <c r="D50" s="11" t="n">
         <v>2546</v>
       </c>
       <c r="E50" s="6" t="n">
         <v>32.1</v>
       </c>
-      <c r="F50" s="9" t="n">
+      <c r="F50" s="10" t="n">
         <v>1136</v>
       </c>
       <c r="G50" s="6" t="n">
         <v>66.59999999999999</v>
       </c>
-      <c r="H50" s="8" t="n">
+      <c r="H50" s="9" t="n">
         <v>579</v>
       </c>
       <c r="I50" s="6" t="n">
         <v>83.2</v>
       </c>
-      <c r="K50" s="5" t="n">
+      <c r="K50" s="7" t="n">
         <v>74.90000000000001</v>
       </c>
     </row>
@@ -2205,31 +2213,31 @@
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C51" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" s="8" t="n">
+      <c r="B51" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C51" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" s="9" t="n">
         <v>1043</v>
       </c>
-      <c r="E51" s="7" t="n">
+      <c r="E51" s="8" t="n">
         <v>73.3</v>
       </c>
-      <c r="F51" s="9" t="n">
+      <c r="F51" s="10" t="n">
         <v>2069</v>
       </c>
-      <c r="G51" s="7" t="n">
+      <c r="G51" s="8" t="n">
         <v>47.3</v>
       </c>
-      <c r="H51" s="9" t="n">
+      <c r="H51" s="10" t="n">
         <v>790</v>
       </c>
-      <c r="I51" s="7" t="n">
+      <c r="I51" s="8" t="n">
         <v>73.90000000000001</v>
       </c>
-      <c r="K51" s="5" t="n">
+      <c r="K51" s="7" t="n">
         <v>73.59999999999999</v>
       </c>
     </row>
@@ -2237,31 +2245,31 @@
       <c r="A52" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B52" s="10" t="n">
+      <c r="B52" s="11" t="n">
         <v>2018</v>
       </c>
       <c r="C52" s="6" t="n">
         <v>40</v>
       </c>
-      <c r="D52" s="8" t="n">
+      <c r="D52" s="9" t="n">
         <v>510</v>
       </c>
       <c r="E52" s="6" t="n">
         <v>84.40000000000001</v>
       </c>
-      <c r="F52" s="9" t="n">
+      <c r="F52" s="10" t="n">
         <v>1414</v>
       </c>
       <c r="G52" s="6" t="n">
         <v>60.8</v>
       </c>
-      <c r="H52" s="10" t="n">
+      <c r="H52" s="11" t="n">
         <v>1900</v>
       </c>
       <c r="I52" s="6" t="n">
         <v>46.3</v>
       </c>
-      <c r="K52" s="5" t="n">
+      <c r="K52" s="7" t="n">
         <v>72.59999999999999</v>
       </c>
     </row>
@@ -2269,31 +2277,31 @@
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="9" t="n">
+      <c r="B53" s="10" t="n">
         <v>870</v>
       </c>
-      <c r="C53" s="7" t="n">
+      <c r="C53" s="8" t="n">
         <v>70.59999999999999</v>
       </c>
-      <c r="D53" s="8" t="n">
+      <c r="D53" s="9" t="n">
         <v>385</v>
       </c>
-      <c r="E53" s="7" t="n">
+      <c r="E53" s="8" t="n">
         <v>87</v>
       </c>
-      <c r="F53" s="9" t="n">
+      <c r="F53" s="10" t="n">
         <v>1727</v>
       </c>
-      <c r="G53" s="7" t="n">
+      <c r="G53" s="8" t="n">
         <v>54.4</v>
       </c>
-      <c r="H53" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I53" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K53" s="5" t="n">
+      <c r="H53" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I53" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K53" s="7" t="n">
         <v>70.7</v>
       </c>
     </row>
@@ -2301,13 +2309,13 @@
       <c r="A54" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B54" s="9" t="n">
+      <c r="B54" s="10" t="n">
         <v>858</v>
       </c>
       <c r="C54" s="6" t="n">
         <v>70.90000000000001</v>
       </c>
-      <c r="D54" s="8" t="n">
+      <c r="D54" s="9" t="n">
         <v>458</v>
       </c>
       <c r="E54" s="6" t="n">
@@ -2319,13 +2327,13 @@
       <c r="G54" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H54" s="10" t="n">
+      <c r="H54" s="11" t="n">
         <v>1463</v>
       </c>
       <c r="I54" s="6" t="n">
         <v>55.2</v>
       </c>
-      <c r="K54" s="5" t="n">
+      <c r="K54" s="7" t="n">
         <v>70.3</v>
       </c>
     </row>
@@ -2333,31 +2341,31 @@
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B55" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C55" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D55" s="9" t="n">
+      <c r="B55" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C55" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" s="10" t="n">
         <v>1223</v>
       </c>
-      <c r="E55" s="7" t="n">
+      <c r="E55" s="8" t="n">
         <v>64.59999999999999</v>
       </c>
-      <c r="F55" s="9" t="n">
+      <c r="F55" s="10" t="n">
         <v>1340</v>
       </c>
-      <c r="G55" s="7" t="n">
+      <c r="G55" s="8" t="n">
         <v>62.3</v>
       </c>
-      <c r="H55" s="9" t="n">
+      <c r="H55" s="10" t="n">
         <v>740</v>
       </c>
-      <c r="I55" s="7" t="n">
+      <c r="I55" s="8" t="n">
         <v>74.90000000000001</v>
       </c>
-      <c r="K55" s="5" t="n">
+      <c r="K55" s="7" t="n">
         <v>69.8</v>
       </c>
     </row>
@@ -2365,31 +2373,31 @@
       <c r="A56" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B56" s="9" t="n">
+      <c r="B56" s="10" t="n">
         <v>736</v>
       </c>
       <c r="C56" s="6" t="n">
         <v>73.59999999999999</v>
       </c>
-      <c r="D56" s="9" t="n">
+      <c r="D56" s="10" t="n">
         <v>1283</v>
       </c>
       <c r="E56" s="6" t="n">
         <v>63.3</v>
       </c>
-      <c r="F56" s="10" t="n">
+      <c r="F56" s="11" t="n">
         <v>2615</v>
       </c>
       <c r="G56" s="6" t="n">
         <v>31</v>
       </c>
-      <c r="H56" s="9" t="n">
+      <c r="H56" s="10" t="n">
         <v>792</v>
       </c>
       <c r="I56" s="6" t="n">
         <v>73.90000000000001</v>
       </c>
-      <c r="K56" s="5" t="n">
+      <c r="K56" s="7" t="n">
         <v>68.59999999999999</v>
       </c>
     </row>
@@ -2397,31 +2405,31 @@
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="9" t="n">
+      <c r="B57" s="10" t="n">
         <v>1109</v>
       </c>
-      <c r="C57" s="7" t="n">
+      <c r="C57" s="8" t="n">
         <v>65.3</v>
       </c>
-      <c r="D57" s="9" t="n">
+      <c r="D57" s="10" t="n">
         <v>1181</v>
       </c>
-      <c r="E57" s="7" t="n">
+      <c r="E57" s="8" t="n">
         <v>65.40000000000001</v>
       </c>
-      <c r="F57" s="9" t="n">
+      <c r="F57" s="10" t="n">
         <v>1223</v>
       </c>
-      <c r="G57" s="7" t="n">
+      <c r="G57" s="8" t="n">
         <v>64.8</v>
       </c>
-      <c r="H57" s="9" t="n">
+      <c r="H57" s="10" t="n">
         <v>913</v>
       </c>
-      <c r="I57" s="7" t="n">
+      <c r="I57" s="8" t="n">
         <v>71.40000000000001</v>
       </c>
-      <c r="K57" s="5" t="n">
+      <c r="K57" s="7" t="n">
         <v>68.40000000000001</v>
       </c>
     </row>
@@ -2429,31 +2437,31 @@
       <c r="A58" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B58" s="8" t="n">
+      <c r="B58" s="9" t="n">
         <v>315</v>
       </c>
       <c r="C58" s="6" t="n">
         <v>88</v>
       </c>
-      <c r="D58" s="9" t="n">
+      <c r="D58" s="10" t="n">
         <v>2123</v>
       </c>
       <c r="E58" s="6" t="n">
         <v>45.9</v>
       </c>
-      <c r="F58" s="8" t="n">
+      <c r="F58" s="9" t="n">
         <v>757</v>
       </c>
       <c r="G58" s="6" t="n">
         <v>79.40000000000001</v>
       </c>
-      <c r="H58" s="10" t="n">
+      <c r="H58" s="11" t="n">
         <v>1642</v>
       </c>
       <c r="I58" s="6" t="n">
         <v>51.5</v>
       </c>
-      <c r="K58" s="5" t="n">
+      <c r="K58" s="7" t="n">
         <v>65.5</v>
       </c>
     </row>
@@ -2461,31 +2469,31 @@
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B59" s="10" t="n">
+      <c r="B59" s="11" t="n">
         <v>2048</v>
       </c>
-      <c r="C59" s="7" t="n">
+      <c r="C59" s="8" t="n">
         <v>39.3</v>
       </c>
-      <c r="D59" s="9" t="n">
+      <c r="D59" s="10" t="n">
         <v>1234</v>
       </c>
-      <c r="E59" s="7" t="n">
+      <c r="E59" s="8" t="n">
         <v>64.3</v>
       </c>
-      <c r="F59" s="9" t="n">
+      <c r="F59" s="10" t="n">
         <v>1181</v>
       </c>
-      <c r="G59" s="7" t="n">
+      <c r="G59" s="8" t="n">
         <v>65.59999999999999</v>
       </c>
-      <c r="H59" s="9" t="n">
+      <c r="H59" s="10" t="n">
         <v>1297</v>
       </c>
-      <c r="I59" s="7" t="n">
+      <c r="I59" s="8" t="n">
         <v>63.6</v>
       </c>
-      <c r="K59" s="5" t="n">
+      <c r="K59" s="7" t="n">
         <v>65</v>
       </c>
     </row>
@@ -2493,13 +2501,13 @@
       <c r="A60" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B60" s="10" t="n">
+      <c r="B60" s="11" t="n">
         <v>2157</v>
       </c>
       <c r="C60" s="6" t="n">
         <v>36.9</v>
       </c>
-      <c r="D60" s="9" t="n">
+      <c r="D60" s="10" t="n">
         <v>1642</v>
       </c>
       <c r="E60" s="6" t="n">
@@ -2511,13 +2519,13 @@
       <c r="G60" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="H60" s="9" t="n">
+      <c r="H60" s="10" t="n">
         <v>789</v>
       </c>
       <c r="I60" s="6" t="n">
         <v>73.90000000000001</v>
       </c>
-      <c r="K60" s="5" t="n">
+      <c r="K60" s="7" t="n">
         <v>64.90000000000001</v>
       </c>
     </row>
@@ -2525,31 +2533,31 @@
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B61" s="9" t="n">
+      <c r="B61" s="10" t="n">
         <v>1215</v>
       </c>
-      <c r="C61" s="7" t="n">
+      <c r="C61" s="8" t="n">
         <v>62.9</v>
       </c>
-      <c r="D61" s="9" t="n">
+      <c r="D61" s="10" t="n">
         <v>1648</v>
       </c>
-      <c r="E61" s="7" t="n">
+      <c r="E61" s="8" t="n">
         <v>55.7</v>
       </c>
-      <c r="F61" s="9" t="n">
+      <c r="F61" s="10" t="n">
         <v>1754</v>
       </c>
-      <c r="G61" s="7" t="n">
+      <c r="G61" s="8" t="n">
         <v>53.8</v>
       </c>
-      <c r="H61" s="9" t="n">
+      <c r="H61" s="10" t="n">
         <v>883</v>
       </c>
-      <c r="I61" s="7" t="n">
+      <c r="I61" s="8" t="n">
         <v>72</v>
       </c>
-      <c r="K61" s="5" t="n">
+      <c r="K61" s="7" t="n">
         <v>63.9</v>
       </c>
     </row>
@@ -2569,19 +2577,19 @@
       <c r="E62" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F62" s="8" t="n">
+      <c r="F62" s="9" t="n">
         <v>608</v>
       </c>
       <c r="G62" s="6" t="n">
         <v>82.5</v>
       </c>
-      <c r="H62" s="10" t="n">
+      <c r="H62" s="11" t="n">
         <v>1959</v>
       </c>
       <c r="I62" s="6" t="n">
         <v>45.1</v>
       </c>
-      <c r="K62" s="5" t="n">
+      <c r="K62" s="7" t="n">
         <v>63.8</v>
       </c>
     </row>
@@ -2589,31 +2597,31 @@
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B63" s="9" t="n">
+      <c r="B63" s="10" t="n">
         <v>867</v>
       </c>
-      <c r="C63" s="7" t="n">
+      <c r="C63" s="8" t="n">
         <v>70.7</v>
       </c>
-      <c r="D63" s="9" t="n">
+      <c r="D63" s="10" t="n">
         <v>1421</v>
       </c>
-      <c r="E63" s="7" t="n">
+      <c r="E63" s="8" t="n">
         <v>60.4</v>
       </c>
-      <c r="F63" s="10" t="n">
+      <c r="F63" s="11" t="n">
         <v>2124</v>
       </c>
-      <c r="G63" s="7" t="n">
+      <c r="G63" s="8" t="n">
         <v>41.2</v>
       </c>
-      <c r="H63" s="9" t="n">
+      <c r="H63" s="10" t="n">
         <v>1153</v>
       </c>
-      <c r="I63" s="7" t="n">
+      <c r="I63" s="8" t="n">
         <v>66.5</v>
       </c>
-      <c r="K63" s="5" t="n">
+      <c r="K63" s="7" t="n">
         <v>63.4</v>
       </c>
     </row>
@@ -2621,19 +2629,19 @@
       <c r="A64" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B64" s="9" t="n">
+      <c r="B64" s="10" t="n">
         <v>995</v>
       </c>
       <c r="C64" s="6" t="n">
         <v>67.8</v>
       </c>
-      <c r="D64" s="8" t="n">
+      <c r="D64" s="9" t="n">
         <v>914</v>
       </c>
       <c r="E64" s="6" t="n">
         <v>76</v>
       </c>
-      <c r="F64" s="9" t="n">
+      <c r="F64" s="10" t="n">
         <v>2034</v>
       </c>
       <c r="G64" s="6" t="n">
@@ -2645,7 +2653,7 @@
       <c r="I64" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="K64" s="5" t="n">
+      <c r="K64" s="7" t="n">
         <v>62</v>
       </c>
     </row>
@@ -2653,31 +2661,31 @@
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B65" s="10" t="n">
+      <c r="B65" s="11" t="n">
         <v>1537</v>
       </c>
-      <c r="C65" s="7" t="n">
+      <c r="C65" s="8" t="n">
         <v>50.7</v>
       </c>
-      <c r="D65" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E65" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F65" s="8" t="n">
+      <c r="D65" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E65" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F65" s="9" t="n">
         <v>986</v>
       </c>
-      <c r="G65" s="7" t="n">
+      <c r="G65" s="8" t="n">
         <v>74.59999999999999</v>
       </c>
-      <c r="H65" s="10" t="n">
+      <c r="H65" s="11" t="n">
         <v>1778</v>
       </c>
-      <c r="I65" s="7" t="n">
+      <c r="I65" s="8" t="n">
         <v>48.8</v>
       </c>
-      <c r="K65" s="5" t="n">
+      <c r="K65" s="7" t="n">
         <v>61.7</v>
       </c>
     </row>
@@ -2685,31 +2693,31 @@
       <c r="A66" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B66" s="10" t="n">
+      <c r="B66" s="11" t="n">
         <v>2119</v>
       </c>
       <c r="C66" s="6" t="n">
         <v>37.7</v>
       </c>
-      <c r="D66" s="9" t="n">
+      <c r="D66" s="10" t="n">
         <v>1412</v>
       </c>
       <c r="E66" s="6" t="n">
         <v>60.6</v>
       </c>
-      <c r="F66" s="9" t="n">
+      <c r="F66" s="10" t="n">
         <v>1876</v>
       </c>
       <c r="G66" s="6" t="n">
         <v>51.3</v>
       </c>
-      <c r="H66" s="10" t="n">
+      <c r="H66" s="11" t="n">
         <v>1373</v>
       </c>
       <c r="I66" s="6" t="n">
         <v>57</v>
       </c>
-      <c r="K66" s="5" t="n">
+      <c r="K66" s="7" t="n">
         <v>58.8</v>
       </c>
     </row>
@@ -2717,31 +2725,31 @@
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B67" s="10" t="n">
+      <c r="B67" s="11" t="n">
         <v>2011</v>
       </c>
-      <c r="C67" s="7" t="n">
+      <c r="C67" s="8" t="n">
         <v>40.1</v>
       </c>
-      <c r="D67" s="9" t="n">
+      <c r="D67" s="10" t="n">
         <v>1398</v>
       </c>
-      <c r="E67" s="7" t="n">
+      <c r="E67" s="8" t="n">
         <v>60.9</v>
       </c>
-      <c r="F67" s="9" t="n">
+      <c r="F67" s="10" t="n">
         <v>2099</v>
       </c>
-      <c r="G67" s="7" t="n">
+      <c r="G67" s="8" t="n">
         <v>46.7</v>
       </c>
-      <c r="H67" s="10" t="n">
+      <c r="H67" s="11" t="n">
         <v>1665</v>
       </c>
-      <c r="I67" s="7" t="n">
+      <c r="I67" s="8" t="n">
         <v>51.1</v>
       </c>
-      <c r="K67" s="5" t="n">
+      <c r="K67" s="7" t="n">
         <v>56</v>
       </c>
     </row>
@@ -2755,13 +2763,13 @@
       <c r="C68" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D68" s="8" t="n">
+      <c r="D68" s="9" t="n">
         <v>942</v>
       </c>
       <c r="E68" s="6" t="n">
         <v>75.40000000000001</v>
       </c>
-      <c r="F68" s="10" t="n">
+      <c r="F68" s="11" t="n">
         <v>2382</v>
       </c>
       <c r="G68" s="6" t="n">
@@ -2773,7 +2781,7 @@
       <c r="I68" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="K68" s="5" t="n">
+      <c r="K68" s="7" t="n">
         <v>55.6</v>
       </c>
     </row>
@@ -2781,31 +2789,31 @@
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B69" s="10" t="n">
+      <c r="B69" s="11" t="n">
         <v>2014</v>
       </c>
-      <c r="C69" s="7" t="n">
+      <c r="C69" s="8" t="n">
         <v>40.1</v>
       </c>
-      <c r="D69" s="9" t="n">
+      <c r="D69" s="10" t="n">
         <v>2067</v>
       </c>
-      <c r="E69" s="7" t="n">
+      <c r="E69" s="8" t="n">
         <v>47</v>
       </c>
-      <c r="F69" s="9" t="n">
+      <c r="F69" s="10" t="n">
         <v>1309</v>
       </c>
-      <c r="G69" s="7" t="n">
+      <c r="G69" s="8" t="n">
         <v>63</v>
       </c>
-      <c r="H69" s="10" t="n">
+      <c r="H69" s="11" t="n">
         <v>1917</v>
       </c>
-      <c r="I69" s="7" t="n">
+      <c r="I69" s="8" t="n">
         <v>45.9</v>
       </c>
-      <c r="K69" s="5" t="n">
+      <c r="K69" s="7" t="n">
         <v>55</v>
       </c>
     </row>
@@ -2819,13 +2827,13 @@
       <c r="C70" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="D70" s="9" t="n">
+      <c r="D70" s="10" t="n">
         <v>1657</v>
       </c>
       <c r="E70" s="6" t="n">
         <v>55.5</v>
       </c>
-      <c r="F70" s="9" t="n">
+      <c r="F70" s="10" t="n">
         <v>1955</v>
       </c>
       <c r="G70" s="6" t="n">
@@ -2837,7 +2845,7 @@
       <c r="I70" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="K70" s="5" t="n">
+      <c r="K70" s="7" t="n">
         <v>52.5</v>
       </c>
     </row>
@@ -2845,31 +2853,31 @@
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B71" s="10" t="n">
+      <c r="B71" s="11" t="n">
         <v>1637</v>
       </c>
-      <c r="C71" s="7" t="n">
+      <c r="C71" s="8" t="n">
         <v>48.5</v>
       </c>
-      <c r="D71" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E71" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F71" s="10" t="n">
+      <c r="D71" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E71" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F71" s="11" t="n">
         <v>2217</v>
       </c>
-      <c r="G71" s="7" t="n">
+      <c r="G71" s="8" t="n">
         <v>39.2</v>
       </c>
-      <c r="H71" s="9" t="n">
+      <c r="H71" s="10" t="n">
         <v>1275</v>
       </c>
-      <c r="I71" s="7" t="n">
+      <c r="I71" s="8" t="n">
         <v>64</v>
       </c>
-      <c r="K71" s="5" t="n">
+      <c r="K71" s="7" t="n">
         <v>51.6</v>
       </c>
     </row>
@@ -2889,19 +2897,19 @@
       <c r="E72" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F72" s="9" t="n">
+      <c r="F72" s="10" t="n">
         <v>1761</v>
       </c>
       <c r="G72" s="6" t="n">
         <v>53.7</v>
       </c>
-      <c r="H72" s="10" t="n">
+      <c r="H72" s="11" t="n">
         <v>1838</v>
       </c>
       <c r="I72" s="6" t="n">
         <v>47.5</v>
       </c>
-      <c r="K72" s="5" t="n">
+      <c r="K72" s="7" t="n">
         <v>50.6</v>
       </c>
     </row>
@@ -2909,31 +2917,31 @@
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B73" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="C73" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D73" s="9" t="n">
+      <c r="B73" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="C73" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D73" s="10" t="n">
         <v>2027</v>
       </c>
-      <c r="E73" s="7" t="n">
+      <c r="E73" s="8" t="n">
         <v>47.8</v>
       </c>
-      <c r="F73" s="9" t="n">
+      <c r="F73" s="10" t="n">
         <v>2079</v>
       </c>
-      <c r="G73" s="7" t="n">
+      <c r="G73" s="8" t="n">
         <v>47.1</v>
       </c>
-      <c r="H73" s="10" t="n">
+      <c r="H73" s="11" t="n">
         <v>1762</v>
       </c>
-      <c r="I73" s="7" t="n">
+      <c r="I73" s="8" t="n">
         <v>49.1</v>
       </c>
-      <c r="K73" s="5" t="n">
+      <c r="K73" s="7" t="n">
         <v>48.5</v>
       </c>
     </row>
@@ -2941,7 +2949,7 @@
       <c r="A74" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B74" s="8" t="n">
+      <c r="B74" s="9" t="n">
         <v>461</v>
       </c>
       <c r="C74" s="6" t="n">
@@ -2953,7 +2961,7 @@
       <c r="E74" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="F74" s="8" t="n">
+      <c r="F74" s="9" t="n">
         <v>544</v>
       </c>
       <c r="G74" s="6" t="n">
@@ -2965,7 +2973,7 @@
       <c r="I74" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="K74" s="5" t="n">
+      <c r="K74" s="7" t="n">
         <v>41.9</v>
       </c>
     </row>
@@ -2973,31 +2981,31 @@
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B75" s="9" t="n">
+      <c r="B75" s="10" t="n">
         <v>1361</v>
       </c>
-      <c r="C75" s="7" t="n">
+      <c r="C75" s="8" t="n">
         <v>59.6</v>
       </c>
-      <c r="D75" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="E75" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F75" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="G75" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H75" s="9" t="n">
+      <c r="D75" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="E75" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F75" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="G75" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H75" s="10" t="n">
         <v>908</v>
       </c>
-      <c r="I75" s="7" t="n">
+      <c r="I75" s="8" t="n">
         <v>71.5</v>
       </c>
-      <c r="K75" s="5" t="n">
+      <c r="K75" s="7" t="n">
         <v>35.8</v>
       </c>
     </row>
@@ -3005,7 +3013,7 @@
       <c r="A76" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B76" s="8" t="n">
+      <c r="B76" s="9" t="n">
         <v>641</v>
       </c>
       <c r="C76" s="6" t="n">
@@ -3029,7 +3037,7 @@
       <c r="I76" s="6" t="n">
         <v>0</v>
       </c>
-      <c r="K76" s="5" t="n">
+      <c r="K76" s="7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3037,41 +3045,41 @@
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B77" s="7" t="n">
+      <c r="B77" s="8" t="n">
         <v>-2</v>
       </c>
-      <c r="C77" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D77" s="7" t="n">
+      <c r="C77" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="D77" s="8" t="n">
         <v>-2</v>
       </c>
-      <c r="E77" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F77" s="7" t="n">
+      <c r="E77" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F77" s="8" t="n">
         <v>-2</v>
       </c>
-      <c r="G77" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H77" s="7" t="n">
-        <v>-1</v>
-      </c>
-      <c r="I77" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K77" s="5" t="n">
+      <c r="G77" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="H77" s="8" t="n">
+        <v>-1</v>
+      </c>
+      <c r="I77" s="8" t="n">
+        <v>0</v>
+      </c>
+      <c r="K77" s="7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="11" t="s">
+      <c r="A80" s="12" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="81" spans="1:11">
-      <c r="A81" s="11" t="s">
+      <c r="A81" s="12" t="s">
         <v>77</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ansonluo renamed to Ansonluo1
</commit_message>
<xml_diff>
--- a/generateEXCEL/index.xlsx
+++ b/generateEXCEL/index.xlsx
@@ -128,7 +128,7 @@
     <t>bifeitang</t>
   </si>
   <si>
-    <t>Ansonluo</t>
+    <t>Ansonluo1</t>
   </si>
   <si>
     <t>softair</t>
@@ -1836,10 +1836,10 @@
         <v>44.9</v>
       </c>
       <c r="D39" s="9" t="n">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="E39" s="8" t="n">
-        <v>83.5</v>
+        <v>83.40000000000001</v>
       </c>
       <c r="F39" s="10" t="n">
         <v>1622</v>

</xml_diff>

<commit_message>
add missing persons in 2019
</commit_message>
<xml_diff>
--- a/generateEXCEL/index.xlsx
+++ b/generateEXCEL/index.xlsx
@@ -461,7 +461,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BJ160"/>
+  <dimension ref="A1:BJ168"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -12777,11 +12777,11 @@
       </c>
       <c r="B133" s="18" t="inlineStr">
         <is>
-          <t>banrenmasanxing</t>
+          <t>aerzitudou</t>
         </is>
       </c>
       <c r="C133" s="5" t="n">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="D133" s="19" t="inlineStr">
         <is>
@@ -12818,62 +12818,62 @@
       <c r="N133" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="O133" s="23" t="n">
-        <v>1852</v>
+      <c r="O133" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="P133" s="20" t="n">
-        <v>58.6</v>
-      </c>
-      <c r="Q133" s="24" t="n">
-        <v>2042</v>
+        <v>0</v>
+      </c>
+      <c r="Q133" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="R133" s="20" t="n">
-        <v>54.2</v>
-      </c>
-      <c r="S133" s="24" t="n">
-        <v>2579</v>
+        <v>0</v>
+      </c>
+      <c r="S133" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="T133" s="20" t="n">
-        <v>41.9</v>
-      </c>
-      <c r="U133" s="25" t="n">
-        <v>2502</v>
+        <v>0</v>
+      </c>
+      <c r="U133" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="V133" s="20" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
       <c r="W133" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="X133" s="20" t="n">
         <v>0</v>
       </c>
       <c r="Y133" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="Z133" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AA133" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AB133" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AC133" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AD133" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AE133" s="20" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AF133" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AG133" s="20" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AH133" s="20" t="n">
         <v>0</v>
@@ -12887,11 +12887,11 @@
       </c>
       <c r="B134" s="1" t="inlineStr">
         <is>
-          <t>bellumpara</t>
+          <t>banrenmasanxing</t>
         </is>
       </c>
       <c r="C134" s="11" t="n">
-        <v>166</v>
+        <v>26</v>
       </c>
       <c r="D134" s="19" t="inlineStr">
         <is>
@@ -12928,65 +12928,65 @@
       <c r="N134" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="O134" s="22" t="n">
-        <v>-3</v>
+      <c r="O134" s="23" t="n">
+        <v>1852</v>
       </c>
       <c r="P134" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q134" s="22" t="n">
-        <v>-3</v>
+        <v>58.6</v>
+      </c>
+      <c r="Q134" s="24" t="n">
+        <v>2042</v>
       </c>
       <c r="R134" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="S134" s="22" t="n">
-        <v>-3</v>
+        <v>54.2</v>
+      </c>
+      <c r="S134" s="24" t="n">
+        <v>2579</v>
       </c>
       <c r="T134" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="U134" s="22" t="n">
-        <v>-3</v>
+        <v>41.9</v>
+      </c>
+      <c r="U134" s="25" t="n">
+        <v>2502</v>
       </c>
       <c r="V134" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="W134" s="23" t="n">
-        <v>379</v>
+        <v>37</v>
+      </c>
+      <c r="W134" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="X134" s="22" t="n">
-        <v>86.3</v>
+        <v>0</v>
       </c>
       <c r="Y134" s="22" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="Z134" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="AA134" s="24" t="n">
-        <v>913</v>
+      <c r="AA134" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AB134" s="22" t="n">
-        <v>71.40000000000001</v>
-      </c>
-      <c r="AC134" s="24" t="n">
-        <v>1223</v>
+        <v>0</v>
+      </c>
+      <c r="AC134" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AD134" s="22" t="n">
-        <v>64.8</v>
-      </c>
-      <c r="AE134" s="24" t="n">
-        <v>1181</v>
+        <v>0</v>
+      </c>
+      <c r="AE134" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AF134" s="22" t="n">
-        <v>65.40000000000001</v>
-      </c>
-      <c r="AG134" s="24" t="n">
-        <v>1109</v>
+        <v>0</v>
+      </c>
+      <c r="AG134" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AH134" s="22" t="n">
-        <v>65.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -12997,11 +12997,11 @@
       </c>
       <c r="B135" s="18" t="inlineStr">
         <is>
-          <t>cookiecookie</t>
+          <t>bellumpara</t>
         </is>
       </c>
       <c r="C135" s="5" t="n">
-        <v>15</v>
+        <v>166</v>
       </c>
       <c r="D135" s="19" t="inlineStr">
         <is>
@@ -13032,71 +13032,71 @@
       <c r="L135" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="M135" s="24" t="n">
-        <v>2236</v>
+      <c r="M135" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="N135" s="20" t="n">
-        <v>55.4</v>
-      </c>
-      <c r="O135" s="25" t="n">
-        <v>3055</v>
+        <v>0</v>
+      </c>
+      <c r="O135" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="P135" s="20" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="Q135" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="R135" s="20" t="n">
         <v>0</v>
       </c>
       <c r="S135" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="T135" s="20" t="n">
         <v>0</v>
       </c>
       <c r="U135" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="V135" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="W135" s="20" t="n">
-        <v>-2</v>
+      <c r="W135" s="23" t="n">
+        <v>379</v>
       </c>
       <c r="X135" s="20" t="n">
-        <v>0</v>
+        <v>86.3</v>
       </c>
       <c r="Y135" s="20" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="Z135" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AA135" s="20" t="n">
-        <v>-2</v>
+      <c r="AA135" s="24" t="n">
+        <v>913</v>
       </c>
       <c r="AB135" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC135" s="20" t="n">
-        <v>-2</v>
+        <v>71.40000000000001</v>
+      </c>
+      <c r="AC135" s="24" t="n">
+        <v>1223</v>
       </c>
       <c r="AD135" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE135" s="20" t="n">
-        <v>-2</v>
+        <v>64.8</v>
+      </c>
+      <c r="AE135" s="24" t="n">
+        <v>1181</v>
       </c>
       <c r="AF135" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG135" s="20" t="n">
-        <v>-2</v>
+        <v>65.40000000000001</v>
+      </c>
+      <c r="AG135" s="24" t="n">
+        <v>1109</v>
       </c>
       <c r="AH135" s="20" t="n">
-        <v>0</v>
+        <v>65.3</v>
       </c>
     </row>
     <row r="136">
@@ -13107,11 +13107,11 @@
       </c>
       <c r="B136" s="1" t="inlineStr">
         <is>
-          <t>crossbowman</t>
+          <t>cookiecookie</t>
         </is>
       </c>
       <c r="C136" s="11" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D136" s="19" t="inlineStr">
         <is>
@@ -13142,20 +13142,20 @@
       <c r="L136" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="M136" s="22" t="n">
-        <v>-3</v>
+      <c r="M136" s="24" t="n">
+        <v>2236</v>
       </c>
       <c r="N136" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="O136" s="22" t="n">
-        <v>-1</v>
+        <v>55.4</v>
+      </c>
+      <c r="O136" s="25" t="n">
+        <v>3055</v>
       </c>
       <c r="P136" s="22" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="Q136" s="22" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="R136" s="22" t="n">
         <v>0</v>
@@ -13217,11 +13217,11 @@
       </c>
       <c r="B137" s="18" t="inlineStr">
         <is>
-          <t>deerstalker</t>
+          <t>crossbowman</t>
         </is>
       </c>
       <c r="C137" s="5" t="n">
-        <v>177</v>
+        <v>17</v>
       </c>
       <c r="D137" s="19" t="inlineStr">
         <is>
@@ -13259,69 +13259,64 @@
         <v>0</v>
       </c>
       <c r="O137" s="20" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="P137" s="20" t="n">
         <v>0</v>
       </c>
       <c r="Q137" s="20" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="R137" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="S137" s="23" t="n">
-        <v>1675</v>
+      <c r="S137" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="T137" s="20" t="n">
-        <v>63.8</v>
-      </c>
-      <c r="U137" s="24" t="n">
-        <v>1870</v>
+        <v>0</v>
+      </c>
+      <c r="U137" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="V137" s="20" t="n">
-        <v>54.2</v>
-      </c>
-      <c r="W137" s="25" t="n">
-        <v>1958</v>
+        <v>0</v>
+      </c>
+      <c r="W137" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="X137" s="20" t="n">
-        <v>39.8</v>
-      </c>
-      <c r="Y137" s="24" t="n">
-        <v>1832</v>
+        <v>0</v>
+      </c>
+      <c r="Y137" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="Z137" s="20" t="n">
-        <v>47.9</v>
-      </c>
-      <c r="AA137" s="24" t="n">
-        <v>908</v>
+        <v>0</v>
+      </c>
+      <c r="AA137" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="AB137" s="20" t="n">
-        <v>71.5</v>
+        <v>0</v>
       </c>
       <c r="AC137" s="20" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AD137" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AE137" s="20" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AF137" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AG137" s="24" t="n">
-        <v>1361</v>
+      <c r="AG137" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="AH137" s="20" t="n">
-        <v>59.6</v>
-      </c>
-      <c r="AI137" s="9" t="inlineStr">
-        <is>
-          <t>Google-Logo</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="138">
@@ -13332,11 +13327,11 @@
       </c>
       <c r="B138" s="1" t="inlineStr">
         <is>
-          <t>dhf13</t>
+          <t>deerstalker</t>
         </is>
       </c>
       <c r="C138" s="11" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D138" s="19" t="inlineStr">
         <is>
@@ -13385,35 +13380,35 @@
       <c r="R138" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="S138" s="22" t="n">
-        <v>-1</v>
+      <c r="S138" s="23" t="n">
+        <v>1675</v>
       </c>
       <c r="T138" s="22" t="n">
-        <v>0</v>
+        <v>63.8</v>
       </c>
       <c r="U138" s="24" t="n">
-        <v>925</v>
+        <v>1870</v>
       </c>
       <c r="V138" s="22" t="n">
-        <v>72.3</v>
+        <v>54.2</v>
       </c>
       <c r="W138" s="25" t="n">
-        <v>1462</v>
+        <v>1958</v>
       </c>
       <c r="X138" s="22" t="n">
-        <v>51.3</v>
-      </c>
-      <c r="Y138" s="22" t="n">
-        <v>-1</v>
+        <v>39.8</v>
+      </c>
+      <c r="Y138" s="24" t="n">
+        <v>1832</v>
       </c>
       <c r="Z138" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA138" s="23" t="n">
-        <v>430</v>
+        <v>47.9</v>
+      </c>
+      <c r="AA138" s="24" t="n">
+        <v>908</v>
       </c>
       <c r="AB138" s="22" t="n">
-        <v>86.2</v>
+        <v>71.5</v>
       </c>
       <c r="AC138" s="22" t="n">
         <v>-1</v>
@@ -13421,17 +13416,22 @@
       <c r="AD138" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="AE138" s="21" t="n">
-        <v>225</v>
+      <c r="AE138" s="22" t="n">
+        <v>-1</v>
       </c>
       <c r="AF138" s="22" t="n">
-        <v>95.3</v>
-      </c>
-      <c r="AG138" s="23" t="n">
-        <v>500</v>
+        <v>0</v>
+      </c>
+      <c r="AG138" s="24" t="n">
+        <v>1361</v>
       </c>
       <c r="AH138" s="22" t="n">
-        <v>83.8</v>
+        <v>59.6</v>
+      </c>
+      <c r="AI138" s="9" t="inlineStr">
+        <is>
+          <t>Google-Logo</t>
+        </is>
       </c>
     </row>
     <row r="139">
@@ -13442,11 +13442,11 @@
       </c>
       <c r="B139" s="18" t="inlineStr">
         <is>
-          <t>fuxuemingzhu</t>
+          <t>dhf13</t>
         </is>
       </c>
       <c r="C139" s="5" t="n">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="D139" s="19" t="inlineStr">
         <is>
@@ -13483,70 +13483,65 @@
       <c r="N139" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="O139" s="21" t="n">
-        <v>28</v>
+      <c r="O139" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="P139" s="20" t="n">
-        <v>99.40000000000001</v>
-      </c>
-      <c r="Q139" s="23" t="n">
-        <v>364</v>
+        <v>0</v>
+      </c>
+      <c r="Q139" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="R139" s="20" t="n">
-        <v>88.59999999999999</v>
-      </c>
-      <c r="S139" s="23" t="n">
-        <v>859</v>
+        <v>0</v>
+      </c>
+      <c r="S139" s="20" t="n">
+        <v>-1</v>
       </c>
       <c r="T139" s="20" t="n">
-        <v>79</v>
+        <v>0</v>
       </c>
       <c r="U139" s="24" t="n">
-        <v>1338</v>
+        <v>925</v>
       </c>
       <c r="V139" s="20" t="n">
-        <v>64.40000000000001</v>
-      </c>
-      <c r="W139" s="24" t="n">
-        <v>885</v>
+        <v>72.3</v>
+      </c>
+      <c r="W139" s="25" t="n">
+        <v>1462</v>
       </c>
       <c r="X139" s="20" t="n">
-        <v>69.59999999999999</v>
-      </c>
-      <c r="Y139" s="24" t="n">
-        <v>1573</v>
+        <v>51.3</v>
+      </c>
+      <c r="Y139" s="20" t="n">
+        <v>-1</v>
       </c>
       <c r="Z139" s="20" t="n">
-        <v>53.9</v>
-      </c>
-      <c r="AA139" s="24" t="n">
-        <v>828</v>
+        <v>0</v>
+      </c>
+      <c r="AA139" s="23" t="n">
+        <v>430</v>
       </c>
       <c r="AB139" s="20" t="n">
-        <v>73.09999999999999</v>
-      </c>
-      <c r="AC139" s="23" t="n">
-        <v>846</v>
+        <v>86.2</v>
+      </c>
+      <c r="AC139" s="20" t="n">
+        <v>-1</v>
       </c>
       <c r="AD139" s="20" t="n">
-        <v>77.5</v>
-      </c>
-      <c r="AE139" s="23" t="n">
-        <v>459</v>
+        <v>0</v>
+      </c>
+      <c r="AE139" s="21" t="n">
+        <v>225</v>
       </c>
       <c r="AF139" s="20" t="n">
-        <v>85.5</v>
-      </c>
-      <c r="AG139" s="24" t="n">
-        <v>1117</v>
+        <v>95.3</v>
+      </c>
+      <c r="AG139" s="23" t="n">
+        <v>500</v>
       </c>
       <c r="AH139" s="20" t="n">
-        <v>65.09999999999999</v>
-      </c>
-      <c r="AI139" s="9" t="inlineStr">
-        <is>
-          <t>ByteDance-Logo</t>
-        </is>
+        <v>83.8</v>
       </c>
     </row>
     <row r="140">
@@ -13557,11 +13552,11 @@
       </c>
       <c r="B140" s="1" t="inlineStr">
         <is>
-          <t>fyang618</t>
+          <t>fbian</t>
         </is>
       </c>
       <c r="C140" s="11" t="n">
-        <v>164</v>
+        <v>120</v>
       </c>
       <c r="D140" s="19" t="inlineStr">
         <is>
@@ -13604,59 +13599,64 @@
       <c r="P140" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="Q140" s="24" t="n">
-        <v>1285</v>
+      <c r="Q140" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="R140" s="22" t="n">
-        <v>67.5</v>
-      </c>
-      <c r="S140" s="23" t="n">
-        <v>1737</v>
+        <v>0</v>
+      </c>
+      <c r="S140" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="T140" s="22" t="n">
-        <v>62.6</v>
-      </c>
-      <c r="U140" s="25" t="n">
-        <v>2064</v>
+        <v>0</v>
+      </c>
+      <c r="U140" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="V140" s="22" t="n">
-        <v>45.4</v>
-      </c>
-      <c r="W140" s="25" t="n">
-        <v>1848</v>
+        <v>0</v>
+      </c>
+      <c r="W140" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="X140" s="22" t="n">
-        <v>42.4</v>
-      </c>
-      <c r="Y140" s="23" t="n">
-        <v>997</v>
+        <v>0</v>
+      </c>
+      <c r="Y140" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="Z140" s="22" t="n">
-        <v>72.09999999999999</v>
+        <v>0</v>
       </c>
       <c r="AA140" s="22" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AB140" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="AC140" s="23" t="n">
-        <v>872</v>
+      <c r="AC140" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="AD140" s="22" t="n">
-        <v>77</v>
-      </c>
-      <c r="AE140" s="23" t="n">
-        <v>484</v>
+        <v>0</v>
+      </c>
+      <c r="AE140" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="AF140" s="22" t="n">
-        <v>84.90000000000001</v>
+        <v>0</v>
       </c>
       <c r="AG140" s="22" t="n">
         <v>-1</v>
       </c>
       <c r="AH140" s="22" t="n">
         <v>0</v>
+      </c>
+      <c r="AI140" s="9" t="inlineStr">
+        <is>
+          <t>Google-Logo</t>
+        </is>
       </c>
     </row>
     <row r="141">
@@ -13667,11 +13667,11 @@
       </c>
       <c r="B141" s="18" t="inlineStr">
         <is>
-          <t>galiniunan</t>
+          <t>fuxuemingzhu</t>
         </is>
       </c>
       <c r="C141" s="5" t="n">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="D141" s="19" t="inlineStr">
         <is>
@@ -13684,89 +13684,94 @@
       <c r="F141" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G141" s="21" t="n">
-        <v>851</v>
+      <c r="G141" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="H141" s="20" t="n">
-        <v>86.09999999999999</v>
-      </c>
-      <c r="I141" s="21" t="n">
-        <v>438</v>
+        <v>0</v>
+      </c>
+      <c r="I141" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="J141" s="20" t="n">
-        <v>93.3</v>
-      </c>
-      <c r="K141" s="21" t="n">
-        <v>52</v>
+        <v>0</v>
+      </c>
+      <c r="K141" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="L141" s="20" t="n">
-        <v>99.09999999999999</v>
-      </c>
-      <c r="M141" s="23" t="n">
-        <v>504</v>
+        <v>0</v>
+      </c>
+      <c r="M141" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="N141" s="20" t="n">
-        <v>87.2</v>
+        <v>0</v>
       </c>
       <c r="O141" s="21" t="n">
-        <v>305</v>
+        <v>28</v>
       </c>
       <c r="P141" s="20" t="n">
-        <v>94</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="Q141" s="23" t="n">
-        <v>1102</v>
+        <v>364</v>
       </c>
       <c r="R141" s="20" t="n">
-        <v>75.7</v>
-      </c>
-      <c r="S141" s="21" t="n">
-        <v>540</v>
+        <v>88.59999999999999</v>
+      </c>
+      <c r="S141" s="23" t="n">
+        <v>859</v>
       </c>
       <c r="T141" s="20" t="n">
-        <v>89.90000000000001</v>
-      </c>
-      <c r="U141" s="21" t="n">
-        <v>56</v>
+        <v>79</v>
+      </c>
+      <c r="U141" s="24" t="n">
+        <v>1338</v>
       </c>
       <c r="V141" s="20" t="n">
-        <v>98.90000000000001</v>
-      </c>
-      <c r="W141" s="21" t="n">
-        <v>97</v>
+        <v>64.40000000000001</v>
+      </c>
+      <c r="W141" s="24" t="n">
+        <v>885</v>
       </c>
       <c r="X141" s="20" t="n">
-        <v>97.8</v>
-      </c>
-      <c r="Y141" s="21" t="n">
-        <v>170</v>
+        <v>69.59999999999999</v>
+      </c>
+      <c r="Y141" s="24" t="n">
+        <v>1573</v>
       </c>
       <c r="Z141" s="20" t="n">
-        <v>96.09999999999999</v>
-      </c>
-      <c r="AA141" s="21" t="n">
-        <v>184</v>
+        <v>53.9</v>
+      </c>
+      <c r="AA141" s="24" t="n">
+        <v>828</v>
       </c>
       <c r="AB141" s="20" t="n">
-        <v>96.2</v>
-      </c>
-      <c r="AC141" s="21" t="n">
-        <v>345</v>
+        <v>73.09999999999999</v>
+      </c>
+      <c r="AC141" s="23" t="n">
+        <v>846</v>
       </c>
       <c r="AD141" s="20" t="n">
-        <v>92.90000000000001</v>
+        <v>77.5</v>
       </c>
       <c r="AE141" s="23" t="n">
-        <v>1023</v>
+        <v>459</v>
       </c>
       <c r="AF141" s="20" t="n">
-        <v>73.7</v>
-      </c>
-      <c r="AG141" s="25" t="n">
-        <v>1455</v>
+        <v>85.5</v>
+      </c>
+      <c r="AG141" s="24" t="n">
+        <v>1117</v>
       </c>
       <c r="AH141" s="20" t="n">
-        <v>52.5</v>
+        <v>65.09999999999999</v>
+      </c>
+      <c r="AI141" s="9" t="inlineStr">
+        <is>
+          <t>ByteDance-Logo</t>
+        </is>
       </c>
     </row>
     <row r="142">
@@ -13777,11 +13782,11 @@
       </c>
       <c r="B142" s="1" t="inlineStr">
         <is>
-          <t>gyf6434</t>
+          <t>fyang618</t>
         </is>
       </c>
       <c r="C142" s="11" t="n">
-        <v>19</v>
+        <v>164</v>
       </c>
       <c r="D142" s="19" t="inlineStr">
         <is>
@@ -13795,85 +13800,85 @@
         <v>0</v>
       </c>
       <c r="G142" s="22" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="H142" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="I142" s="25" t="n">
-        <v>2209</v>
+      <c r="I142" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="J142" s="22" t="n">
-        <v>51.2</v>
-      </c>
-      <c r="K142" s="25" t="n">
-        <v>2198</v>
+        <v>0</v>
+      </c>
+      <c r="K142" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="L142" s="22" t="n">
-        <v>45.5</v>
+        <v>0</v>
       </c>
       <c r="M142" s="22" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="N142" s="22" t="n">
         <v>0</v>
       </c>
       <c r="O142" s="22" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="P142" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="Q142" s="22" t="n">
-        <v>-2</v>
+      <c r="Q142" s="24" t="n">
+        <v>1285</v>
       </c>
       <c r="R142" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="S142" s="22" t="n">
-        <v>-2</v>
+        <v>67.5</v>
+      </c>
+      <c r="S142" s="23" t="n">
+        <v>1737</v>
       </c>
       <c r="T142" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="U142" s="22" t="n">
-        <v>-2</v>
+        <v>62.6</v>
+      </c>
+      <c r="U142" s="25" t="n">
+        <v>2064</v>
       </c>
       <c r="V142" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="W142" s="22" t="n">
-        <v>-2</v>
+        <v>45.4</v>
+      </c>
+      <c r="W142" s="25" t="n">
+        <v>1848</v>
       </c>
       <c r="X142" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y142" s="22" t="n">
-        <v>-2</v>
+        <v>42.4</v>
+      </c>
+      <c r="Y142" s="23" t="n">
+        <v>997</v>
       </c>
       <c r="Z142" s="22" t="n">
-        <v>0</v>
+        <v>72.09999999999999</v>
       </c>
       <c r="AA142" s="22" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AB142" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="AC142" s="22" t="n">
-        <v>-2</v>
+      <c r="AC142" s="23" t="n">
+        <v>872</v>
       </c>
       <c r="AD142" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE142" s="22" t="n">
-        <v>-2</v>
+        <v>77</v>
+      </c>
+      <c r="AE142" s="23" t="n">
+        <v>484</v>
       </c>
       <c r="AF142" s="22" t="n">
-        <v>0</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="AG142" s="22" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AH142" s="22" t="n">
         <v>0</v>
@@ -13887,11 +13892,11 @@
       </c>
       <c r="B143" s="18" t="inlineStr">
         <is>
-          <t>hgzry812</t>
+          <t>galiniunan</t>
         </is>
       </c>
       <c r="C143" s="5" t="n">
-        <v>15</v>
+        <v>199</v>
       </c>
       <c r="D143" s="19" t="inlineStr">
         <is>
@@ -13904,89 +13909,89 @@
       <c r="F143" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G143" s="20" t="n">
-        <v>-3</v>
+      <c r="G143" s="21" t="n">
+        <v>851</v>
       </c>
       <c r="H143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="I143" s="20" t="n">
-        <v>-3</v>
+        <v>86.09999999999999</v>
+      </c>
+      <c r="I143" s="21" t="n">
+        <v>438</v>
       </c>
       <c r="J143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="K143" s="20" t="n">
-        <v>-3</v>
+        <v>93.3</v>
+      </c>
+      <c r="K143" s="21" t="n">
+        <v>52</v>
       </c>
       <c r="L143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="M143" s="20" t="n">
-        <v>-3</v>
+        <v>99.09999999999999</v>
+      </c>
+      <c r="M143" s="23" t="n">
+        <v>504</v>
       </c>
       <c r="N143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="O143" s="20" t="n">
-        <v>-3</v>
+        <v>87.2</v>
+      </c>
+      <c r="O143" s="21" t="n">
+        <v>305</v>
       </c>
       <c r="P143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q143" s="20" t="n">
-        <v>-3</v>
+        <v>94</v>
+      </c>
+      <c r="Q143" s="23" t="n">
+        <v>1102</v>
       </c>
       <c r="R143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="S143" s="20" t="n">
-        <v>-1</v>
+        <v>75.7</v>
+      </c>
+      <c r="S143" s="21" t="n">
+        <v>540</v>
       </c>
       <c r="T143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="U143" s="20" t="n">
-        <v>-1</v>
+        <v>89.90000000000001</v>
+      </c>
+      <c r="U143" s="21" t="n">
+        <v>56</v>
       </c>
       <c r="V143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="W143" s="20" t="n">
-        <v>-2</v>
+        <v>98.90000000000001</v>
+      </c>
+      <c r="W143" s="21" t="n">
+        <v>97</v>
       </c>
       <c r="X143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y143" s="20" t="n">
-        <v>-2</v>
+        <v>97.8</v>
+      </c>
+      <c r="Y143" s="21" t="n">
+        <v>170</v>
       </c>
       <c r="Z143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA143" s="20" t="n">
-        <v>-2</v>
+        <v>96.09999999999999</v>
+      </c>
+      <c r="AA143" s="21" t="n">
+        <v>184</v>
       </c>
       <c r="AB143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC143" s="20" t="n">
-        <v>-2</v>
+        <v>96.2</v>
+      </c>
+      <c r="AC143" s="21" t="n">
+        <v>345</v>
       </c>
       <c r="AD143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE143" s="20" t="n">
-        <v>-2</v>
+        <v>92.90000000000001</v>
+      </c>
+      <c r="AE143" s="23" t="n">
+        <v>1023</v>
       </c>
       <c r="AF143" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG143" s="20" t="n">
-        <v>-2</v>
+        <v>73.7</v>
+      </c>
+      <c r="AG143" s="25" t="n">
+        <v>1455</v>
       </c>
       <c r="AH143" s="20" t="n">
-        <v>0</v>
+        <v>52.5</v>
       </c>
     </row>
     <row r="144">
@@ -13997,11 +14002,11 @@
       </c>
       <c r="B144" s="1" t="inlineStr">
         <is>
-          <t>jiancheng2</t>
+          <t>gyf6434</t>
         </is>
       </c>
       <c r="C144" s="11" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D144" s="19" t="inlineStr">
         <is>
@@ -14015,46 +14020,46 @@
         <v>0</v>
       </c>
       <c r="G144" s="22" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="H144" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="I144" s="22" t="n">
-        <v>-3</v>
+      <c r="I144" s="25" t="n">
+        <v>2209</v>
       </c>
       <c r="J144" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K144" s="22" t="n">
-        <v>-3</v>
+        <v>51.2</v>
+      </c>
+      <c r="K144" s="25" t="n">
+        <v>2198</v>
       </c>
       <c r="L144" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="M144" s="25" t="n">
-        <v>3089</v>
+        <v>45.5</v>
+      </c>
+      <c r="M144" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="N144" s="22" t="n">
-        <v>37.1</v>
-      </c>
-      <c r="O144" s="23" t="n">
-        <v>1457</v>
+        <v>0</v>
+      </c>
+      <c r="O144" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="P144" s="22" t="n">
-        <v>66.40000000000001</v>
-      </c>
-      <c r="Q144" s="23" t="n">
-        <v>819</v>
+        <v>0</v>
+      </c>
+      <c r="Q144" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="R144" s="22" t="n">
-        <v>80.59999999999999</v>
-      </c>
-      <c r="S144" s="21" t="n">
-        <v>514</v>
+        <v>0</v>
+      </c>
+      <c r="S144" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="T144" s="22" t="n">
-        <v>90.40000000000001</v>
+        <v>0</v>
       </c>
       <c r="U144" s="22" t="n">
         <v>-2</v>
@@ -14107,11 +14112,11 @@
       </c>
       <c r="B145" s="18" t="inlineStr">
         <is>
-          <t>jiang718</t>
+          <t>hgzry812</t>
         </is>
       </c>
       <c r="C145" s="5" t="n">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D145" s="19" t="inlineStr">
         <is>
@@ -14161,57 +14166,52 @@
         <v>0</v>
       </c>
       <c r="S145" s="20" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="T145" s="20" t="n">
         <v>0</v>
       </c>
       <c r="U145" s="20" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="V145" s="20" t="n">
         <v>0</v>
       </c>
       <c r="W145" s="20" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="X145" s="20" t="n">
         <v>0</v>
       </c>
       <c r="Y145" s="20" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="Z145" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AA145" s="20" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AB145" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AC145" s="23" t="n">
-        <v>544</v>
+      <c r="AC145" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="AD145" s="20" t="n">
-        <v>83.8</v>
+        <v>0</v>
       </c>
       <c r="AE145" s="20" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AF145" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AG145" s="23" t="n">
-        <v>461</v>
+      <c r="AG145" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="AH145" s="20" t="n">
-        <v>84.7</v>
-      </c>
-      <c r="AI145" s="9" t="inlineStr">
-        <is>
-          <t>PureStorage-Logo</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -14222,11 +14222,11 @@
       </c>
       <c r="B146" s="1" t="inlineStr">
         <is>
-          <t>jianzhun</t>
+          <t>jiancheng2</t>
         </is>
       </c>
       <c r="C146" s="11" t="n">
-        <v>74</v>
+        <v>14</v>
       </c>
       <c r="D146" s="19" t="inlineStr">
         <is>
@@ -14257,76 +14257,71 @@
       <c r="L146" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="M146" s="22" t="n">
-        <v>-3</v>
+      <c r="M146" s="25" t="n">
+        <v>3089</v>
       </c>
       <c r="N146" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="O146" s="22" t="n">
-        <v>-3</v>
+        <v>37.1</v>
+      </c>
+      <c r="O146" s="23" t="n">
+        <v>1457</v>
       </c>
       <c r="P146" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q146" s="22" t="n">
-        <v>-3</v>
+        <v>66.40000000000001</v>
+      </c>
+      <c r="Q146" s="23" t="n">
+        <v>819</v>
       </c>
       <c r="R146" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="S146" s="22" t="n">
-        <v>-3</v>
+        <v>80.59999999999999</v>
+      </c>
+      <c r="S146" s="21" t="n">
+        <v>514</v>
       </c>
       <c r="T146" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="U146" s="23" t="n">
-        <v>448</v>
+        <v>90.40000000000001</v>
+      </c>
+      <c r="U146" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="V146" s="22" t="n">
-        <v>86.40000000000001</v>
-      </c>
-      <c r="W146" s="25" t="n">
-        <v>1841</v>
+        <v>0</v>
+      </c>
+      <c r="W146" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="X146" s="22" t="n">
-        <v>42.5</v>
-      </c>
-      <c r="Y146" s="21" t="n">
-        <v>813</v>
+        <v>0</v>
+      </c>
+      <c r="Y146" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="Z146" s="22" t="n">
-        <v>81.3</v>
-      </c>
-      <c r="AA146" s="21" t="n">
-        <v>205</v>
+        <v>0</v>
+      </c>
+      <c r="AA146" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AB146" s="22" t="n">
-        <v>95.8</v>
-      </c>
-      <c r="AC146" s="21" t="n">
-        <v>518</v>
+        <v>0</v>
+      </c>
+      <c r="AC146" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AD146" s="22" t="n">
-        <v>89.3</v>
-      </c>
-      <c r="AE146" s="23" t="n">
-        <v>672</v>
+        <v>0</v>
+      </c>
+      <c r="AE146" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AF146" s="22" t="n">
-        <v>81</v>
-      </c>
-      <c r="AG146" s="23" t="n">
-        <v>642</v>
+        <v>0</v>
+      </c>
+      <c r="AG146" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AH146" s="22" t="n">
-        <v>80.7</v>
-      </c>
-      <c r="AI146" s="9" t="inlineStr">
-        <is>
-          <t>SnowFlake-Logo</t>
-        </is>
+        <v>0</v>
       </c>
     </row>
     <row r="147">
@@ -14337,11 +14332,11 @@
       </c>
       <c r="B147" s="18" t="inlineStr">
         <is>
-          <t>kaihaohust</t>
+          <t>jiang718</t>
         </is>
       </c>
       <c r="C147" s="5" t="n">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="D147" s="19" t="inlineStr">
         <is>
@@ -14385,62 +14380,62 @@
         <v>0</v>
       </c>
       <c r="Q147" s="20" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="R147" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="S147" s="23" t="n">
-        <v>838</v>
+      <c r="S147" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="T147" s="20" t="n">
-        <v>79.40000000000001</v>
-      </c>
-      <c r="U147" s="24" t="n">
-        <v>917</v>
+        <v>0</v>
+      </c>
+      <c r="U147" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="V147" s="20" t="n">
-        <v>72.40000000000001</v>
-      </c>
-      <c r="W147" s="23" t="n">
-        <v>195</v>
+        <v>0</v>
+      </c>
+      <c r="W147" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="X147" s="20" t="n">
-        <v>90.5</v>
-      </c>
-      <c r="Y147" s="21" t="n">
-        <v>45</v>
+        <v>0</v>
+      </c>
+      <c r="Y147" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="Z147" s="20" t="n">
-        <v>99</v>
-      </c>
-      <c r="AA147" s="23" t="n">
-        <v>497</v>
+        <v>0</v>
+      </c>
+      <c r="AA147" s="20" t="n">
+        <v>-1</v>
       </c>
       <c r="AB147" s="20" t="n">
-        <v>84.90000000000001</v>
-      </c>
-      <c r="AC147" s="21" t="n">
-        <v>336</v>
+        <v>0</v>
+      </c>
+      <c r="AC147" s="23" t="n">
+        <v>544</v>
       </c>
       <c r="AD147" s="20" t="n">
-        <v>93.09999999999999</v>
-      </c>
-      <c r="AE147" s="23" t="n">
-        <v>443</v>
+        <v>83.8</v>
+      </c>
+      <c r="AE147" s="20" t="n">
+        <v>-1</v>
       </c>
       <c r="AF147" s="20" t="n">
-        <v>85.8</v>
+        <v>0</v>
       </c>
       <c r="AG147" s="23" t="n">
-        <v>290</v>
+        <v>461</v>
       </c>
       <c r="AH147" s="20" t="n">
-        <v>88.5</v>
+        <v>84.7</v>
       </c>
       <c r="AI147" s="9" t="inlineStr">
         <is>
-          <t>Walmart-Logo</t>
+          <t>PureStorage-Logo</t>
         </is>
       </c>
     </row>
@@ -14452,11 +14447,11 @@
       </c>
       <c r="B148" s="1" t="inlineStr">
         <is>
-          <t>liuguanhualouie</t>
+          <t>jianzhun</t>
         </is>
       </c>
       <c r="C148" s="11" t="n">
-        <v>24</v>
+        <v>74</v>
       </c>
       <c r="D148" s="19" t="inlineStr">
         <is>
@@ -14469,93 +14464,93 @@
       <c r="F148" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="G148" s="25" t="n">
-        <v>2605</v>
+      <c r="G148" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="H148" s="22" t="n">
-        <v>42.4</v>
+        <v>0</v>
       </c>
       <c r="I148" s="22" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="J148" s="22" t="n">
         <v>0</v>
       </c>
       <c r="K148" s="22" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="L148" s="22" t="n">
         <v>0</v>
       </c>
       <c r="M148" s="22" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="N148" s="22" t="n">
         <v>0</v>
       </c>
       <c r="O148" s="22" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="P148" s="22" t="n">
         <v>0</v>
       </c>
       <c r="Q148" s="22" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="R148" s="22" t="n">
         <v>0</v>
       </c>
       <c r="S148" s="22" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="T148" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="U148" s="22" t="n">
-        <v>-2</v>
+      <c r="U148" s="23" t="n">
+        <v>448</v>
       </c>
       <c r="V148" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="W148" s="22" t="n">
-        <v>-2</v>
+        <v>86.40000000000001</v>
+      </c>
+      <c r="W148" s="25" t="n">
+        <v>1841</v>
       </c>
       <c r="X148" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y148" s="22" t="n">
-        <v>-2</v>
+        <v>42.5</v>
+      </c>
+      <c r="Y148" s="21" t="n">
+        <v>813</v>
       </c>
       <c r="Z148" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA148" s="22" t="n">
-        <v>-2</v>
+        <v>81.3</v>
+      </c>
+      <c r="AA148" s="21" t="n">
+        <v>205</v>
       </c>
       <c r="AB148" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC148" s="22" t="n">
-        <v>-2</v>
+        <v>95.8</v>
+      </c>
+      <c r="AC148" s="21" t="n">
+        <v>518</v>
       </c>
       <c r="AD148" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE148" s="22" t="n">
-        <v>-2</v>
+        <v>89.3</v>
+      </c>
+      <c r="AE148" s="23" t="n">
+        <v>672</v>
       </c>
       <c r="AF148" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG148" s="22" t="n">
-        <v>-2</v>
+        <v>81</v>
+      </c>
+      <c r="AG148" s="23" t="n">
+        <v>642</v>
       </c>
       <c r="AH148" s="22" t="n">
-        <v>0</v>
+        <v>80.7</v>
       </c>
       <c r="AI148" s="9" t="inlineStr">
         <is>
-          <t>Amazon-Logo</t>
+          <t>SnowFlake-Logo</t>
         </is>
       </c>
     </row>
@@ -14567,11 +14562,11 @@
       </c>
       <c r="B149" s="18" t="inlineStr">
         <is>
-          <t>memoryfraction</t>
+          <t>jzcheng</t>
         </is>
       </c>
       <c r="C149" s="5" t="n">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="D149" s="19" t="inlineStr">
         <is>
@@ -14602,68 +14597,68 @@
       <c r="L149" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="M149" s="25" t="n">
-        <v>3161</v>
+      <c r="M149" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="N149" s="20" t="n">
-        <v>36</v>
-      </c>
-      <c r="O149" s="21" t="n">
-        <v>845</v>
+        <v>0</v>
+      </c>
+      <c r="O149" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="P149" s="20" t="n">
-        <v>83.40000000000001</v>
-      </c>
-      <c r="Q149" s="25" t="n">
-        <v>2634</v>
+        <v>0</v>
+      </c>
+      <c r="Q149" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="R149" s="20" t="n">
-        <v>38.8</v>
-      </c>
-      <c r="S149" s="23" t="n">
-        <v>1461</v>
+        <v>0</v>
+      </c>
+      <c r="S149" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="T149" s="20" t="n">
-        <v>67.7</v>
-      </c>
-      <c r="U149" s="24" t="n">
-        <v>1686</v>
+        <v>0</v>
+      </c>
+      <c r="U149" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="V149" s="20" t="n">
-        <v>57.7</v>
-      </c>
-      <c r="W149" s="25" t="n">
-        <v>1913</v>
+        <v>0</v>
+      </c>
+      <c r="W149" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="X149" s="20" t="n">
-        <v>40.9</v>
-      </c>
-      <c r="Y149" s="23" t="n">
-        <v>931</v>
+        <v>0</v>
+      </c>
+      <c r="Y149" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="Z149" s="20" t="n">
-        <v>73.59999999999999</v>
-      </c>
-      <c r="AA149" s="25" t="n">
-        <v>1762</v>
+        <v>0</v>
+      </c>
+      <c r="AA149" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="AB149" s="20" t="n">
-        <v>49.1</v>
-      </c>
-      <c r="AC149" s="24" t="n">
-        <v>2079</v>
+        <v>0</v>
+      </c>
+      <c r="AC149" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="AD149" s="20" t="n">
-        <v>47.1</v>
-      </c>
-      <c r="AE149" s="24" t="n">
-        <v>2027</v>
+        <v>0</v>
+      </c>
+      <c r="AE149" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="AF149" s="20" t="n">
-        <v>47.8</v>
+        <v>0</v>
       </c>
       <c r="AG149" s="20" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AH149" s="20" t="n">
         <v>0</v>
@@ -14677,11 +14672,11 @@
       </c>
       <c r="B150" s="1" t="inlineStr">
         <is>
-          <t>pjincz</t>
+          <t>kaihaohust</t>
         </is>
       </c>
       <c r="C150" s="11" t="n">
-        <v>62</v>
+        <v>74</v>
       </c>
       <c r="D150" s="19" t="inlineStr">
         <is>
@@ -14724,59 +14719,64 @@
       <c r="P150" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="Q150" s="21" t="n">
-        <v>35</v>
+      <c r="Q150" s="22" t="n">
+        <v>-1</v>
       </c>
       <c r="R150" s="22" t="n">
-        <v>99.40000000000001</v>
-      </c>
-      <c r="S150" s="22" t="n">
-        <v>-1</v>
+        <v>0</v>
+      </c>
+      <c r="S150" s="23" t="n">
+        <v>838</v>
       </c>
       <c r="T150" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="U150" s="21" t="n">
-        <v>48</v>
+        <v>79.40000000000001</v>
+      </c>
+      <c r="U150" s="24" t="n">
+        <v>917</v>
       </c>
       <c r="V150" s="22" t="n">
-        <v>99.09999999999999</v>
-      </c>
-      <c r="W150" s="22" t="n">
-        <v>-1</v>
+        <v>72.40000000000001</v>
+      </c>
+      <c r="W150" s="23" t="n">
+        <v>195</v>
       </c>
       <c r="X150" s="22" t="n">
-        <v>0</v>
+        <v>90.5</v>
       </c>
       <c r="Y150" s="21" t="n">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="Z150" s="22" t="n">
-        <v>99.3</v>
-      </c>
-      <c r="AA150" s="21" t="n">
-        <v>7</v>
+        <v>99</v>
+      </c>
+      <c r="AA150" s="23" t="n">
+        <v>497</v>
       </c>
       <c r="AB150" s="22" t="n">
-        <v>99.90000000000001</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="AC150" s="21" t="n">
-        <v>93</v>
+        <v>336</v>
       </c>
       <c r="AD150" s="22" t="n">
-        <v>98.09999999999999</v>
-      </c>
-      <c r="AE150" s="21" t="n">
-        <v>20</v>
+        <v>93.09999999999999</v>
+      </c>
+      <c r="AE150" s="23" t="n">
+        <v>443</v>
       </c>
       <c r="AF150" s="22" t="n">
-        <v>99.59999999999999</v>
-      </c>
-      <c r="AG150" s="21" t="n">
-        <v>39</v>
+        <v>85.8</v>
+      </c>
+      <c r="AG150" s="23" t="n">
+        <v>290</v>
       </c>
       <c r="AH150" s="22" t="n">
-        <v>99.09999999999999</v>
+        <v>88.5</v>
+      </c>
+      <c r="AI150" s="9" t="inlineStr">
+        <is>
+          <t>Walmart-Logo</t>
+        </is>
       </c>
     </row>
     <row r="151">
@@ -14787,11 +14787,11 @@
       </c>
       <c r="B151" s="18" t="inlineStr">
         <is>
-          <t>shuizhouwang</t>
+          <t>linshenknows</t>
         </is>
       </c>
       <c r="C151" s="5" t="n">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D151" s="19" t="inlineStr">
         <is>
@@ -14805,85 +14805,85 @@
         <v>0</v>
       </c>
       <c r="G151" s="20" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="H151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="I151" s="20" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="J151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="K151" s="20" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="L151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="M151" s="20" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="N151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="O151" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="P151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="Q151" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="R151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="S151" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="T151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="U151" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="V151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="W151" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="X151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="Y151" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="Z151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AA151" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AB151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AC151" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AD151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AE151" s="20" t="n">
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="AF151" s="20" t="n">
         <v>0</v>
       </c>
       <c r="AG151" s="20" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AH151" s="20" t="n">
         <v>0</v>
@@ -14897,11 +14897,11 @@
       </c>
       <c r="B152" s="1" t="inlineStr">
         <is>
-          <t>sissishiny</t>
+          <t>littleRainRain</t>
         </is>
       </c>
       <c r="C152" s="11" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D152" s="19" t="inlineStr">
         <is>
@@ -14969,34 +14969,34 @@
         <v>0</v>
       </c>
       <c r="Y152" s="22" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="Z152" s="22" t="n">
         <v>0</v>
       </c>
       <c r="AA152" s="22" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AB152" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="AC152" s="24" t="n">
-        <v>1727</v>
+      <c r="AC152" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="AD152" s="22" t="n">
-        <v>54.4</v>
-      </c>
-      <c r="AE152" s="23" t="n">
-        <v>385</v>
+        <v>0</v>
+      </c>
+      <c r="AE152" s="24" t="n">
+        <v>2155</v>
       </c>
       <c r="AF152" s="22" t="n">
-        <v>87</v>
-      </c>
-      <c r="AG152" s="24" t="n">
-        <v>870</v>
+        <v>45.2</v>
+      </c>
+      <c r="AG152" s="25" t="n">
+        <v>2001</v>
       </c>
       <c r="AH152" s="22" t="n">
-        <v>70.59999999999999</v>
+        <v>40.4</v>
       </c>
     </row>
     <row r="153">
@@ -15007,11 +15007,11 @@
       </c>
       <c r="B153" s="18" t="inlineStr">
         <is>
-          <t>softair</t>
+          <t>liuguanhualouie</t>
         </is>
       </c>
       <c r="C153" s="5" t="n">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="D153" s="19" t="inlineStr">
         <is>
@@ -15024,93 +15024,93 @@
       <c r="F153" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="G153" s="20" t="n">
-        <v>-3</v>
+      <c r="G153" s="25" t="n">
+        <v>2605</v>
       </c>
       <c r="H153" s="20" t="n">
-        <v>0</v>
+        <v>42.4</v>
       </c>
       <c r="I153" s="20" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="J153" s="20" t="n">
         <v>0</v>
       </c>
       <c r="K153" s="20" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="L153" s="20" t="n">
         <v>0</v>
       </c>
       <c r="M153" s="20" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="N153" s="20" t="n">
         <v>0</v>
       </c>
       <c r="O153" s="20" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="P153" s="20" t="n">
         <v>0</v>
       </c>
       <c r="Q153" s="20" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="R153" s="20" t="n">
         <v>0</v>
       </c>
       <c r="S153" s="20" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="T153" s="20" t="n">
         <v>0</v>
       </c>
       <c r="U153" s="20" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="V153" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="W153" s="24" t="n">
-        <v>781</v>
+      <c r="W153" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="X153" s="20" t="n">
-        <v>72</v>
-      </c>
-      <c r="Y153" s="23" t="n">
-        <v>1262</v>
+        <v>0</v>
+      </c>
+      <c r="Y153" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="Z153" s="20" t="n">
-        <v>66</v>
-      </c>
-      <c r="AA153" s="23" t="n">
-        <v>617</v>
+        <v>0</v>
+      </c>
+      <c r="AA153" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="AB153" s="20" t="n">
-        <v>82.40000000000001</v>
-      </c>
-      <c r="AC153" s="23" t="n">
-        <v>948</v>
+        <v>0</v>
+      </c>
+      <c r="AC153" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="AD153" s="20" t="n">
-        <v>75.40000000000001</v>
+        <v>0</v>
       </c>
       <c r="AE153" s="20" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="AF153" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AG153" s="24" t="n">
-        <v>1332</v>
+      <c r="AG153" s="20" t="n">
+        <v>-2</v>
       </c>
       <c r="AH153" s="20" t="n">
-        <v>60.3</v>
+        <v>0</v>
       </c>
       <c r="AI153" s="9" t="inlineStr">
         <is>
-          <t>Google-Logo</t>
+          <t>Amazon-Logo</t>
         </is>
       </c>
     </row>
@@ -15122,11 +15122,11 @@
       </c>
       <c r="B154" s="1" t="inlineStr">
         <is>
-          <t>wendyimayday</t>
+          <t>memoryfraction</t>
         </is>
       </c>
       <c r="C154" s="11" t="n">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D154" s="19" t="inlineStr">
         <is>
@@ -15157,71 +15157,71 @@
       <c r="L154" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="M154" s="22" t="n">
-        <v>-3</v>
+      <c r="M154" s="25" t="n">
+        <v>3161</v>
       </c>
       <c r="N154" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="O154" s="22" t="n">
-        <v>-3</v>
+        <v>36</v>
+      </c>
+      <c r="O154" s="21" t="n">
+        <v>845</v>
       </c>
       <c r="P154" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q154" s="22" t="n">
-        <v>-3</v>
+        <v>83.40000000000001</v>
+      </c>
+      <c r="Q154" s="25" t="n">
+        <v>2634</v>
       </c>
       <c r="R154" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="S154" s="22" t="n">
-        <v>-3</v>
+        <v>38.8</v>
+      </c>
+      <c r="S154" s="23" t="n">
+        <v>1461</v>
       </c>
       <c r="T154" s="22" t="n">
-        <v>0</v>
+        <v>67.7</v>
       </c>
       <c r="U154" s="24" t="n">
-        <v>1089</v>
+        <v>1686</v>
       </c>
       <c r="V154" s="22" t="n">
-        <v>69.09999999999999</v>
-      </c>
-      <c r="W154" s="24" t="n">
-        <v>1074</v>
+        <v>57.7</v>
+      </c>
+      <c r="W154" s="25" t="n">
+        <v>1913</v>
       </c>
       <c r="X154" s="22" t="n">
-        <v>65.2</v>
+        <v>40.9</v>
       </c>
       <c r="Y154" s="23" t="n">
-        <v>1228</v>
+        <v>931</v>
       </c>
       <c r="Z154" s="22" t="n">
-        <v>66.8</v>
-      </c>
-      <c r="AA154" s="24" t="n">
-        <v>721</v>
+        <v>73.59999999999999</v>
+      </c>
+      <c r="AA154" s="25" t="n">
+        <v>1762</v>
       </c>
       <c r="AB154" s="22" t="n">
-        <v>75.3</v>
-      </c>
-      <c r="AC154" s="21" t="n">
-        <v>420</v>
+        <v>49.1</v>
+      </c>
+      <c r="AC154" s="24" t="n">
+        <v>2079</v>
       </c>
       <c r="AD154" s="22" t="n">
-        <v>91.3</v>
-      </c>
-      <c r="AE154" s="23" t="n">
-        <v>793</v>
+        <v>47.1</v>
+      </c>
+      <c r="AE154" s="24" t="n">
+        <v>2027</v>
       </c>
       <c r="AF154" s="22" t="n">
-        <v>78.5</v>
-      </c>
-      <c r="AG154" s="25" t="n">
-        <v>1904</v>
+        <v>47.8</v>
+      </c>
+      <c r="AG154" s="22" t="n">
+        <v>-1</v>
       </c>
       <c r="AH154" s="22" t="n">
-        <v>42.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155">
@@ -15232,106 +15232,106 @@
       </c>
       <c r="B155" s="18" t="inlineStr">
         <is>
-          <t>wolf940509</t>
+          <t>pjincz</t>
         </is>
       </c>
       <c r="C155" s="5" t="n">
+        <v>62</v>
+      </c>
+      <c r="D155" s="19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E155" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F155" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G155" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H155" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I155" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="J155" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K155" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L155" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M155" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="N155" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O155" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="P155" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q155" s="21" t="n">
+        <v>35</v>
+      </c>
+      <c r="R155" s="20" t="n">
+        <v>99.40000000000001</v>
+      </c>
+      <c r="S155" s="20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T155" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U155" s="21" t="n">
+        <v>48</v>
+      </c>
+      <c r="V155" s="20" t="n">
+        <v>99.09999999999999</v>
+      </c>
+      <c r="W155" s="20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X155" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y155" s="21" t="n">
+        <v>30</v>
+      </c>
+      <c r="Z155" s="20" t="n">
+        <v>99.3</v>
+      </c>
+      <c r="AA155" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="D155" s="19" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="E155" s="20" t="n">
-        <v>-3</v>
-      </c>
-      <c r="F155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="G155" s="20" t="n">
-        <v>-3</v>
-      </c>
-      <c r="H155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="I155" s="20" t="n">
-        <v>-3</v>
-      </c>
-      <c r="J155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="K155" s="20" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="M155" s="20" t="n">
-        <v>-2</v>
-      </c>
-      <c r="N155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="O155" s="20" t="n">
-        <v>-2</v>
-      </c>
-      <c r="P155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q155" s="20" t="n">
-        <v>-2</v>
-      </c>
-      <c r="R155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="S155" s="20" t="n">
-        <v>-2</v>
-      </c>
-      <c r="T155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="U155" s="20" t="n">
-        <v>-2</v>
-      </c>
-      <c r="V155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="W155" s="20" t="n">
-        <v>-2</v>
-      </c>
-      <c r="X155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y155" s="20" t="n">
-        <v>-2</v>
-      </c>
-      <c r="Z155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA155" s="20" t="n">
-        <v>-2</v>
-      </c>
       <c r="AB155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC155" s="20" t="n">
-        <v>-2</v>
+        <v>99.90000000000001</v>
+      </c>
+      <c r="AC155" s="21" t="n">
+        <v>93</v>
       </c>
       <c r="AD155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE155" s="20" t="n">
-        <v>-2</v>
+        <v>98.09999999999999</v>
+      </c>
+      <c r="AE155" s="21" t="n">
+        <v>20</v>
       </c>
       <c r="AF155" s="20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG155" s="20" t="n">
-        <v>-2</v>
+        <v>99.59999999999999</v>
+      </c>
+      <c r="AG155" s="21" t="n">
+        <v>39</v>
       </c>
       <c r="AH155" s="20" t="n">
-        <v>0</v>
+        <v>99.09999999999999</v>
       </c>
     </row>
     <row r="156">
@@ -15342,11 +15342,11 @@
       </c>
       <c r="B156" s="1" t="inlineStr">
         <is>
-          <t>xfzhao</t>
+          <t>shuizhouwang</t>
         </is>
       </c>
       <c r="C156" s="11" t="n">
-        <v>174</v>
+        <v>26</v>
       </c>
       <c r="D156" s="19" t="inlineStr">
         <is>
@@ -15360,88 +15360,88 @@
         <v>0</v>
       </c>
       <c r="G156" s="22" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="H156" s="22" t="n">
         <v>0</v>
       </c>
       <c r="I156" s="22" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="J156" s="22" t="n">
         <v>0</v>
       </c>
       <c r="K156" s="22" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="L156" s="22" t="n">
         <v>0</v>
       </c>
       <c r="M156" s="22" t="n">
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="N156" s="22" t="n">
         <v>0</v>
       </c>
       <c r="O156" s="22" t="n">
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="P156" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="Q156" s="25" t="n">
-        <v>2477</v>
+      <c r="Q156" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="R156" s="22" t="n">
-        <v>41.6</v>
+        <v>0</v>
       </c>
       <c r="S156" s="22" t="n">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="T156" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="U156" s="25" t="n">
-        <v>2022</v>
+      <c r="U156" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="V156" s="22" t="n">
-        <v>46.2</v>
-      </c>
-      <c r="W156" s="24" t="n">
-        <v>587</v>
+        <v>0</v>
+      </c>
+      <c r="W156" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="X156" s="22" t="n">
-        <v>76.5</v>
-      </c>
-      <c r="Y156" s="21" t="n">
-        <v>654</v>
+        <v>0</v>
+      </c>
+      <c r="Y156" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="Z156" s="22" t="n">
-        <v>85</v>
-      </c>
-      <c r="AA156" s="24" t="n">
-        <v>1297</v>
+        <v>0</v>
+      </c>
+      <c r="AA156" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AB156" s="22" t="n">
-        <v>63.6</v>
-      </c>
-      <c r="AC156" s="24" t="n">
-        <v>1181</v>
+        <v>0</v>
+      </c>
+      <c r="AC156" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AD156" s="22" t="n">
-        <v>65.59999999999999</v>
-      </c>
-      <c r="AE156" s="24" t="n">
-        <v>1234</v>
+        <v>0</v>
+      </c>
+      <c r="AE156" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AF156" s="22" t="n">
-        <v>64.3</v>
-      </c>
-      <c r="AG156" s="25" t="n">
-        <v>2048</v>
+        <v>0</v>
+      </c>
+      <c r="AG156" s="22" t="n">
+        <v>-2</v>
       </c>
       <c r="AH156" s="22" t="n">
-        <v>39.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -15452,11 +15452,11 @@
       </c>
       <c r="B157" s="18" t="inlineStr">
         <is>
-          <t>xxnzym</t>
+          <t>sissishiny</t>
         </is>
       </c>
       <c r="C157" s="5" t="n">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="D157" s="19" t="inlineStr">
         <is>
@@ -15517,46 +15517,41 @@
       <c r="V157" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="W157" s="25" t="n">
-        <v>1799</v>
+      <c r="W157" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="X157" s="20" t="n">
-        <v>43.5</v>
-      </c>
-      <c r="Y157" s="21" t="n">
-        <v>404</v>
+        <v>0</v>
+      </c>
+      <c r="Y157" s="20" t="n">
+        <v>-1</v>
       </c>
       <c r="Z157" s="20" t="n">
-        <v>90.7</v>
-      </c>
-      <c r="AA157" s="23" t="n">
-        <v>629</v>
+        <v>0</v>
+      </c>
+      <c r="AA157" s="20" t="n">
+        <v>-1</v>
       </c>
       <c r="AB157" s="20" t="n">
-        <v>82.2</v>
+        <v>0</v>
       </c>
       <c r="AC157" s="24" t="n">
-        <v>1612</v>
+        <v>1727</v>
       </c>
       <c r="AD157" s="20" t="n">
-        <v>56.7</v>
+        <v>54.4</v>
       </c>
       <c r="AE157" s="23" t="n">
-        <v>477</v>
+        <v>385</v>
       </c>
       <c r="AF157" s="20" t="n">
-        <v>85.09999999999999</v>
+        <v>87</v>
       </c>
       <c r="AG157" s="24" t="n">
-        <v>1153</v>
+        <v>870</v>
       </c>
       <c r="AH157" s="20" t="n">
-        <v>64.3</v>
-      </c>
-      <c r="AI157" s="9" t="inlineStr">
-        <is>
-          <t>Microsoft-Logo</t>
-        </is>
+        <v>70.59999999999999</v>
       </c>
     </row>
     <row r="158">
@@ -15567,11 +15562,11 @@
       </c>
       <c r="B158" s="1" t="inlineStr">
         <is>
-          <t>yexiaoxiao2102</t>
+          <t>softair</t>
         </is>
       </c>
       <c r="C158" s="11" t="n">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D158" s="19" t="inlineStr">
         <is>
@@ -15603,70 +15598,70 @@
         <v>0</v>
       </c>
       <c r="M158" s="22" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="N158" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="O158" s="21" t="n">
-        <v>441</v>
+      <c r="O158" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="P158" s="22" t="n">
-        <v>91.3</v>
-      </c>
-      <c r="Q158" s="23" t="n">
-        <v>773</v>
+        <v>0</v>
+      </c>
+      <c r="Q158" s="22" t="n">
+        <v>-3</v>
       </c>
       <c r="R158" s="22" t="n">
-        <v>81.5</v>
-      </c>
-      <c r="S158" s="21" t="n">
-        <v>225</v>
+        <v>0</v>
+      </c>
+      <c r="S158" s="22" t="n">
+        <v>-1</v>
       </c>
       <c r="T158" s="22" t="n">
-        <v>95.8</v>
-      </c>
-      <c r="U158" s="24" t="n">
-        <v>1256</v>
+        <v>0</v>
+      </c>
+      <c r="U158" s="22" t="n">
+        <v>-1</v>
       </c>
       <c r="V158" s="22" t="n">
-        <v>65.90000000000001</v>
-      </c>
-      <c r="W158" s="22" t="n">
-        <v>-1</v>
+        <v>0</v>
+      </c>
+      <c r="W158" s="24" t="n">
+        <v>781</v>
       </c>
       <c r="X158" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y158" s="24" t="n">
-        <v>1344</v>
+        <v>72</v>
+      </c>
+      <c r="Y158" s="23" t="n">
+        <v>1262</v>
       </c>
       <c r="Z158" s="22" t="n">
-        <v>59.1</v>
+        <v>66</v>
       </c>
       <c r="AA158" s="23" t="n">
-        <v>541</v>
+        <v>617</v>
       </c>
       <c r="AB158" s="22" t="n">
-        <v>84</v>
-      </c>
-      <c r="AC158" s="22" t="n">
-        <v>-2</v>
+        <v>82.40000000000001</v>
+      </c>
+      <c r="AC158" s="23" t="n">
+        <v>948</v>
       </c>
       <c r="AD158" s="22" t="n">
-        <v>0</v>
+        <v>75.40000000000001</v>
       </c>
       <c r="AE158" s="22" t="n">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="AF158" s="22" t="n">
         <v>0</v>
       </c>
-      <c r="AG158" s="22" t="n">
-        <v>-2</v>
+      <c r="AG158" s="24" t="n">
+        <v>1332</v>
       </c>
       <c r="AH158" s="22" t="n">
-        <v>0</v>
+        <v>60.3</v>
       </c>
       <c r="AI158" s="9" t="inlineStr">
         <is>
@@ -15682,11 +15677,11 @@
       </c>
       <c r="B159" s="18" t="inlineStr">
         <is>
-          <t>yykfight</t>
+          <t>tclu82</t>
         </is>
       </c>
       <c r="C159" s="5" t="n">
-        <v>184</v>
+        <v>20</v>
       </c>
       <c r="D159" s="19" t="inlineStr">
         <is>
@@ -15729,59 +15724,59 @@
       <c r="P159" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="Q159" s="25" t="n">
-        <v>2517</v>
+      <c r="Q159" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="R159" s="20" t="n">
-        <v>40.9</v>
+        <v>0</v>
       </c>
       <c r="S159" s="20" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="T159" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="U159" s="24" t="n">
-        <v>1315</v>
+      <c r="U159" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="V159" s="20" t="n">
-        <v>64.8</v>
-      </c>
-      <c r="W159" s="24" t="n">
-        <v>957</v>
+        <v>0</v>
+      </c>
+      <c r="W159" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="X159" s="20" t="n">
-        <v>67.90000000000001</v>
-      </c>
-      <c r="Y159" s="21" t="n">
-        <v>741</v>
+        <v>0</v>
+      </c>
+      <c r="Y159" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="Z159" s="20" t="n">
-        <v>83</v>
+        <v>0</v>
       </c>
       <c r="AA159" s="20" t="n">
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AB159" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="AC159" s="24" t="n">
-        <v>2034</v>
+      <c r="AC159" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="AD159" s="20" t="n">
-        <v>48</v>
-      </c>
-      <c r="AE159" s="23" t="n">
-        <v>914</v>
+        <v>0</v>
+      </c>
+      <c r="AE159" s="20" t="n">
+        <v>-3</v>
       </c>
       <c r="AF159" s="20" t="n">
-        <v>76</v>
-      </c>
-      <c r="AG159" s="24" t="n">
-        <v>995</v>
+        <v>0</v>
+      </c>
+      <c r="AG159" s="25" t="n">
+        <v>1941</v>
       </c>
       <c r="AH159" s="20" t="n">
-        <v>67.8</v>
+        <v>41.7</v>
       </c>
     </row>
     <row r="160">
@@ -15792,108 +15787,998 @@
       </c>
       <c r="B160" s="1" t="inlineStr">
         <is>
+          <t>wendyimayday</t>
+        </is>
+      </c>
+      <c r="C160" s="11" t="n">
+        <v>94</v>
+      </c>
+      <c r="D160" s="19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E160" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F160" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G160" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H160" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I160" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="J160" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K160" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L160" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M160" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="N160" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O160" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="P160" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q160" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="R160" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S160" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T160" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U160" s="24" t="n">
+        <v>1089</v>
+      </c>
+      <c r="V160" s="22" t="n">
+        <v>69.09999999999999</v>
+      </c>
+      <c r="W160" s="24" t="n">
+        <v>1074</v>
+      </c>
+      <c r="X160" s="22" t="n">
+        <v>65.2</v>
+      </c>
+      <c r="Y160" s="23" t="n">
+        <v>1228</v>
+      </c>
+      <c r="Z160" s="22" t="n">
+        <v>66.8</v>
+      </c>
+      <c r="AA160" s="24" t="n">
+        <v>721</v>
+      </c>
+      <c r="AB160" s="22" t="n">
+        <v>75.3</v>
+      </c>
+      <c r="AC160" s="21" t="n">
+        <v>420</v>
+      </c>
+      <c r="AD160" s="22" t="n">
+        <v>91.3</v>
+      </c>
+      <c r="AE160" s="23" t="n">
+        <v>793</v>
+      </c>
+      <c r="AF160" s="22" t="n">
+        <v>78.5</v>
+      </c>
+      <c r="AG160" s="25" t="n">
+        <v>1904</v>
+      </c>
+      <c r="AH160" s="22" t="n">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B161" s="18" t="inlineStr">
+        <is>
+          <t>wolf940509</t>
+        </is>
+      </c>
+      <c r="C161" s="5" t="n">
+        <v>7</v>
+      </c>
+      <c r="D161" s="19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E161" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G161" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I161" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="J161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K161" s="20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M161" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="N161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O161" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="P161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q161" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="R161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S161" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="T161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U161" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="V161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W161" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="X161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y161" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="Z161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA161" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AB161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC161" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AD161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE161" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AF161" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG161" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AH161" s="20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B162" s="1" t="inlineStr">
+        <is>
+          <t>xfzhao</t>
+        </is>
+      </c>
+      <c r="C162" s="11" t="n">
+        <v>174</v>
+      </c>
+      <c r="D162" s="19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E162" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F162" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G162" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H162" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I162" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="J162" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K162" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L162" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M162" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="N162" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O162" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="P162" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q162" s="25" t="n">
+        <v>2477</v>
+      </c>
+      <c r="R162" s="22" t="n">
+        <v>41.6</v>
+      </c>
+      <c r="S162" s="22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T162" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U162" s="25" t="n">
+        <v>2022</v>
+      </c>
+      <c r="V162" s="22" t="n">
+        <v>46.2</v>
+      </c>
+      <c r="W162" s="24" t="n">
+        <v>587</v>
+      </c>
+      <c r="X162" s="22" t="n">
+        <v>76.5</v>
+      </c>
+      <c r="Y162" s="21" t="n">
+        <v>654</v>
+      </c>
+      <c r="Z162" s="22" t="n">
+        <v>85</v>
+      </c>
+      <c r="AA162" s="24" t="n">
+        <v>1297</v>
+      </c>
+      <c r="AB162" s="22" t="n">
+        <v>63.6</v>
+      </c>
+      <c r="AC162" s="24" t="n">
+        <v>1181</v>
+      </c>
+      <c r="AD162" s="22" t="n">
+        <v>65.59999999999999</v>
+      </c>
+      <c r="AE162" s="24" t="n">
+        <v>1234</v>
+      </c>
+      <c r="AF162" s="22" t="n">
+        <v>64.3</v>
+      </c>
+      <c r="AG162" s="25" t="n">
+        <v>2048</v>
+      </c>
+      <c r="AH162" s="22" t="n">
+        <v>39.3</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B163" s="18" t="inlineStr">
+        <is>
+          <t>xiaozhi1</t>
+        </is>
+      </c>
+      <c r="C163" s="5" t="n">
+        <v>139</v>
+      </c>
+      <c r="D163" s="19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="J163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="N163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="P163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="R163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="V163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="X163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="Z163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="AB163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC163" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="AD163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE163" s="20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AF163" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG163" s="25" t="n">
+        <v>1710</v>
+      </c>
+      <c r="AH163" s="20" t="n">
+        <v>46.9</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B164" s="1" t="inlineStr">
+        <is>
+          <t>xxnzym</t>
+        </is>
+      </c>
+      <c r="C164" s="11" t="n">
+        <v>66</v>
+      </c>
+      <c r="D164" s="19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E164" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F164" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G164" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H164" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I164" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="J164" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K164" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L164" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M164" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="N164" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O164" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="P164" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q164" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="R164" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="S164" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T164" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U164" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="V164" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="W164" s="25" t="n">
+        <v>1799</v>
+      </c>
+      <c r="X164" s="22" t="n">
+        <v>43.5</v>
+      </c>
+      <c r="Y164" s="21" t="n">
+        <v>404</v>
+      </c>
+      <c r="Z164" s="22" t="n">
+        <v>90.7</v>
+      </c>
+      <c r="AA164" s="23" t="n">
+        <v>629</v>
+      </c>
+      <c r="AB164" s="22" t="n">
+        <v>82.2</v>
+      </c>
+      <c r="AC164" s="24" t="n">
+        <v>1612</v>
+      </c>
+      <c r="AD164" s="22" t="n">
+        <v>56.7</v>
+      </c>
+      <c r="AE164" s="23" t="n">
+        <v>477</v>
+      </c>
+      <c r="AF164" s="22" t="n">
+        <v>85.09999999999999</v>
+      </c>
+      <c r="AG164" s="24" t="n">
+        <v>1153</v>
+      </c>
+      <c r="AH164" s="22" t="n">
+        <v>64.3</v>
+      </c>
+      <c r="AI164" s="9" t="inlineStr">
+        <is>
+          <t>Microsoft-Logo</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B165" s="18" t="inlineStr">
+        <is>
+          <t>yexiaoxiao2102</t>
+        </is>
+      </c>
+      <c r="C165" s="5" t="n">
+        <v>60</v>
+      </c>
+      <c r="D165" s="19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E165" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F165" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G165" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H165" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I165" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="J165" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K165" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L165" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M165" s="20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="N165" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O165" s="21" t="n">
+        <v>441</v>
+      </c>
+      <c r="P165" s="20" t="n">
+        <v>91.3</v>
+      </c>
+      <c r="Q165" s="23" t="n">
+        <v>773</v>
+      </c>
+      <c r="R165" s="20" t="n">
+        <v>81.5</v>
+      </c>
+      <c r="S165" s="21" t="n">
+        <v>225</v>
+      </c>
+      <c r="T165" s="20" t="n">
+        <v>95.8</v>
+      </c>
+      <c r="U165" s="24" t="n">
+        <v>1256</v>
+      </c>
+      <c r="V165" s="20" t="n">
+        <v>65.90000000000001</v>
+      </c>
+      <c r="W165" s="20" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X165" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y165" s="24" t="n">
+        <v>1344</v>
+      </c>
+      <c r="Z165" s="20" t="n">
+        <v>59.1</v>
+      </c>
+      <c r="AA165" s="23" t="n">
+        <v>541</v>
+      </c>
+      <c r="AB165" s="20" t="n">
+        <v>84</v>
+      </c>
+      <c r="AC165" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AD165" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE165" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AF165" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG165" s="20" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AH165" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI165" s="9" t="inlineStr">
+        <is>
+          <t>Google-Logo</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B166" s="1" t="inlineStr">
+        <is>
+          <t>yykfight</t>
+        </is>
+      </c>
+      <c r="C166" s="11" t="n">
+        <v>184</v>
+      </c>
+      <c r="D166" s="19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E166" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F166" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G166" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H166" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I166" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="J166" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K166" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L166" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M166" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="N166" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="O166" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="P166" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q166" s="25" t="n">
+        <v>2517</v>
+      </c>
+      <c r="R166" s="22" t="n">
+        <v>40.9</v>
+      </c>
+      <c r="S166" s="22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="T166" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="U166" s="24" t="n">
+        <v>1315</v>
+      </c>
+      <c r="V166" s="22" t="n">
+        <v>64.8</v>
+      </c>
+      <c r="W166" s="24" t="n">
+        <v>957</v>
+      </c>
+      <c r="X166" s="22" t="n">
+        <v>67.90000000000001</v>
+      </c>
+      <c r="Y166" s="21" t="n">
+        <v>741</v>
+      </c>
+      <c r="Z166" s="22" t="n">
+        <v>83</v>
+      </c>
+      <c r="AA166" s="22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AB166" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC166" s="24" t="n">
+        <v>2034</v>
+      </c>
+      <c r="AD166" s="22" t="n">
+        <v>48</v>
+      </c>
+      <c r="AE166" s="23" t="n">
+        <v>914</v>
+      </c>
+      <c r="AF166" s="22" t="n">
+        <v>76</v>
+      </c>
+      <c r="AG166" s="24" t="n">
+        <v>995</v>
+      </c>
+      <c r="AH166" s="22" t="n">
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="18" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B167" s="18" t="inlineStr">
+        <is>
+          <t>z3493021</t>
+        </is>
+      </c>
+      <c r="C167" s="5" t="n">
+        <v>42</v>
+      </c>
+      <c r="D167" s="19" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="J167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="K167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="L167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="M167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="N167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="P167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="R167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="S167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="T167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="U167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="V167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="W167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="X167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="Z167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="AB167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="AD167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="AF167" s="20" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG167" s="20" t="n">
+        <v>-3</v>
+      </c>
+      <c r="AH167" s="20" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="1" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B168" s="1" t="inlineStr">
+        <is>
           <t>zhangsikai123</t>
         </is>
       </c>
-      <c r="C160" s="11" t="n">
+      <c r="C168" s="11" t="n">
         <v>165</v>
       </c>
-      <c r="D160" s="19" t="inlineStr">
+      <c r="D168" s="19" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="E160" s="22" t="n">
-        <v>-3</v>
-      </c>
-      <c r="F160" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="G160" s="22" t="n">
-        <v>-3</v>
-      </c>
-      <c r="H160" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="I160" s="22" t="n">
-        <v>-3</v>
-      </c>
-      <c r="J160" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="K160" s="22" t="n">
-        <v>-1</v>
-      </c>
-      <c r="L160" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="M160" s="25" t="n">
+      <c r="E168" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="F168" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G168" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="H168" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I168" s="22" t="n">
+        <v>-3</v>
+      </c>
+      <c r="J168" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="K168" s="22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="L168" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="M168" s="25" t="n">
         <v>3004</v>
       </c>
-      <c r="N160" s="22" t="n">
+      <c r="N168" s="22" t="n">
         <v>38.5</v>
       </c>
-      <c r="O160" s="24" t="n">
+      <c r="O168" s="24" t="n">
         <v>2495</v>
       </c>
-      <c r="P160" s="22" t="n">
+      <c r="P168" s="22" t="n">
         <v>41</v>
       </c>
-      <c r="Q160" s="23" t="n">
+      <c r="Q168" s="23" t="n">
         <v>1128</v>
       </c>
-      <c r="R160" s="22" t="n">
+      <c r="R168" s="22" t="n">
         <v>75.2</v>
       </c>
-      <c r="S160" s="24" t="n">
+      <c r="S168" s="24" t="n">
         <v>2266</v>
       </c>
-      <c r="T160" s="22" t="n">
+      <c r="T168" s="22" t="n">
         <v>47.7</v>
       </c>
-      <c r="U160" s="25" t="n">
+      <c r="U168" s="25" t="n">
         <v>2338</v>
       </c>
-      <c r="V160" s="22" t="n">
+      <c r="V168" s="22" t="n">
         <v>40.2</v>
       </c>
-      <c r="W160" s="22" t="n">
-        <v>-1</v>
-      </c>
-      <c r="X160" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y160" s="25" t="n">
+      <c r="W168" s="22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="X168" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y168" s="25" t="n">
         <v>2316</v>
       </c>
-      <c r="Z160" s="22" t="n">
+      <c r="Z168" s="22" t="n">
         <v>31.8</v>
       </c>
-      <c r="AA160" s="25" t="n">
+      <c r="AA168" s="25" t="n">
         <v>1778</v>
       </c>
-      <c r="AB160" s="22" t="n">
+      <c r="AB168" s="22" t="n">
         <v>48.8</v>
       </c>
-      <c r="AC160" s="23" t="n">
+      <c r="AC168" s="23" t="n">
         <v>986</v>
       </c>
-      <c r="AD160" s="22" t="n">
+      <c r="AD168" s="22" t="n">
         <v>74.59999999999999</v>
       </c>
-      <c r="AE160" s="22" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AF160" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG160" s="25" t="n">
+      <c r="AE168" s="22" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AF168" s="22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG168" s="25" t="n">
         <v>1537</v>
       </c>
-      <c r="AH160" s="22" t="n">
+      <c r="AH168" s="22" t="n">
         <v>50.7</v>
       </c>
-      <c r="AI160" s="9" t="inlineStr">
+      <c r="AI168" s="9" t="inlineStr">
         <is>
           <t>RedBook-Logo</t>
         </is>
@@ -16082,6 +16967,14 @@
     <hyperlink ref="B158" r:id="rId141"/>
     <hyperlink ref="B159" r:id="rId142"/>
     <hyperlink ref="B160" r:id="rId143"/>
+    <hyperlink ref="B161" r:id="rId144"/>
+    <hyperlink ref="B162" r:id="rId145"/>
+    <hyperlink ref="B163" r:id="rId146"/>
+    <hyperlink ref="B164" r:id="rId147"/>
+    <hyperlink ref="B165" r:id="rId148"/>
+    <hyperlink ref="B166" r:id="rId149"/>
+    <hyperlink ref="B167" r:id="rId150"/>
+    <hyperlink ref="B168" r:id="rId151"/>
   </hyperlinks>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>

<commit_message>
update Ansonluo and curve
</commit_message>
<xml_diff>
--- a/generateEXCEL/index.xlsx
+++ b/generateEXCEL/index.xlsx
@@ -272,7 +272,7 @@
     <t>ellaliu</t>
   </si>
   <si>
-    <t>Ansonluo1</t>
+    <t>Ansonluo</t>
   </si>
   <si>
     <t>MaggieZhao95</t>
@@ -9527,11 +9527,11 @@
       <c r="X71" s="14" t="n">
         <v>84.59999999999999</v>
       </c>
-      <c r="Y71" s="7" t="n">
+      <c r="Y71" s="13" t="n">
         <v>1778</v>
       </c>
       <c r="Z71" s="14" t="n">
-        <v>61.8</v>
+        <v>56.8</v>
       </c>
       <c r="AA71" s="13" t="n">
         <v>1133</v>
@@ -19231,7 +19231,7 @@
         <v>184</v>
       </c>
       <c r="C167" s="5" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D167" s="19" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
add new members' records
</commit_message>
<xml_diff>
--- a/generateEXCEL/index.xlsx
+++ b/generateEXCEL/index.xlsx
@@ -638,7 +638,7 @@
         </is>
       </c>
       <c r="C4" s="5" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D4" s="6" t="n">
         <v>99.5</v>
@@ -791,7 +791,7 @@
         </is>
       </c>
       <c r="C5" s="13" t="n">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="D5" s="6" t="n">
         <v>99.3</v>
@@ -944,7 +944,7 @@
         </is>
       </c>
       <c r="C6" s="5" t="n">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D6" s="6" t="n">
         <v>99</v>
@@ -1097,7 +1097,7 @@
         </is>
       </c>
       <c r="C7" s="13" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D7" s="6" t="n">
         <v>98.8</v>
@@ -1245,7 +1245,7 @@
         </is>
       </c>
       <c r="C8" s="5" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D8" s="6" t="n">
         <v>98.5</v>
@@ -1393,7 +1393,7 @@
         </is>
       </c>
       <c r="C9" s="13" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D9" s="6" t="n">
         <v>98.5</v>
@@ -1541,7 +1541,7 @@
         </is>
       </c>
       <c r="C10" s="5" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D10" s="6" t="n">
         <v>97.7</v>
@@ -1694,7 +1694,7 @@
         </is>
       </c>
       <c r="C11" s="13" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D11" s="6" t="n">
         <v>97.59999999999999</v>
@@ -1842,7 +1842,7 @@
         </is>
       </c>
       <c r="C12" s="5" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12" s="6" t="n">
         <v>97.3</v>
@@ -1990,7 +1990,7 @@
         </is>
       </c>
       <c r="C13" s="13" t="n">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D13" s="6" t="n">
         <v>97.09999999999999</v>
@@ -2143,7 +2143,7 @@
         </is>
       </c>
       <c r="C14" s="5" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D14" s="6" t="n">
         <v>96.90000000000001</v>
@@ -2291,7 +2291,7 @@
         </is>
       </c>
       <c r="C15" s="13" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D15" s="6" t="n">
         <v>96.90000000000001</v>
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="C16" s="5" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D16" s="6" t="n">
         <v>95.7</v>
@@ -2592,7 +2592,7 @@
         </is>
       </c>
       <c r="C17" s="13" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D17" s="6" t="n">
         <v>95.2</v>
@@ -2740,7 +2740,7 @@
         </is>
       </c>
       <c r="C18" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D18" s="6" t="n">
         <v>94.8</v>
@@ -2888,7 +2888,7 @@
         </is>
       </c>
       <c r="C19" s="13" t="n">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D19" s="6" t="n">
         <v>94.40000000000001</v>
@@ -3041,7 +3041,7 @@
         </is>
       </c>
       <c r="C20" s="5" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D20" s="6" t="n">
         <v>94.09999999999999</v>
@@ -3189,7 +3189,7 @@
         </is>
       </c>
       <c r="C21" s="13" t="n">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D21" s="6" t="n">
         <v>94.09999999999999</v>
@@ -3337,7 +3337,7 @@
         </is>
       </c>
       <c r="C22" s="5" t="n">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="D22" s="6" t="n">
         <v>93.7</v>
@@ -3485,7 +3485,7 @@
         </is>
       </c>
       <c r="C23" s="13" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D23" s="6" t="n">
         <v>93.5</v>
@@ -3638,7 +3638,7 @@
         </is>
       </c>
       <c r="C24" s="5" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D24" s="6" t="n">
         <v>93.09999999999999</v>
@@ -3786,7 +3786,7 @@
         </is>
       </c>
       <c r="C25" s="13" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D25" s="6" t="n">
         <v>92.90000000000001</v>
@@ -3939,7 +3939,7 @@
         </is>
       </c>
       <c r="C26" s="5" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D26" s="6" t="n">
         <v>92.7</v>
@@ -4092,7 +4092,7 @@
         </is>
       </c>
       <c r="C27" s="13" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D27" s="6" t="n">
         <v>92.40000000000001</v>
@@ -4240,7 +4240,7 @@
         </is>
       </c>
       <c r="C28" s="5" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D28" s="6" t="n">
         <v>92</v>
@@ -4388,7 +4388,7 @@
         </is>
       </c>
       <c r="C29" s="13" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D29" s="6" t="n">
         <v>91.90000000000001</v>
@@ -4536,7 +4536,7 @@
         </is>
       </c>
       <c r="C30" s="5" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D30" s="6" t="n">
         <v>91.5</v>
@@ -4684,7 +4684,7 @@
         </is>
       </c>
       <c r="C31" s="13" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D31" s="6" t="n">
         <v>91.40000000000001</v>
@@ -4837,7 +4837,7 @@
         </is>
       </c>
       <c r="C32" s="5" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D32" s="6" t="n">
         <v>90.59999999999999</v>
@@ -4985,7 +4985,7 @@
         </is>
       </c>
       <c r="C33" s="13" t="n">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D33" s="6" t="n">
         <v>90.09999999999999</v>
@@ -5133,7 +5133,7 @@
         </is>
       </c>
       <c r="C34" s="5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D34" s="6" t="n">
         <v>89.7</v>
@@ -5281,7 +5281,7 @@
         </is>
       </c>
       <c r="C35" s="13" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D35" s="6" t="n">
         <v>89.2</v>
@@ -5429,7 +5429,7 @@
         </is>
       </c>
       <c r="C36" s="5" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D36" s="6" t="n">
         <v>89.2</v>
@@ -5577,7 +5577,7 @@
         </is>
       </c>
       <c r="C37" s="13" t="n">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D37" s="6" t="n">
         <v>89.09999999999999</v>
@@ -5725,7 +5725,7 @@
         </is>
       </c>
       <c r="C38" s="5" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D38" s="6" t="n">
         <v>88.90000000000001</v>
@@ -5873,7 +5873,7 @@
         </is>
       </c>
       <c r="C39" s="13" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D39" s="6" t="n">
         <v>88.8</v>
@@ -6026,7 +6026,7 @@
         </is>
       </c>
       <c r="C40" s="5" t="n">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D40" s="6" t="n">
         <v>87.59999999999999</v>
@@ -6174,7 +6174,7 @@
         </is>
       </c>
       <c r="C41" s="13" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D41" s="6" t="n">
         <v>86.5</v>
@@ -6322,7 +6322,7 @@
         </is>
       </c>
       <c r="C42" s="5" t="n">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="D42" s="6" t="n">
         <v>86</v>
@@ -6475,7 +6475,7 @@
         </is>
       </c>
       <c r="C43" s="13" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D43" s="6" t="n">
         <v>85.7</v>
@@ -6623,7 +6623,7 @@
         </is>
       </c>
       <c r="C44" s="5" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D44" s="6" t="n">
         <v>85.59999999999999</v>
@@ -6776,7 +6776,7 @@
         </is>
       </c>
       <c r="C45" s="13" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D45" s="6" t="n">
         <v>85.5</v>
@@ -6924,7 +6924,7 @@
         </is>
       </c>
       <c r="C46" s="5" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D46" s="6" t="n">
         <v>83.2</v>
@@ -7072,7 +7072,7 @@
         </is>
       </c>
       <c r="C47" s="13" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D47" s="6" t="n">
         <v>82.5</v>
@@ -7220,7 +7220,7 @@
         </is>
       </c>
       <c r="C48" s="5" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D48" s="6" t="n">
         <v>81.3</v>
@@ -7368,7 +7368,7 @@
         </is>
       </c>
       <c r="C49" s="13" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D49" s="6" t="n">
         <v>80.8</v>
@@ -7516,7 +7516,7 @@
         </is>
       </c>
       <c r="C50" s="5" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D50" s="6" t="n">
         <v>80.2</v>
@@ -7664,7 +7664,7 @@
         </is>
       </c>
       <c r="C51" s="13" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D51" s="6" t="n">
         <v>79.8</v>
@@ -7817,7 +7817,7 @@
         </is>
       </c>
       <c r="C52" s="5" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D52" s="6" t="n">
         <v>78.40000000000001</v>
@@ -7970,7 +7970,7 @@
         </is>
       </c>
       <c r="C53" s="13" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="D53" s="6" t="n">
         <v>78</v>
@@ -8118,7 +8118,7 @@
         </is>
       </c>
       <c r="C54" s="5" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D54" s="6" t="n">
         <v>77.8</v>
@@ -8266,7 +8266,7 @@
         </is>
       </c>
       <c r="C55" s="13" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D55" s="6" t="n">
         <v>77.8</v>
@@ -8419,7 +8419,7 @@
         </is>
       </c>
       <c r="C56" s="5" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D56" s="6" t="n">
         <v>73.40000000000001</v>
@@ -8567,7 +8567,7 @@
         </is>
       </c>
       <c r="C57" s="13" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D57" s="6" t="n">
         <v>72.8</v>
@@ -8715,7 +8715,7 @@
         </is>
       </c>
       <c r="C58" s="5" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D58" s="6" t="n">
         <v>71.5</v>
@@ -8863,7 +8863,7 @@
         </is>
       </c>
       <c r="C59" s="13" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D59" s="6" t="n">
         <v>71.2</v>
@@ -9011,7 +9011,7 @@
         </is>
       </c>
       <c r="C60" s="5" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D60" s="6" t="n">
         <v>69.7</v>
@@ -9159,7 +9159,7 @@
         </is>
       </c>
       <c r="C61" s="13" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D61" s="6" t="n">
         <v>68.8</v>
@@ -9307,7 +9307,7 @@
         </is>
       </c>
       <c r="C62" s="5" t="n">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D62" s="6" t="n">
         <v>68.2</v>
@@ -9455,7 +9455,7 @@
         </is>
       </c>
       <c r="C63" s="13" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D63" s="6" t="n">
         <v>68.09999999999999</v>
@@ -9761,7 +9761,7 @@
         </is>
       </c>
       <c r="C65" s="13" t="n">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D65" s="6" t="n">
         <v>65.5</v>
@@ -9909,7 +9909,7 @@
         </is>
       </c>
       <c r="C66" s="5" t="n">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="D66" s="6" t="n">
         <v>64.8</v>
@@ -10205,7 +10205,7 @@
         </is>
       </c>
       <c r="C68" s="5" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D68" s="6" t="n">
         <v>63</v>
@@ -10353,7 +10353,7 @@
         </is>
       </c>
       <c r="C69" s="13" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D69" s="6" t="n">
         <v>62.6</v>
@@ -10501,7 +10501,7 @@
         </is>
       </c>
       <c r="C70" s="5" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D70" s="6" t="n">
         <v>62.5</v>
@@ -10649,7 +10649,7 @@
         </is>
       </c>
       <c r="C71" s="13" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D71" s="6" t="n">
         <v>61.3</v>
@@ -10797,7 +10797,7 @@
         </is>
       </c>
       <c r="C72" s="5" t="n">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D72" s="6" t="n">
         <v>60</v>
@@ -10945,7 +10945,7 @@
         </is>
       </c>
       <c r="C73" s="13" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D73" s="6" t="n">
         <v>59.8</v>
@@ -11093,7 +11093,7 @@
         </is>
       </c>
       <c r="C74" s="5" t="n">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D74" s="6" t="n">
         <v>58.6</v>
@@ -11246,7 +11246,7 @@
         </is>
       </c>
       <c r="C75" s="13" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D75" s="6" t="n">
         <v>58.6</v>
@@ -11394,7 +11394,7 @@
         </is>
       </c>
       <c r="C76" s="5" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D76" s="6" t="n">
         <v>57.5</v>
@@ -11547,7 +11547,7 @@
         </is>
       </c>
       <c r="C77" s="13" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D77" s="6" t="n">
         <v>56</v>
@@ -11695,7 +11695,7 @@
         </is>
       </c>
       <c r="C78" s="5" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="D78" s="6" t="n">
         <v>52.5</v>
@@ -11843,7 +11843,7 @@
         </is>
       </c>
       <c r="C79" s="13" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D79" s="6" t="n">
         <v>52.3</v>
@@ -11991,7 +11991,7 @@
         </is>
       </c>
       <c r="C80" s="5" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D80" s="6" t="n">
         <v>50.9</v>
@@ -12292,7 +12292,7 @@
         </is>
       </c>
       <c r="C82" s="5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D82" s="6" t="n">
         <v>47.2</v>
@@ -12440,7 +12440,7 @@
         </is>
       </c>
       <c r="C83" s="13" t="n">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D83" s="6" t="n">
         <v>43.5</v>
@@ -12588,7 +12588,7 @@
         </is>
       </c>
       <c r="C84" s="5" t="n">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="D84" s="6" t="n">
         <v>42.7</v>
@@ -12736,7 +12736,7 @@
         </is>
       </c>
       <c r="C85" s="13" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D85" s="6" t="n">
         <v>42.5</v>
@@ -12884,7 +12884,7 @@
         </is>
       </c>
       <c r="C86" s="5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D86" s="6" t="n">
         <v>41.2</v>
@@ -13032,7 +13032,7 @@
         </is>
       </c>
       <c r="C87" s="13" t="n">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D87" s="6" t="n">
         <v>40.3</v>
@@ -13180,7 +13180,7 @@
         </is>
       </c>
       <c r="C88" s="5" t="n">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="D88" s="6" t="n">
         <v>37.9</v>
@@ -13328,7 +13328,7 @@
         </is>
       </c>
       <c r="C89" s="13" t="n">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D89" s="6" t="n">
         <v>36.1</v>
@@ -13481,7 +13481,7 @@
         </is>
       </c>
       <c r="C90" s="5" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D90" s="6" t="n">
         <v>31</v>
@@ -13629,7 +13629,7 @@
         </is>
       </c>
       <c r="C91" s="13" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D91" s="6" t="n">
         <v>29.2</v>
@@ -13777,7 +13777,7 @@
         </is>
       </c>
       <c r="C92" s="5" t="n">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D92" s="6" t="n">
         <v>22.6</v>
@@ -13925,7 +13925,7 @@
         </is>
       </c>
       <c r="C93" s="13" t="n">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D93" s="6" t="n">
         <v>0</v>
@@ -14078,7 +14078,7 @@
         </is>
       </c>
       <c r="C94" s="5" t="n">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="D94" s="6" t="n">
         <v>0</v>
@@ -14226,7 +14226,7 @@
         </is>
       </c>
       <c r="C95" s="13" t="n">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D95" s="6" t="n">
         <v>0</v>
@@ -14519,7 +14519,7 @@
         </is>
       </c>
       <c r="C98" s="5" t="n">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D98" s="6" t="inlineStr">
         <is>
@@ -14619,7 +14619,7 @@
         </is>
       </c>
       <c r="C115" s="5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D115" s="19" t="inlineStr">
         <is>
@@ -15850,7 +15850,7 @@
         </is>
       </c>
       <c r="C123" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D123" s="19" t="inlineStr">
         <is>
@@ -18909,7 +18909,7 @@
       </c>
       <c r="AW142" s="11" t="inlineStr">
         <is>
-          <t>Microsoft-Logo</t>
+          <t>Alibaba-Logo</t>
         </is>
       </c>
     </row>
@@ -18925,7 +18925,7 @@
         </is>
       </c>
       <c r="C143" s="5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D143" s="19" t="inlineStr">
         <is>
@@ -27390,7 +27390,7 @@
         </is>
       </c>
       <c r="C198" s="13" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D198" s="19" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
update rule - split red packet groups
</commit_message>
<xml_diff>
--- a/generateEXCEL/index.xlsx
+++ b/generateEXCEL/index.xlsx
@@ -891,7 +891,7 @@
         </is>
       </c>
       <c r="C12" s="10" t="n">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="D12" s="11" t="n">
         <v>2987</v>
@@ -1228,7 +1228,7 @@
         </is>
       </c>
       <c r="C13" s="17" t="n">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="D13" s="18" t="n">
         <v>3387</v>
@@ -1570,7 +1570,7 @@
         </is>
       </c>
       <c r="C14" s="10" t="n">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c r="D14" s="11" t="n">
         <v>3064</v>
@@ -1907,7 +1907,7 @@
         </is>
       </c>
       <c r="C15" s="17" t="n">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="D15" s="18" t="n">
         <v>2623</v>
@@ -2249,7 +2249,7 @@
         </is>
       </c>
       <c r="C16" s="10" t="n">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="D16" s="11" t="n">
         <v>2946</v>
@@ -2586,7 +2586,7 @@
         </is>
       </c>
       <c r="C17" s="17" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D17" s="18" t="n">
         <v>2684</v>
@@ -2923,7 +2923,7 @@
         </is>
       </c>
       <c r="C18" s="10" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D18" s="11" t="n">
         <v>2694</v>
@@ -3260,7 +3260,7 @@
         </is>
       </c>
       <c r="C19" s="17" t="n">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="D19" s="18" t="n">
         <v>2634</v>
@@ -3597,7 +3597,7 @@
         </is>
       </c>
       <c r="C20" s="10" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D20" s="11" t="n">
         <v>2524</v>
@@ -3934,7 +3934,7 @@
         </is>
       </c>
       <c r="C21" s="17" t="n">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="D21" s="18" t="n">
         <v>2880</v>
@@ -4276,7 +4276,7 @@
         </is>
       </c>
       <c r="C22" s="10" t="n">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D22" s="11" t="n">
         <v>2684</v>
@@ -4613,7 +4613,7 @@
         </is>
       </c>
       <c r="C23" s="17" t="n">
-        <v>1167</v>
+        <v>1170</v>
       </c>
       <c r="D23" s="18" t="n">
         <v>3120</v>
@@ -4955,7 +4955,7 @@
         </is>
       </c>
       <c r="C24" s="10" t="n">
-        <v>733</v>
+        <v>736</v>
       </c>
       <c r="D24" s="11" t="n">
         <v>2498</v>
@@ -5297,7 +5297,7 @@
         </is>
       </c>
       <c r="C25" s="17" t="n">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D25" s="18" t="n">
         <v>2449</v>
@@ -5634,7 +5634,7 @@
         </is>
       </c>
       <c r="C26" s="10" t="n">
-        <v>985</v>
+        <v>988</v>
       </c>
       <c r="D26" s="11" t="n">
         <v>2692</v>
@@ -5976,7 +5976,7 @@
         </is>
       </c>
       <c r="C27" s="17" t="n">
-        <v>858</v>
+        <v>861</v>
       </c>
       <c r="D27" s="18" t="n">
         <v>2860</v>
@@ -6318,7 +6318,7 @@
         </is>
       </c>
       <c r="C28" s="10" t="n">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="D28" s="11" t="n">
         <v>2646</v>
@@ -6660,7 +6660,7 @@
         </is>
       </c>
       <c r="C29" s="17" t="n">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D29" s="18" t="n">
         <v>2372</v>
@@ -6997,7 +6997,7 @@
         </is>
       </c>
       <c r="C30" s="10" t="n">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="D30" s="11" t="n">
         <v>2740</v>
@@ -7334,7 +7334,7 @@
         </is>
       </c>
       <c r="C31" s="17" t="n">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D31" s="18" t="n">
         <v>2586</v>
@@ -7676,7 +7676,7 @@
         </is>
       </c>
       <c r="C32" s="10" t="n">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="D32" s="11" t="n">
         <v>2753</v>
@@ -8013,7 +8013,7 @@
         </is>
       </c>
       <c r="C33" s="17" t="n">
-        <v>881</v>
+        <v>884</v>
       </c>
       <c r="D33" s="18" t="n">
         <v>2516</v>
@@ -8355,7 +8355,7 @@
         </is>
       </c>
       <c r="C34" s="10" t="n">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="D34" s="11" t="n">
         <v>2454</v>
@@ -8697,7 +8697,7 @@
         </is>
       </c>
       <c r="C35" s="17" t="n">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D35" s="18" t="n">
         <v>2305</v>
@@ -9039,7 +9039,7 @@
         </is>
       </c>
       <c r="C36" s="10" t="n">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="D36" s="11" t="n">
         <v>2368</v>
@@ -9376,7 +9376,7 @@
         </is>
       </c>
       <c r="C37" s="17" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D37" s="18" t="n">
         <v>2310</v>
@@ -9713,7 +9713,7 @@
         </is>
       </c>
       <c r="C38" s="10" t="n">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="D38" s="11" t="n">
         <v>2460</v>
@@ -10055,7 +10055,7 @@
         </is>
       </c>
       <c r="C39" s="17" t="n">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="D39" s="18" t="n">
         <v>2380</v>
@@ -10397,7 +10397,7 @@
         </is>
       </c>
       <c r="C40" s="10" t="n">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="D40" s="11" t="n">
         <v>2370</v>
@@ -10739,7 +10739,7 @@
         </is>
       </c>
       <c r="C41" s="17" t="n">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="D41" s="18" t="n">
         <v>2611</v>
@@ -11081,7 +11081,7 @@
         </is>
       </c>
       <c r="C42" s="10" t="n">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="D42" s="11" t="n">
         <v>2399</v>
@@ -11423,7 +11423,7 @@
         </is>
       </c>
       <c r="C43" s="17" t="n">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="D43" s="18" t="n">
         <v>2728</v>
@@ -11760,7 +11760,7 @@
         </is>
       </c>
       <c r="C44" s="10" t="n">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="D44" s="11" t="n">
         <v>2301</v>
@@ -12102,7 +12102,7 @@
         </is>
       </c>
       <c r="C45" s="17" t="n">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="D45" s="18" t="n">
         <v>2247</v>
@@ -12439,7 +12439,7 @@
         </is>
       </c>
       <c r="C46" s="10" t="n">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="D46" s="11" t="n">
         <v>2501</v>
@@ -12776,7 +12776,7 @@
         </is>
       </c>
       <c r="C47" s="17" t="n">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D47" s="18" t="n">
         <v>2338</v>
@@ -13118,7 +13118,7 @@
         </is>
       </c>
       <c r="C48" s="10" t="n">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D48" s="11" t="n">
         <v>2369</v>
@@ -13460,7 +13460,7 @@
         </is>
       </c>
       <c r="C49" s="17" t="n">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="D49" s="18" t="n">
         <v>2688</v>
@@ -13797,7 +13797,7 @@
         </is>
       </c>
       <c r="C50" s="10" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D50" s="11" t="n">
         <v>2747</v>
@@ -14134,7 +14134,7 @@
         </is>
       </c>
       <c r="C51" s="17" t="n">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="D51" s="18" t="n">
         <v>2297</v>
@@ -14471,7 +14471,7 @@
         </is>
       </c>
       <c r="C52" s="10" t="n">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="D52" s="11" t="n">
         <v>2291</v>
@@ -14808,7 +14808,7 @@
         </is>
       </c>
       <c r="C53" s="17" t="n">
-        <v>1109</v>
+        <v>1112</v>
       </c>
       <c r="D53" s="18" t="n">
         <v>2221</v>
@@ -15150,7 +15150,7 @@
         </is>
       </c>
       <c r="C54" s="10" t="n">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="D54" s="11" t="n">
         <v>2379</v>
@@ -15492,7 +15492,7 @@
         </is>
       </c>
       <c r="C55" s="17" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D55" s="18" t="n">
         <v>2383</v>
@@ -15829,7 +15829,7 @@
         </is>
       </c>
       <c r="C56" s="10" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D56" s="11" t="n">
         <v>2331</v>
@@ -16166,7 +16166,7 @@
         </is>
       </c>
       <c r="C57" s="17" t="n">
-        <v>986</v>
+        <v>989</v>
       </c>
       <c r="D57" s="18" t="n">
         <v>2185</v>
@@ -16503,7 +16503,7 @@
         </is>
       </c>
       <c r="C58" s="10" t="n">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D58" s="11" t="n">
         <v>2242</v>
@@ -16840,7 +16840,7 @@
         </is>
       </c>
       <c r="C59" s="17" t="n">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="D59" s="18" t="n">
         <v>2410</v>
@@ -17182,7 +17182,7 @@
         </is>
       </c>
       <c r="C60" s="10" t="n">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D60" s="22" t="n">
         <v>2026</v>
@@ -17519,7 +17519,7 @@
         </is>
       </c>
       <c r="C61" s="17" t="n">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D61" s="18" t="n">
         <v>2196</v>
@@ -17856,7 +17856,7 @@
         </is>
       </c>
       <c r="C62" s="10" t="n">
-        <v>1035</v>
+        <v>1038</v>
       </c>
       <c r="D62" s="11" t="n">
         <v>2378</v>
@@ -18193,7 +18193,7 @@
         </is>
       </c>
       <c r="C63" s="17" t="n">
-        <v>872</v>
+        <v>875</v>
       </c>
       <c r="D63" s="18" t="n">
         <v>2329</v>
@@ -18530,7 +18530,7 @@
         </is>
       </c>
       <c r="C64" s="10" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D64" s="11" t="n">
         <v>2275</v>
@@ -18867,7 +18867,7 @@
         </is>
       </c>
       <c r="C65" s="17" t="n">
-        <v>1217</v>
+        <v>1220</v>
       </c>
       <c r="D65" s="18" t="n">
         <v>2417</v>
@@ -19209,7 +19209,7 @@
         </is>
       </c>
       <c r="C66" s="10" t="n">
-        <v>904</v>
+        <v>907</v>
       </c>
       <c r="D66" s="11" t="n">
         <v>2152</v>
@@ -19551,7 +19551,7 @@
         </is>
       </c>
       <c r="C67" s="17" t="n">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D67" s="18" t="n">
         <v>2447</v>
@@ -19888,7 +19888,7 @@
         </is>
       </c>
       <c r="C68" s="10" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D68" s="22" t="n">
         <v>2098</v>
@@ -20230,7 +20230,7 @@
         </is>
       </c>
       <c r="C69" s="17" t="n">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D69" s="18" t="n">
         <v>2289</v>
@@ -20572,7 +20572,7 @@
         </is>
       </c>
       <c r="C70" s="10" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D70" s="11" t="n">
         <v>2282</v>
@@ -20909,7 +20909,7 @@
         </is>
       </c>
       <c r="C71" s="17" t="n">
-        <v>844</v>
+        <v>847</v>
       </c>
       <c r="D71" s="18" t="n">
         <v>2200</v>
@@ -21251,7 +21251,7 @@
         </is>
       </c>
       <c r="C72" s="10" t="n">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D72" s="11" t="n">
         <v>2130</v>
@@ -21588,7 +21588,7 @@
         </is>
       </c>
       <c r="C73" s="17" t="n">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="D73" s="18" t="n">
         <v>2491</v>
@@ -21925,7 +21925,7 @@
         </is>
       </c>
       <c r="C74" s="10" t="n">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="D74" s="22" t="n">
         <v>2080</v>
@@ -22262,7 +22262,7 @@
         </is>
       </c>
       <c r="C75" s="17" t="n">
-        <v>1211</v>
+        <v>1214</v>
       </c>
       <c r="D75" s="18" t="n">
         <v>2710</v>
@@ -22604,7 +22604,7 @@
         </is>
       </c>
       <c r="C76" s="10" t="n">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="D76" s="11" t="n">
         <v>2335</v>
@@ -22946,7 +22946,7 @@
         </is>
       </c>
       <c r="C77" s="17" t="n">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="D77" s="18" t="n">
         <v>2260</v>
@@ -23288,7 +23288,7 @@
         </is>
       </c>
       <c r="C78" s="10" t="n">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D78" s="11" t="n">
         <v>2326</v>
@@ -23625,7 +23625,7 @@
         </is>
       </c>
       <c r="C79" s="17" t="n">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="D79" s="18" t="n">
         <v>2326</v>
@@ -23962,7 +23962,7 @@
         </is>
       </c>
       <c r="C80" s="10" t="n">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="D80" s="11" t="n">
         <v>2365</v>
@@ -24304,7 +24304,7 @@
         </is>
       </c>
       <c r="C81" s="17" t="n">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D81" s="23" t="n">
         <v>2040</v>
@@ -24646,7 +24646,7 @@
         </is>
       </c>
       <c r="C82" s="10" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D82" s="22" t="n">
         <v>1955</v>
@@ -24983,7 +24983,7 @@
         </is>
       </c>
       <c r="C83" s="17" t="n">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D83" s="23" t="n">
         <v>2066</v>
@@ -25325,7 +25325,7 @@
         </is>
       </c>
       <c r="C84" s="10" t="n">
-        <v>1217</v>
+        <v>1220</v>
       </c>
       <c r="D84" s="22" t="n">
         <v>2089</v>
@@ -25667,7 +25667,7 @@
         </is>
       </c>
       <c r="C85" s="17" t="n">
-        <v>805</v>
+        <v>808</v>
       </c>
       <c r="D85" s="18" t="n">
         <v>2308</v>
@@ -26009,7 +26009,7 @@
         </is>
       </c>
       <c r="C86" s="10" t="n">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D86" s="22" t="n">
         <v>1865</v>
@@ -26346,7 +26346,7 @@
         </is>
       </c>
       <c r="C87" s="17" t="n">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="D87" s="18" t="n">
         <v>2710</v>
@@ -26688,7 +26688,7 @@
         </is>
       </c>
       <c r="C88" s="10" t="n">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="D88" s="11" t="n">
         <v>2212</v>
@@ -27030,7 +27030,7 @@
         </is>
       </c>
       <c r="C89" s="17" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D89" s="23" t="n">
         <v>1919</v>
@@ -27367,7 +27367,7 @@
         </is>
       </c>
       <c r="C90" s="10" t="n">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="D90" s="22" t="n">
         <v>1884</v>
@@ -27704,7 +27704,7 @@
         </is>
       </c>
       <c r="C91" s="17" t="n">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="D91" s="18" t="n">
         <v>2134</v>
@@ -28046,7 +28046,7 @@
         </is>
       </c>
       <c r="C92" s="10" t="n">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D92" s="22" t="n">
         <v>1922</v>
@@ -28383,7 +28383,7 @@
         </is>
       </c>
       <c r="C93" s="17" t="n">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="D93" s="18" t="n">
         <v>2279</v>
@@ -28720,7 +28720,7 @@
         </is>
       </c>
       <c r="C94" s="10" t="n">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D94" s="22" t="n">
         <v>1880</v>
@@ -29057,7 +29057,7 @@
         </is>
       </c>
       <c r="C95" s="17" t="n">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D95" s="23" t="n">
         <v>2091</v>
@@ -29399,7 +29399,7 @@
         </is>
       </c>
       <c r="C96" s="10" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D96" s="22" t="n">
         <v>2021</v>
@@ -29736,7 +29736,7 @@
         </is>
       </c>
       <c r="C97" s="17" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D97" s="23" t="n">
         <v>1968</v>
@@ -30073,7 +30073,7 @@
         </is>
       </c>
       <c r="C98" s="10" t="n">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D98" s="11" t="n">
         <v>2327</v>
@@ -30415,7 +30415,7 @@
         </is>
       </c>
       <c r="C99" s="17" t="n">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="D99" s="18" t="n">
         <v>2367</v>
@@ -30757,7 +30757,7 @@
         </is>
       </c>
       <c r="C100" s="10" t="n">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D100" s="22" t="n">
         <v>1908</v>
@@ -31094,7 +31094,7 @@
         </is>
       </c>
       <c r="C101" s="17" t="n">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="D101" s="18" t="n">
         <v>2237</v>
@@ -31436,7 +31436,7 @@
         </is>
       </c>
       <c r="C102" s="10" t="n">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="D102" s="22" t="n">
         <v>1920</v>
@@ -31773,7 +31773,7 @@
         </is>
       </c>
       <c r="C103" s="17" t="n">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D103" s="23" t="n">
         <v>2069</v>
@@ -32110,7 +32110,7 @@
         </is>
       </c>
       <c r="C104" s="10" t="n">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="D104" s="11" t="n">
         <v>2167</v>
@@ -32452,7 +32452,7 @@
         </is>
       </c>
       <c r="C105" s="17" t="n">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D105" s="23" t="n">
         <v>2090</v>
@@ -32789,7 +32789,7 @@
         </is>
       </c>
       <c r="C106" s="10" t="n">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D106" s="22" t="n">
         <v>1790</v>
@@ -33131,7 +33131,7 @@
         </is>
       </c>
       <c r="C107" s="17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D107" s="18" t="n">
         <v>2116</v>
@@ -33468,7 +33468,7 @@
         </is>
       </c>
       <c r="C108" s="10" t="n">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D108" s="22" t="n">
         <v>2067</v>
@@ -33810,7 +33810,7 @@
         </is>
       </c>
       <c r="C109" s="17" t="n">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="D109" s="23" t="n">
         <v>2098</v>
@@ -34147,7 +34147,7 @@
         </is>
       </c>
       <c r="C110" s="10" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D110" s="22" t="n">
         <v>1926</v>
@@ -34484,7 +34484,7 @@
         </is>
       </c>
       <c r="C111" s="17" t="n">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="D111" s="23" t="n">
         <v>1940</v>
@@ -34821,7 +34821,7 @@
         </is>
       </c>
       <c r="C112" s="10" t="n">
-        <v>942</v>
+        <v>945</v>
       </c>
       <c r="D112" s="22" t="n">
         <v>2071</v>
@@ -35163,7 +35163,7 @@
         </is>
       </c>
       <c r="C113" s="17" t="n">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D113" s="23" t="n">
         <v>2011</v>
@@ -35500,7 +35500,7 @@
         </is>
       </c>
       <c r="C114" s="10" t="n">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D114" s="22" t="n">
         <v>1955</v>
@@ -35837,7 +35837,7 @@
         </is>
       </c>
       <c r="C115" s="17" t="n">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="D115" s="23" t="n">
         <v>2094</v>
@@ -36174,7 +36174,7 @@
         </is>
       </c>
       <c r="C116" s="10" t="n">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D116" s="22" t="n">
         <v>1875</v>
@@ -36511,7 +36511,7 @@
         </is>
       </c>
       <c r="C117" s="17" t="n">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="D117" s="23" t="n">
         <v>2020</v>
@@ -36848,7 +36848,7 @@
         </is>
       </c>
       <c r="C118" s="10" t="n">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="D118" s="11" t="n">
         <v>2154</v>
@@ -37185,7 +37185,7 @@
         </is>
       </c>
       <c r="C119" s="17" t="n">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="D119" s="23" t="n">
         <v>2003</v>
@@ -37522,7 +37522,7 @@
         </is>
       </c>
       <c r="C120" s="10" t="n">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="D120" s="22" t="n">
         <v>1996</v>
@@ -37859,7 +37859,7 @@
         </is>
       </c>
       <c r="C121" s="17" t="n">
-        <v>942</v>
+        <v>945</v>
       </c>
       <c r="D121" s="23" t="n">
         <v>1980</v>
@@ -38196,7 +38196,7 @@
         </is>
       </c>
       <c r="C122" s="10" t="n">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D122" s="22" t="n">
         <v>1923</v>
@@ -38533,7 +38533,7 @@
         </is>
       </c>
       <c r="C123" s="17" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D123" s="23" t="n">
         <v>1790</v>
@@ -38870,7 +38870,7 @@
         </is>
       </c>
       <c r="C124" s="10" t="n">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D124" s="11" t="n">
         <v>2292</v>
@@ -39207,7 +39207,7 @@
         </is>
       </c>
       <c r="C125" s="17" t="n">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="D125" s="18" t="n">
         <v>2109</v>
@@ -39544,7 +39544,7 @@
         </is>
       </c>
       <c r="C126" s="10" t="n">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D126" s="22" t="n">
         <v>1897</v>
@@ -39881,7 +39881,7 @@
         </is>
       </c>
       <c r="C127" s="17" t="n">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="D127" s="23" t="n">
         <v>2059</v>
@@ -40223,7 +40223,7 @@
         </is>
       </c>
       <c r="C128" s="10" t="n">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D128" s="22" t="n">
         <v>1975</v>
@@ -40560,7 +40560,7 @@
         </is>
       </c>
       <c r="C129" s="17" t="n">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="D129" s="23" t="n">
         <v>1631</v>
@@ -40897,7 +40897,7 @@
         </is>
       </c>
       <c r="C130" s="10" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D130" s="22" t="n">
         <v>1949</v>
@@ -41239,7 +41239,7 @@
         </is>
       </c>
       <c r="C131" s="17" t="n">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D131" s="18" t="n">
         <v>2142</v>
@@ -41576,7 +41576,7 @@
         </is>
       </c>
       <c r="C132" s="10" t="n">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="D132" s="22" t="n">
         <v>1959</v>
@@ -41913,7 +41913,7 @@
         </is>
       </c>
       <c r="C133" s="17" t="n">
-        <v>1134</v>
+        <v>1137</v>
       </c>
       <c r="D133" s="23" t="n">
         <v>1950</v>
@@ -42250,7 +42250,7 @@
         </is>
       </c>
       <c r="C134" s="10" t="n">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="D134" s="22" t="n">
         <v>1920</v>
@@ -42592,7 +42592,7 @@
         </is>
       </c>
       <c r="C135" s="17" t="n">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D135" s="23" t="n">
         <v>1869</v>
@@ -42929,7 +42929,7 @@
         </is>
       </c>
       <c r="C136" s="10" t="n">
-        <v>956</v>
+        <v>959</v>
       </c>
       <c r="D136" s="22" t="n">
         <v>2018</v>
@@ -43271,7 +43271,7 @@
         </is>
       </c>
       <c r="C137" s="17" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D137" s="23" t="n">
         <v>1862</v>
@@ -43608,7 +43608,7 @@
         </is>
       </c>
       <c r="C138" s="10" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D138" s="22" t="n">
         <v>1765</v>
@@ -43945,7 +43945,7 @@
         </is>
       </c>
       <c r="C139" s="17" t="n">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="D139" s="23" t="n">
         <v>2019</v>
@@ -44287,7 +44287,7 @@
         </is>
       </c>
       <c r="C140" s="10" t="n">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="D140" s="22" t="n">
         <v>1869</v>
@@ -44624,7 +44624,7 @@
         </is>
       </c>
       <c r="C141" s="17" t="n">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="D141" s="23" t="n">
         <v>1945</v>
@@ -44961,7 +44961,7 @@
         </is>
       </c>
       <c r="C142" s="10" t="n">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D142" s="22" t="n">
         <v>1840</v>
@@ -45303,7 +45303,7 @@
         </is>
       </c>
       <c r="C143" s="17" t="n">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="D143" s="18" t="n">
         <v>2177</v>
@@ -45645,7 +45645,7 @@
         </is>
       </c>
       <c r="C144" s="10" t="n">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="D144" s="22" t="n">
         <v>1884</v>
@@ -45982,7 +45982,7 @@
         </is>
       </c>
       <c r="C145" s="17" t="n">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D145" s="23" t="n">
         <v>1938</v>
@@ -46319,7 +46319,7 @@
         </is>
       </c>
       <c r="C146" s="10" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D146" s="22" t="n">
         <v>1894</v>
@@ -46656,7 +46656,7 @@
         </is>
       </c>
       <c r="C147" s="17" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D147" s="23" t="n">
         <v>1815</v>
@@ -46993,7 +46993,7 @@
         </is>
       </c>
       <c r="C148" s="10" t="n">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D148" s="22" t="n">
         <v>1733</v>
@@ -47330,7 +47330,7 @@
         </is>
       </c>
       <c r="C149" s="17" t="n">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D149" s="18" t="n">
         <v>2117</v>
@@ -47672,7 +47672,7 @@
         </is>
       </c>
       <c r="C150" s="10" t="n">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D150" s="22" t="n">
         <v>1929</v>
@@ -48009,7 +48009,7 @@
         </is>
       </c>
       <c r="C151" s="17" t="n">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="D151" s="18" t="n">
         <v>2102</v>
@@ -48346,7 +48346,7 @@
         </is>
       </c>
       <c r="C152" s="10" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D152" s="22" t="n">
         <v>2054</v>
@@ -48688,7 +48688,7 @@
         </is>
       </c>
       <c r="C153" s="17" t="n">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D153" s="23" t="n">
         <v>1772</v>
@@ -49030,7 +49030,7 @@
         </is>
       </c>
       <c r="C154" s="10" t="n">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="D154" s="22" t="n">
         <v>1980</v>
@@ -49367,7 +49367,7 @@
         </is>
       </c>
       <c r="C155" s="17" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D155" s="23" t="n">
         <v>1692</v>
@@ -49704,7 +49704,7 @@
         </is>
       </c>
       <c r="C156" s="10" t="n">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="D156" s="22" t="n">
         <v>1828</v>
@@ -50041,7 +50041,7 @@
         </is>
       </c>
       <c r="C157" s="17" t="n">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D157" s="23" t="n">
         <v>1682</v>
@@ -50378,7 +50378,7 @@
         </is>
       </c>
       <c r="C158" s="10" t="n">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="D158" s="22" t="n">
         <v>1811</v>
@@ -50715,7 +50715,7 @@
         </is>
       </c>
       <c r="C159" s="17" t="n">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="D159" s="23" t="n">
         <v>1960</v>
@@ -51057,7 +51057,7 @@
         </is>
       </c>
       <c r="C160" s="10" t="n">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="D160" s="22" t="n">
         <v>1807</v>
@@ -51394,7 +51394,7 @@
         </is>
       </c>
       <c r="C161" s="17" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D161" s="23" t="n">
         <v>1827</v>
@@ -51731,7 +51731,7 @@
         </is>
       </c>
       <c r="C162" s="10" t="n">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="D162" s="22" t="n">
         <v>1887</v>
@@ -52073,7 +52073,7 @@
         </is>
       </c>
       <c r="C163" s="17" t="n">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="D163" s="23" t="n">
         <v>1720</v>
@@ -52415,7 +52415,7 @@
         </is>
       </c>
       <c r="C164" s="10" t="n">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D164" s="22" t="n">
         <v>1780</v>
@@ -52752,7 +52752,7 @@
         </is>
       </c>
       <c r="C165" s="17" t="n">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="D165" s="23" t="n">
         <v>1841</v>
@@ -53089,7 +53089,7 @@
         </is>
       </c>
       <c r="C166" s="10" t="n">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="D166" s="22" t="n">
         <v>1641</v>
@@ -53431,7 +53431,7 @@
         </is>
       </c>
       <c r="C167" s="17" t="n">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="D167" s="23" t="n">
         <v>1668</v>
@@ -53768,7 +53768,7 @@
         </is>
       </c>
       <c r="C168" s="10" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D168" s="22" t="n">
         <v>1697</v>
@@ -54110,7 +54110,7 @@
         </is>
       </c>
       <c r="C169" s="17" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D169" s="23" t="n">
         <v>1776</v>
@@ -54447,7 +54447,7 @@
         </is>
       </c>
       <c r="C170" s="10" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D170" s="22" t="n">
         <v>1750</v>
@@ -54789,7 +54789,7 @@
         </is>
       </c>
       <c r="C171" s="17" t="n">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="D171" s="23" t="n">
         <v>1890</v>
@@ -55131,7 +55131,7 @@
         </is>
       </c>
       <c r="C172" s="10" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D172" s="22" t="n">
         <v>1598</v>
@@ -55468,7 +55468,7 @@
         </is>
       </c>
       <c r="C173" s="17" t="n">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="D173" s="23" t="n">
         <v>1841</v>
@@ -55805,7 +55805,7 @@
         </is>
       </c>
       <c r="C174" s="10" t="n">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D174" s="22" t="n">
         <v>1603</v>
@@ -56142,7 +56142,7 @@
         </is>
       </c>
       <c r="C175" s="17" t="n">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="D175" s="23" t="n">
         <v>1645</v>
@@ -56479,7 +56479,7 @@
         </is>
       </c>
       <c r="C176" s="10" t="n">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D176" s="22" t="n">
         <v>1595</v>
@@ -56821,7 +56821,7 @@
         </is>
       </c>
       <c r="C177" s="17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D177" s="23" t="n">
         <v>-1</v>
@@ -57158,7 +57158,7 @@
         </is>
       </c>
       <c r="C178" s="10" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D178" s="22" t="n">
         <v>-1</v>
@@ -57495,7 +57495,7 @@
         </is>
       </c>
       <c r="C179" s="17" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D179" s="23" t="n">
         <v>1881</v>
@@ -57832,7 +57832,7 @@
         </is>
       </c>
       <c r="C180" s="10" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D180" s="22" t="n">
         <v>1610</v>
@@ -58174,7 +58174,7 @@
         </is>
       </c>
       <c r="C181" s="17" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="D181" s="23" t="n">
         <v>1922</v>
@@ -58511,7 +58511,7 @@
         </is>
       </c>
       <c r="C182" s="10" t="n">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="D182" s="22" t="n">
         <v>1475</v>
@@ -58848,7 +58848,7 @@
         </is>
       </c>
       <c r="C183" s="17" t="n">
-        <v>1176</v>
+        <v>1179</v>
       </c>
       <c r="D183" s="23" t="n">
         <v>1641</v>
@@ -59190,7 +59190,7 @@
         </is>
       </c>
       <c r="C184" s="10" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D184" s="22" t="n">
         <v>1627</v>
@@ -59527,7 +59527,7 @@
         </is>
       </c>
       <c r="C185" s="17" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D185" s="23" t="n">
         <v>1624</v>
@@ -59864,7 +59864,7 @@
         </is>
       </c>
       <c r="C186" s="10" t="n">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D186" s="22" t="n">
         <v>1538</v>
@@ -60201,7 +60201,7 @@
         </is>
       </c>
       <c r="C187" s="17" t="n">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="D187" s="23" t="n">
         <v>1611</v>
@@ -60538,7 +60538,7 @@
         </is>
       </c>
       <c r="C188" s="10" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D188" s="22" t="n">
         <v>1549</v>
@@ -60875,7 +60875,7 @@
         </is>
       </c>
       <c r="C189" s="17" t="n">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D189" s="23" t="n">
         <v>1719</v>
@@ -61212,7 +61212,7 @@
         </is>
       </c>
       <c r="C190" s="10" t="n">
-        <v>1199</v>
+        <v>1202</v>
       </c>
       <c r="D190" s="22" t="n">
         <v>1942</v>
@@ -61554,7 +61554,7 @@
         </is>
       </c>
       <c r="C191" s="17" t="n">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D191" s="23" t="n">
         <v>1385</v>
@@ -61891,7 +61891,7 @@
         </is>
       </c>
       <c r="C192" s="10" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="D192" s="22" t="n">
         <v>1516</v>
@@ -62233,7 +62233,7 @@
         </is>
       </c>
       <c r="C193" s="17" t="n">
-        <v>1092</v>
+        <v>1095</v>
       </c>
       <c r="D193" s="18" t="n">
         <v>2523</v>
@@ -62575,7 +62575,7 @@
         </is>
       </c>
       <c r="C194" s="10" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="D194" s="22" t="n">
         <v>1722</v>
@@ -62917,7 +62917,7 @@
         </is>
       </c>
       <c r="C195" s="17" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D195" s="23" t="n">
         <v>1381</v>
@@ -63254,7 +63254,7 @@
         </is>
       </c>
       <c r="C196" s="10" t="n">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="D196" s="22" t="n">
         <v>1992</v>
@@ -63596,7 +63596,7 @@
         </is>
       </c>
       <c r="C197" s="17" t="n">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="D197" s="23" t="n">
         <v>1433</v>
@@ -63933,7 +63933,7 @@
         </is>
       </c>
       <c r="C198" s="10" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D198" s="22" t="n">
         <v>1495</v>
@@ -64270,7 +64270,7 @@
         </is>
       </c>
       <c r="C199" s="17" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D199" s="23" t="n">
         <v>1458</v>
@@ -64607,7 +64607,7 @@
         </is>
       </c>
       <c r="C200" s="10" t="n">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="D200" s="22" t="n">
         <v>1622</v>
@@ -64949,7 +64949,7 @@
         </is>
       </c>
       <c r="C201" s="17" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D201" s="23" t="n">
         <v>1664</v>
@@ -65286,7 +65286,7 @@
         </is>
       </c>
       <c r="C202" s="10" t="n">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D202" s="22" t="n">
         <v>-1</v>
@@ -65623,7 +65623,7 @@
         </is>
       </c>
       <c r="C203" s="17" t="n">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D203" s="23" t="n">
         <v>2086</v>

</xml_diff>